<commit_message>
rescaling + ignore another moment
+ cathing errors in regressions
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1119" documentId="8_{B9F5EDDD-5B41-4F7E-B91F-85F1F4692D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B8E8DE0-3645-4DE2-82A8-33FD2E13DD1A}"/>
+  <xr:revisionPtr revIDLastSave="1141" documentId="8_{B9F5EDDD-5B41-4F7E-B91F-85F1F4692D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB176F4E-83C8-4BD9-9561-746CE4101964}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" firstSheet="1" activeTab="2" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="206">
   <si>
     <t>label</t>
   </si>
@@ -723,6 +723,12 @@
   <si>
     <t>bla</t>
   </si>
+  <si>
+    <t>I think the weight is screwed up?</t>
+  </si>
+  <si>
+    <t>it makes not sense that it is so much more precise than above.</t>
+  </si>
 </sst>
 </file>
 
@@ -1426,7 +1432,7 @@
       </c>
       <c r="R4">
         <f ca="1">RAND()</f>
-        <v>0.4624788916073268</v>
+        <v>8.2077784065309412E-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -1834,15 +1840,15 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>25.315894905342514</v>
+        <v>23.737194185778787</v>
       </c>
       <c r="C12">
         <f>PARS!C12</f>
-        <v>17.626998263015263</v>
+        <v>16.527777597673573</v>
       </c>
       <c r="D12">
         <f>PARS!D12</f>
-        <v>26.44049739452289</v>
+        <v>24.791666396510362</v>
       </c>
       <c r="E12">
         <f>PARS!H12</f>
@@ -4002,8 +4008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD5CC74-B573-41B1-AB75-48DBC5AE1670}">
   <dimension ref="A1:CU99"/>
   <sheetViews>
-    <sheetView topLeftCell="CM1" workbookViewId="0">
-      <selection activeCell="CU100" sqref="CU100"/>
+    <sheetView topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BC1" sqref="BC1:BC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4011,6 +4017,7 @@
     <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99" x14ac:dyDescent="0.35">
@@ -28895,11 +28902,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29059,7 +29065,7 @@
         <v>0.53600000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -29350,7 +29356,7 @@
         <v>0.86309999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -29435,21 +29441,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>81</v>
       </c>
       <c r="B12">
-        <f>EXP(-0.0135*B37)*2*(1-MOMS!C52)/(MOMS!C47*(MOMS!C29/(24*365)+EXP(MOMS!C44)*(MOMS!C29/(24*365)+MOMS!C5/(24*365))))</f>
-        <v>22.033747828769076</v>
+        <f>EXP(-0.0135*$E$37)*2*(1-MOMS!C52)/(MOMS!C47*(MOMS!C29/(24*365)+EXP(MOMS!C44)*(MOMS!C29/(24*365)+MOMS!C5/(24*365))))</f>
+        <v>20.659721997091967</v>
       </c>
       <c r="C12">
         <f>B12*0.8</f>
-        <v>17.626998263015263</v>
+        <v>16.527777597673573</v>
       </c>
       <c r="D12">
         <f>B12*1.2</f>
-        <v>26.44049739452289</v>
+        <v>24.791666396510362</v>
       </c>
       <c r="E12">
         <v>20.659721997091967</v>
@@ -29521,7 +29527,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -30025,7 +30031,7 @@
         <v>8.1480999999999977</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -30064,7 +30070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -30199,7 +30205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -30250,7 +30256,7 @@
         <v>0.63890000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -30349,7 +30355,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -30395,7 +30401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -30434,7 +30440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -30480,7 +30486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -30518,7 +30524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -30643,7 +30649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -30683,7 +30689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -30724,7 +30730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>109</v>
       </c>
@@ -30764,7 +30770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>110</v>
       </c>
@@ -30808,7 +30814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>111</v>
       </c>
@@ -30848,7 +30854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -30888,7 +30894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>113</v>
       </c>
@@ -30928,7 +30934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -30969,7 +30975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>182</v>
       </c>
@@ -31009,7 +31015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>183</v>
       </c>
@@ -31049,7 +31055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>184</v>
       </c>
@@ -31090,23 +31096,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P49" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
-    <filterColumn colId="15">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P49" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A002A-BEAD-45BB-A257-D80A19A6BE2C}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31654,7 +31654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -31671,7 +31671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -31688,7 +31688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -31705,7 +31705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -31722,7 +31722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -31735,11 +31735,16 @@
         <v>277.39608436846476</v>
       </c>
       <c r="D37">
-        <f>1</f>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" t="s">
+        <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -31756,7 +31761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -31773,7 +31778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -31790,7 +31795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -31807,7 +31812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -31824,7 +31829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>175</v>
       </c>
@@ -31842,7 +31847,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -31858,7 +31863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -31875,7 +31880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>114</v>
       </c>
@@ -31890,7 +31895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>63</v>
       </c>
@@ -31907,7 +31912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -32034,13 +32039,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EFA40D-2664-412E-B9B4-3734B019C060}">
   <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AJ36" sqref="AJ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="35" max="35" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.35">
@@ -43820,8 +43827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50173A7-B186-45C1-8337-B5032812D8C9}">
   <dimension ref="A1:BD56"/>
   <sheetViews>
-    <sheetView topLeftCell="AN42" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="AB20" workbookViewId="0">
+      <selection activeCell="AM40" sqref="AM40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43829,6 +43836,8 @@
     <col min="2" max="2" width="12.1796875" customWidth="1"/>
     <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
start from a more random point?
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1237" documentId="8_{B9F5EDDD-5B41-4F7E-B91F-85F1F4692D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{551A250B-F013-4F62-A6B0-EE38C0382EF1}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DED15BE8-F7C5-408D-99BE-6852BC4CEE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{619C077B-E7C2-4EDB-9538-DF2DF64D6507}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="213">
   <si>
     <t>label</t>
   </si>
@@ -747,6 +747,9 @@
   <si>
     <t>I still think this is just way too high??</t>
   </si>
+  <si>
+    <t>share perturb</t>
+  </si>
 </sst>
 </file>
 
@@ -1207,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1272,8 +1275,8 @@
         <v>71</v>
       </c>
       <c r="B2">
-        <f>D2*$Q$4+C2*(1-$Q$4)</f>
-        <v>0.57460883117957295</v>
+        <f>(D2*$Q$4+C2*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B2</f>
+        <v>0.51554199656590594</v>
       </c>
       <c r="C2">
         <f>PARS!C2</f>
@@ -1329,8 +1332,8 @@
         <v>72</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B49" si="0">D3*$Q$4+C3*(1-$Q$4)</f>
-        <v>0.62236092741176097</v>
+        <f>(D3*$Q$4+C3*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B3</f>
+        <v>0.23987187255798972</v>
       </c>
       <c r="C3">
         <f>PARS!C3</f>
@@ -1389,7 +1392,7 @@
         <v>73</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f>(D4*$Q$4+C4*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B4</f>
         <v>-2.5836226227271579</v>
       </c>
       <c r="C4">
@@ -1445,7 +1448,7 @@
       </c>
       <c r="R4">
         <f ca="1">RAND()</f>
-        <v>0.97894623173766415</v>
+        <v>0.83775034972002071</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -1453,8 +1456,8 @@
         <v>74</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>2.1561459451779652</v>
+        <f>(D5*$Q$4+C5*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B5</f>
+        <v>2.0947824223794616</v>
       </c>
       <c r="C5">
         <f>PARS!C5</f>
@@ -1510,16 +1513,16 @@
         <v>75</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>6.1483183318086301</v>
+        <f>(D6*$Q$4+C6*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B6</f>
+        <v>2.0664092910330836</v>
       </c>
       <c r="C6">
         <f>PARS!C6</f>
-        <v>3.912023005428146</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D6">
         <f>PARS!D6</f>
-        <v>6.9077552789821368</v>
+        <v>2.3025850929940459</v>
       </c>
       <c r="E6">
         <f>PARS!H6</f>
@@ -1560,6 +1563,9 @@
       <c r="N6">
         <f>PARS!Q6</f>
         <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -1567,8 +1573,8 @@
         <v>76</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>0.63250253100494158</v>
+        <f>(D7*$Q$4+C7*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B7</f>
+        <v>0.13930077927814119</v>
       </c>
       <c r="C7">
         <f>PARS!C7</f>
@@ -1617,6 +1623,10 @@
       <c r="N7">
         <f>PARS!Q7</f>
         <v>1</v>
+      </c>
+      <c r="Q7">
+        <f>0.2</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -1624,8 +1634,8 @@
         <v>77</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>-0.84997538874761558</v>
+        <f>(D8*$Q$4+C8*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B8</f>
+        <v>-1.4575454076968035</v>
       </c>
       <c r="C8">
         <f>PARS!C8</f>
@@ -1681,8 +1691,8 @@
         <v>78</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>-0.28104262680294673</v>
+        <f>(D9*$Q$4+C9*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B9</f>
+        <v>-0.17398830116580949</v>
       </c>
       <c r="C9">
         <f>PARS!C9</f>
@@ -1738,8 +1748,8 @@
         <v>79</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>-0.28104262680294673</v>
+        <f>(D10*$Q$4+C10*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B10</f>
+        <v>-0.17398830116580949</v>
       </c>
       <c r="C10">
         <f>PARS!C10</f>
@@ -1795,8 +1805,8 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>-7.9093959633794286E-2</v>
+        <f>(D11*$Q$4+C11*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B11</f>
+        <v>-0.21099875517314412</v>
       </c>
       <c r="C11">
         <f>PARS!C11</f>
@@ -1852,8 +1862,8 @@
         <v>81</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>20.659721997091967</v>
+        <f>(D12*$Q$4+C12*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B12</f>
+        <v>20.552805894085484</v>
       </c>
       <c r="C12">
         <f>PARS!C12</f>
@@ -1909,8 +1919,8 @@
         <v>82</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>6.1558490617802413</v>
+        <f>(D13*$Q$4+C13*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B13</f>
+        <v>2.7090081006658115</v>
       </c>
       <c r="C13">
         <f>PARS!C13</f>
@@ -1966,7 +1976,7 @@
         <v>83</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f>(D14*$Q$4+C14*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B14</f>
         <v>0</v>
       </c>
       <c r="C14">
@@ -2023,8 +2033,8 @@
         <v>193</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0.49298743824490843</v>
+        <f>(D15*$Q$4+C15*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B15</f>
+        <v>9.8597487648981685E-2</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2078,8 +2088,8 @@
         <v>84</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>0.74649371912245421</v>
+        <f>(D16*$Q$4+C16*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B16</f>
+        <v>0.28929874382449083</v>
       </c>
       <c r="C16">
         <f>PARS!C16</f>
@@ -2135,8 +2145,8 @@
         <v>85</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>0.72968783472137333</v>
+        <f>(D17*$Q$4+C17*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B17</f>
+        <v>-0.1394023882067113</v>
       </c>
       <c r="C17">
         <f>PARS!C17</f>
@@ -2192,8 +2202,8 @@
         <v>86</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>1.1838676447996261</v>
+        <f>(D18*$Q$4+C18*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B18</f>
+        <v>0.96980611445924936</v>
       </c>
       <c r="C18">
         <f>PARS!C18</f>
@@ -2249,8 +2259,8 @@
         <v>87</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
-        <v>4.5988388309268338</v>
+        <f>(D19*$Q$4+C19*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B19</f>
+        <v>0.3651300187371106</v>
       </c>
       <c r="C19">
         <f>PARS!C19</f>
@@ -2306,8 +2316,8 @@
         <v>88</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
-        <v>5.1558490617800761</v>
+        <f>(D20*$Q$4+C20*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B20</f>
+        <v>1.7090081006657782</v>
       </c>
       <c r="C20">
         <f>PARS!C20</f>
@@ -2363,8 +2373,8 @@
         <v>89</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1.7188653096650475</v>
+        <f>(D21*$Q$4+C21*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B21</f>
+        <v>1.4528085508289219</v>
       </c>
       <c r="C21">
         <f>PARS!C21</f>
@@ -2420,8 +2430,8 @@
         <v>90</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
-        <v>0.45114025010187542</v>
+        <f>(D22*$Q$4+C22*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B22</f>
+        <v>-0.15358028116885067</v>
       </c>
       <c r="C22">
         <f>PARS!C22</f>
@@ -2477,8 +2487,8 @@
         <v>91</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
-        <v>-0.25124100691168311</v>
+        <f>(D23*$Q$4+C23*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B23</f>
+        <v>-0.33558815653332263</v>
       </c>
       <c r="C23">
         <f>PARS!C23</f>
@@ -2534,8 +2544,8 @@
         <v>92</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
-        <v>0.10380785668536685</v>
+        <f>(D24*$Q$4+C24*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B24</f>
+        <v>1.6989893883288052</v>
       </c>
       <c r="C24">
         <f>PARS!C24</f>
@@ -2591,7 +2601,7 @@
         <v>93</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f>(D25*$Q$4+C25*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B25</f>
         <v>0.1449</v>
       </c>
       <c r="C25">
@@ -2648,7 +2658,7 @@
         <v>94</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f>(D26*$Q$4+C26*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B26</f>
         <v>0.1449</v>
       </c>
       <c r="C26">
@@ -2705,8 +2715,8 @@
         <v>95</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
-        <v>0.47623044732625586</v>
+        <f>(D27*$Q$4+C27*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B27</f>
+        <v>9.5246089465251177E-2</v>
       </c>
       <c r="C27">
         <f>PARS!C27</f>
@@ -2762,8 +2772,8 @@
         <v>96</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
-        <v>1.5132543538014338</v>
+        <f>(D28*$Q$4+C28*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B28</f>
+        <v>1.4116863596561993</v>
       </c>
       <c r="C28">
         <f>PARS!C28</f>
@@ -2819,8 +2829,8 @@
         <v>97</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
-        <v>0.68428933482175858</v>
+        <f>(D29*$Q$4+C29*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B29</f>
+        <v>0.59333228242426028</v>
       </c>
       <c r="C29">
         <f>PARS!C29</f>
@@ -2876,8 +2886,8 @@
         <v>98</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
-        <v>-4.185130455588383</v>
+        <f>(D30*$Q$4+C30*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B30</f>
+        <v>-4.5538198355243544</v>
       </c>
       <c r="C30">
         <f>PARS!C30</f>
@@ -2933,8 +2943,8 @@
         <v>99</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
-        <v>-0.587713243532896</v>
+        <f>(D31*$Q$4+C31*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B31</f>
+        <v>-0.67206039315453547</v>
       </c>
       <c r="C31">
         <f>PARS!C31</f>
@@ -2990,8 +3000,8 @@
         <v>100</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
-        <v>1.0300072885011469</v>
+        <f>(D32*$Q$4+C32*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B32</f>
+        <v>0.92384145770022941</v>
       </c>
       <c r="C32">
         <f>PARS!C32</f>
@@ -3047,8 +3057,8 @@
         <v>101</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
-        <v>0.47623044732625586</v>
+        <f>(D33*$Q$4+C33*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B33</f>
+        <v>9.5246089465251177E-2</v>
       </c>
       <c r="C33">
         <f>PARS!C33</f>
@@ -3104,8 +3114,8 @@
         <v>102</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
-        <v>1.4858368820192629</v>
+        <f>(D34*$Q$4+C34*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B34</f>
+        <v>1.3326873764038525</v>
       </c>
       <c r="C34">
         <f>PARS!C34</f>
@@ -3161,8 +3171,8 @@
         <v>103</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
-        <v>3.732468595612271</v>
+        <f>(D35*$Q$4+C35*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B35</f>
+        <v>0.74649371912245421</v>
       </c>
       <c r="C35">
         <f>PARS!C35</f>
@@ -3218,7 +3228,7 @@
         <v>104</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f>(D36*$Q$4+C36*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B36</f>
         <v>0</v>
       </c>
       <c r="C36">
@@ -3275,8 +3285,8 @@
         <v>105</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
-        <v>1.3838978452763118</v>
+        <f>(D37*$Q$4+C37*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B37</f>
+        <v>1.7944795569539675</v>
       </c>
       <c r="C37">
         <f>PARS!C37</f>
@@ -3332,8 +3342,8 @@
         <v>106</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
-        <v>4.2000000000000003E-2</v>
+        <f>(D38*$Q$4+C38*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B38</f>
+        <v>4.200000000000001E-2</v>
       </c>
       <c r="C38">
         <f>PARS!C38</f>
@@ -3389,7 +3399,7 @@
         <v>107</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f>(D39*$Q$4+C39*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B39</f>
         <v>0</v>
       </c>
       <c r="C39">
@@ -3446,7 +3456,7 @@
         <v>108</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f>(D40*$Q$4+C40*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B40</f>
         <v>0.26712328767123289</v>
       </c>
       <c r="C40">
@@ -3503,7 +3513,7 @@
         <v>109</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f>(D41*$Q$4+C41*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B41</f>
         <v>1.49</v>
       </c>
       <c r="C41">
@@ -3560,7 +3570,7 @@
         <v>110</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f>(D42*$Q$4+C42*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B42</f>
         <v>1</v>
       </c>
       <c r="C42">
@@ -3618,7 +3628,7 @@
         <v>111</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f>(D43*$Q$4+C43*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B43</f>
         <v>1.9809000000000001</v>
       </c>
       <c r="C43">
@@ -3675,8 +3685,8 @@
         <v>112</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
-        <v>1.9083999999999999</v>
+        <f>(D44*$Q$4+C44*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B44</f>
+        <v>1.9084000000000001</v>
       </c>
       <c r="C44">
         <f>PARS!C44</f>
@@ -3732,7 +3742,7 @@
         <v>113</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f>(D45*$Q$4+C45*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B45</f>
         <v>1</v>
       </c>
       <c r="C45">
@@ -3789,7 +3799,7 @@
         <v>114</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f>(D46*$Q$4+C46*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B46</f>
         <v>1.8814014327029097E-3</v>
       </c>
       <c r="C46">
@@ -3846,7 +3856,7 @@
         <v>182</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f>(D47*$Q$4+C47*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B47</f>
         <v>1.1266</v>
       </c>
       <c r="C47">
@@ -3903,7 +3913,7 @@
         <v>183</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f>(D48*$Q$4+C48*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B48</f>
         <v>0.98860000000000003</v>
       </c>
       <c r="C48">
@@ -3960,7 +3970,7 @@
         <v>184</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f>(D49*$Q$4+C49*(1-$Q$4))*$Q$7 +(1-$Q$7)*PARS!B49</f>
         <v>0.9607</v>
       </c>
       <c r="C49">
@@ -32278,8 +32288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32499,7 +32509,7 @@
         <v>2.0794415416798357</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:D6" si="6">LN(F5)</f>
+        <f t="shared" ref="C5:D5" si="6">LN(F5)</f>
         <v>1.6094379124341003</v>
       </c>
       <c r="D5">
@@ -32547,12 +32557,12 @@
         <v>2.1972245773362196</v>
       </c>
       <c r="C6">
-        <f t="shared" si="6"/>
-        <v>3.912023005428146</v>
+        <f t="shared" ref="C6:D6" si="7">LN(F6/100)</f>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D6">
-        <f t="shared" si="6"/>
-        <v>6.9077552789821368</v>
+        <f t="shared" si="7"/>
+        <v>2.3025850929940459</v>
       </c>
       <c r="E6">
         <v>900</v>
@@ -32595,11 +32605,11 @@
         <v>1.6000341346441075E-2</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:D7" si="7">-LN(1/F7 -1)</f>
+        <f t="shared" ref="C7:D7" si="8">-LN(1/F7 -1)</f>
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.84729786038720356</v>
       </c>
       <c r="E7">
@@ -32643,11 +32653,11 @@
         <v>-1.6094379124341003</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:D9" si="8">LN(F8)</f>
+        <f t="shared" ref="C8:D9" si="9">LN(F8)</f>
         <v>-2.3025850929940455</v>
       </c>
       <c r="D8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-0.35667494393873245</v>
       </c>
       <c r="E8">
@@ -32691,11 +32701,11 @@
         <v>-0.14722471975652515</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-2.3025850929940455</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.40546510810816438</v>
       </c>
       <c r="E9">
@@ -32739,11 +32749,11 @@
         <v>-0.14722471975652515</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:D10" si="9">C9</f>
+        <f t="shared" ref="C10:D10" si="10">C9</f>
         <v>-2.3025850929940455</v>
       </c>
       <c r="D10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.40546510810816438</v>
       </c>
       <c r="E10">
@@ -32780,11 +32790,11 @@
         <v>-0.24397495405798156</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:D11" si="10">F11</f>
+        <f t="shared" ref="C11:D11" si="11">F11</f>
         <v>-0.312</v>
       </c>
       <c r="D11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E11">
@@ -32868,7 +32878,7 @@
         <v>1.8472978603872034</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13" si="11">1-LN(1/(F13-1) -1)</f>
+        <f t="shared" ref="C13" si="12">1-LN(1/(F13-1) -1)</f>
         <v>1</v>
       </c>
       <c r="D13">
@@ -32951,11 +32961,11 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:D16" si="12">F15</f>
+        <f t="shared" ref="C15:D16" si="13">F15</f>
         <v>-1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="E15">
@@ -32975,11 +32985,11 @@
         <v>1</v>
       </c>
       <c r="P15">
-        <f t="shared" ref="P15" si="13">I15-N15</f>
+        <f t="shared" ref="P15" si="14">I15-N15</f>
         <v>1</v>
       </c>
       <c r="Q15">
-        <f t="shared" ref="Q15" si="14">P15+K15+N15+J15</f>
+        <f t="shared" ref="Q15" si="15">P15+K15+N15+J15</f>
         <v>1</v>
       </c>
     </row>
@@ -32992,11 +33002,11 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="C16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="E16">
@@ -33033,11 +33043,11 @@
         <v>-0.35667494393873245</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:D18" si="15">LN(F17)</f>
+        <f t="shared" ref="C17:D18" si="16">LN(F17)</f>
         <v>-0.35667494393873245</v>
       </c>
       <c r="D17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0986122886681098</v>
       </c>
       <c r="E17">
@@ -33081,11 +33091,11 @@
         <v>0.91629073187415511</v>
       </c>
       <c r="C18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.58778666490211906</v>
       </c>
       <c r="D18">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.3862943611198906</v>
       </c>
       <c r="E18">
@@ -33132,11 +33142,11 @@
         <v>-0.69329718431032028</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:D20" si="16">-LN(1/F19 -1)</f>
+        <f t="shared" ref="C19:D20" si="17">-LN(1/F19 -1)</f>
         <v>-2.1972245773362196</v>
       </c>
       <c r="D19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.9067547786484651</v>
       </c>
       <c r="E19">
@@ -33177,11 +33187,11 @@
         <v>0.84729786038720356</v>
       </c>
       <c r="C20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>6.9067547786484651</v>
       </c>
       <c r="E20">
@@ -33225,11 +33235,11 @@
         <v>1.3862943611198906</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:D24" si="17">LN(F21)</f>
+        <f t="shared" ref="C21:D24" si="18">LN(F21)</f>
         <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.3025850929940459</v>
       </c>
       <c r="E21">
@@ -33273,11 +33283,11 @@
         <v>-0.3047604139865322</v>
       </c>
       <c r="C22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-2.3025850929940455</v>
       </c>
       <c r="D22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.3862943611198906</v>
       </c>
       <c r="E22">
@@ -33321,11 +33331,11 @@
         <v>-0.35667494393873245</v>
       </c>
       <c r="C23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-0.71334988787746489</v>
       </c>
       <c r="D23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-9.4310679471241415E-2</v>
       </c>
       <c r="E23">
@@ -33369,11 +33379,11 @@
         <v>2.0977847712396644</v>
       </c>
       <c r="C24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-6.9077552789821368</v>
       </c>
       <c r="D24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2.4849066497880004</v>
       </c>
       <c r="E24">
@@ -33503,11 +33513,11 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:D28" si="18">LN(F27)</f>
+        <f t="shared" ref="C27:D28" si="19">LN(F27)</f>
         <v>-0.16251892949777494</v>
       </c>
       <c r="D27">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.69314718055994529</v>
       </c>
       <c r="E27">
@@ -33551,11 +33561,11 @@
         <v>1.3862943611198906</v>
       </c>
       <c r="C28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.69314718055994529</v>
       </c>
       <c r="D28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.791759469228055</v>
       </c>
       <c r="E28">
@@ -33599,11 +33609,11 @@
         <v>0.57059301932488571</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:D29" si="19">-LN(1/F29 -1)</f>
+        <f t="shared" ref="C29:D29" si="20">-LN(1/F29 -1)</f>
         <v>-0.40790273033909435</v>
       </c>
       <c r="D29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.0551933911457412</v>
       </c>
       <c r="E29">
@@ -33650,11 +33660,11 @@
         <v>-4.6459921805083466</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:D30" si="20">LN(F30)</f>
+        <f t="shared" ref="C30:D30" si="21">LN(F30)</f>
         <v>-4.8691357318225563</v>
       </c>
       <c r="D30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>-3.9528449999484012</v>
       </c>
       <c r="E30">
@@ -33703,11 +33713,11 @@
         <v>-0.69314718055994529</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:D31" si="21">LN(F31)</f>
+        <f t="shared" ref="C31:D31" si="22">LN(F31)</f>
         <v>-1.0498221244986778</v>
       </c>
       <c r="D31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>-0.43078291609245423</v>
       </c>
       <c r="E31">
@@ -33751,11 +33761,11 @@
         <v>0.89729999999999999</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:D32" si="22">F32</f>
+        <f t="shared" ref="C32:D32" si="23">F32</f>
         <v>0.62810999999999995</v>
       </c>
       <c r="D32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.16649</v>
       </c>
       <c r="E32">
@@ -33798,23 +33808,23 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:G33" si="23">C27</f>
+        <f t="shared" ref="C33:G33" si="24">C27</f>
         <v>-0.16251892949777494</v>
       </c>
       <c r="D33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.69314718055994529</v>
       </c>
       <c r="E33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="F33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.85</v>
       </c>
       <c r="G33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="L33">
@@ -33965,11 +33975,11 @@
         <v>1.8971249848733813</v>
       </c>
       <c r="C37">
-        <f t="shared" ref="C37:D37" si="24">LN(F37)</f>
+        <f t="shared" ref="C37:D37" si="25">LN(F37)</f>
         <v>-6.9077552789821368</v>
       </c>
       <c r="D37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>4.1997100778674268</v>
       </c>
       <c r="E37">
@@ -34091,11 +34101,11 @@
         <v>0.26712328767123289</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:D43" si="25">B40</f>
+        <f t="shared" ref="C40:D43" si="26">B40</f>
         <v>0.26712328767123289</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D41" si="26">B40</f>
+        <f t="shared" ref="D40:D41" si="27">B40</f>
         <v>0.26712328767123289</v>
       </c>
       <c r="E40">
@@ -34131,11 +34141,11 @@
         <v>1.49</v>
       </c>
       <c r="C41">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.49</v>
       </c>
       <c r="D41">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1.49</v>
       </c>
       <c r="E41">
@@ -34215,11 +34225,11 @@
         <v>1.9809000000000001</v>
       </c>
       <c r="C43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.9809000000000001</v>
       </c>
       <c r="D43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.9809000000000001</v>
       </c>
       <c r="E43">
@@ -34255,11 +34265,11 @@
         <v>1.9084000000000001</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:D44" si="27">B44</f>
+        <f t="shared" ref="C44:D44" si="28">B44</f>
         <v>1.9084000000000001</v>
       </c>
       <c r="D44">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1.9084000000000001</v>
       </c>
       <c r="E44">
@@ -34295,11 +34305,11 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:D45" si="28">B45</f>
+        <f t="shared" ref="C45:D45" si="29">B45</f>
         <v>1</v>
       </c>
       <c r="D45">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1</v>
       </c>
       <c r="E45">
@@ -34336,11 +34346,11 @@
         <v>1.8814014327029097E-3</v>
       </c>
       <c r="C46">
-        <f t="shared" ref="C46:D46" si="29">B46</f>
+        <f t="shared" ref="C46:D46" si="30">B46</f>
         <v>1.8814014327029097E-3</v>
       </c>
       <c r="D46">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1.8814014327029097E-3</v>
       </c>
       <c r="E46">
@@ -34376,11 +34386,11 @@
         <v>1.1266</v>
       </c>
       <c r="C47">
-        <f t="shared" ref="C47:D47" si="30">B47</f>
+        <f t="shared" ref="C47:D47" si="31">B47</f>
         <v>1.1266</v>
       </c>
       <c r="D47">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>1.1266</v>
       </c>
       <c r="E47">
@@ -34416,11 +34426,11 @@
         <v>0.98860000000000003</v>
       </c>
       <c r="C48">
-        <f t="shared" ref="C48:D48" si="31">B48</f>
+        <f t="shared" ref="C48:D48" si="32">B48</f>
         <v>0.98860000000000003</v>
       </c>
       <c r="D48">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.98860000000000003</v>
       </c>
       <c r="E48">
@@ -34456,11 +34466,11 @@
         <v>0.9607</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:D49" si="32">B49</f>
+        <f t="shared" ref="C49:D49" si="33">B49</f>
         <v>0.9607</v>
       </c>
       <c r="D49">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.9607</v>
       </c>
       <c r="E49">
@@ -34489,7 +34499,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P49" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
pnw empty - catch as a large moment error
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EF9D61E6-B168-4AD1-B5B4-FCA6F5A94DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EF395B7-A9DB-4745-9F30-0BFD9A1E00C4}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EF9D61E6-B168-4AD1-B5B4-FCA6F5A94DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D55A0D18-1968-47BF-9665-FA8F592A1954}"/>
   <bookViews>
-    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>0.47715515434632727</v>
+        <v>0.34403793111988268</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="B33">
         <f>(D33*$R$4+C33*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B33</f>
-        <v>-0.27225419177810328</v>
+        <v>-0.35344115077234661</v>
       </c>
       <c r="C33">
         <f>PARS!C33</f>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="D33">
         <f>PARS!D33</f>
-        <v>1.3862943611198906</v>
+        <v>0.69314718055994529</v>
       </c>
       <c r="E33" t="b">
         <f t="shared" si="0"/>
@@ -32607,8 +32607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34429,7 +34429,7 @@
       </c>
       <c r="D33">
         <f t="shared" si="11"/>
-        <v>1.3862943611198906</v>
+        <v>0.69314718055994529</v>
       </c>
       <c r="E33">
         <v>0.73729999999999996</v>
@@ -34438,7 +34438,7 @@
         <v>0.1</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H33">
         <v>6</v>

</xml_diff>

<commit_message>
try to give solve a shot
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B625C4E-5245-43D6-8678-8EBB7228697D}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EA33EB9-3B56-4C52-8536-C207723F7410}"/>
   <bookViews>
     <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="2" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>0.57460757496888504</v>
+        <v>5.6729481891899525E-3</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -35307,8 +35307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A002A-BEAD-45BB-A257-D80A19A6BE2C}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Rescaled eta and new beginning
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1E2C7EE-779C-4B4C-9BF4-2E7B0A9F72DA}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01915952-C660-4DCE-92CA-F0A01045647A}"/>
   <bookViews>
     <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
@@ -1526,11 +1526,11 @@
       </c>
       <c r="B4">
         <f>(D4*$R$4+C4*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B4</f>
-        <v>-0.46556839857654353</v>
+        <v>-0.24677294878368652</v>
       </c>
       <c r="C4">
         <f>PARS!C4</f>
-        <v>-2.3025850929940455</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D4">
         <f>PARS!D4</f>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>9.4615842624177438E-2</v>
+        <v>0.61742169453022755</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1594,11 +1594,11 @@
       </c>
       <c r="B5">
         <f>(D5*$R$4+C5*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B5</f>
-        <v>-0.46556839857654353</v>
+        <v>-0.24677294878368652</v>
       </c>
       <c r="C5">
         <f>PARS!C5</f>
-        <v>-2.3025850929940455</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D5">
         <f>PARS!D5</f>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="B7">
         <f>(D7*$R$4+C7*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B7</f>
-        <v>-1.664457208543453</v>
+        <v>-1.5074950103107991</v>
       </c>
       <c r="C7">
         <f>PARS!C7</f>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D7">
         <f>PARS!D7</f>
-        <v>-0.35667494393873245</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="E7" t="b">
         <f t="shared" si="0"/>
@@ -1906,11 +1906,11 @@
       </c>
       <c r="B10">
         <f>(D10*$R$4+C10*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B10</f>
-        <v>-0.28705355752517575</v>
+        <v>-6.8258107732318746E-2</v>
       </c>
       <c r="C10">
         <f>PARS!C10</f>
-        <v>-2.3025850929940455</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D10">
         <f>PARS!D10</f>
@@ -2272,11 +2272,11 @@
       </c>
       <c r="B16">
         <f>(D16*$R$4+C16*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B16</f>
-        <v>-1.8292107035378664</v>
+        <v>-1.5161851825061017</v>
       </c>
       <c r="C16">
         <f>PARS!C16</f>
-        <v>-4.6051701859880909</v>
+        <v>-2.3025850929940455</v>
       </c>
       <c r="D16">
         <f>PARS!D16</f>
@@ -32607,8 +32607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32795,7 +32795,7 @@
       </c>
       <c r="C4" s="7">
         <f>LN(F4)</f>
-        <v>-2.3025850929940455</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D4" s="7">
         <f>LN(G4)</f>
@@ -32805,7 +32805,7 @@
         <v>0.8</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G4">
         <v>1.5</v>
@@ -32853,7 +32853,7 @@
       </c>
       <c r="C5">
         <f>C4</f>
-        <v>-2.3025850929940455</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D5">
         <f>D4</f>
@@ -32864,11 +32864,10 @@
         <v>0.8</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:G5" si="4">F4</f>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F5:G5" si="4">G4</f>
         <v>1.5</v>
       </c>
       <c r="H5">
@@ -32955,7 +32954,7 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:D9" si="5">LN(E7)</f>
-        <v>-1.6607312068216509</v>
+        <v>-1.4375876555074412</v>
       </c>
       <c r="C7">
         <f t="shared" si="5"/>
@@ -32963,16 +32962,17 @@
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>-0.35667494393873245</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="E7">
-        <v>0.19</v>
+        <f>0.19/0.8</f>
+        <v>0.23749999999999999</v>
       </c>
       <c r="F7">
         <v>0.1</v>
       </c>
       <c r="G7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H7">
         <v>1.1000000000000001</v>
@@ -33004,7 +33004,7 @@
       </c>
       <c r="U7">
         <f>EXP(B7)</f>
-        <v>0.19</v>
+        <v>0.23749999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -33133,7 +33133,7 @@
       </c>
       <c r="C10">
         <f t="shared" ref="C10:G10" si="6">C4</f>
-        <v>-2.3025850929940455</v>
+        <v>-0.69314718055994529</v>
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
@@ -33144,7 +33144,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="6"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G10">
         <f t="shared" si="6"/>
@@ -33484,7 +33484,7 @@
       </c>
       <c r="C16">
         <f>LN(-G16)</f>
-        <v>-4.6051701859880909</v>
+        <v>-2.3025850929940455</v>
       </c>
       <c r="D16">
         <f>LN(-F16)</f>
@@ -33497,7 +33497,7 @@
         <v>-0.312</v>
       </c>
       <c r="G16">
-        <v>-0.01</v>
+        <v>-0.1</v>
       </c>
       <c r="H16">
         <v>1.4</v>

</xml_diff>

<commit_message>
new inputs try around a good guess
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D4861B3-6E08-45D5-B805-ED51A668C87C}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E97CA82-8C65-4434-B18A-93EB2274FB37}"/>
   <bookViews>
-    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="231">
   <si>
     <t>label</t>
   </si>
@@ -840,6 +840,9 @@
   <si>
     <t>ranomd</t>
   </si>
+  <si>
+    <t>ADD, I know weight sucks. But it makes no sense to exclude it.</t>
+  </si>
 </sst>
 </file>
 
@@ -1335,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -1472,7 +1475,7 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>0.60328028821234336</v>
+        <v>4.7081044796112081E-2</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -1540,7 +1543,7 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q49" ca="1" si="1">RAND()</f>
-        <v>0.11042061048061769</v>
+        <v>0.173170298793629</v>
       </c>
       <c r="R3" t="s">
         <v>193</v>
@@ -1611,14 +1614,14 @@
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20176365921010064</v>
+        <v>0.58403073848214548</v>
       </c>
       <c r="R4">
         <v>0.6</v>
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>0.87381522639538356</v>
+        <v>2.0182018374813371E-2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1686,7 +1689,7 @@
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15126474573168436</v>
+        <v>6.3506687183912169E-2</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -1754,7 +1757,7 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64323068317760612</v>
+        <v>0.82372303890884535</v>
       </c>
       <c r="R6" t="s">
         <v>211</v>
@@ -1825,7 +1828,7 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86146243192238448</v>
+        <v>0.51889980004854752</v>
       </c>
       <c r="R7">
         <v>0.5</v>
@@ -1896,7 +1899,7 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65218604783901835</v>
+        <v>0.31819234871989943</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -1964,7 +1967,7 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94191031574644823</v>
+        <v>4.0194841858134267E-2</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -2032,7 +2035,7 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9571280667603883E-2</v>
+        <v>0.13383370793322713</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -2100,7 +2103,7 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23558120501155499</v>
+        <v>0.10823377595541217</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
@@ -2168,7 +2171,7 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53233697419842507</v>
+        <v>0.65423015873308443</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -2236,7 +2239,7 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7115292119247254E-2</v>
+        <v>0.63468939021204185</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2304,7 +2307,7 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55182527254994407</v>
+        <v>0.78356607985052351</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -2372,7 +2375,7 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63079497762887959</v>
+        <v>3.0070441632859102E-2</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -2381,7 +2384,7 @@
       </c>
       <c r="B16">
         <f>(D16*$R$4+C16*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B16</f>
-        <v>-1.5152874990810479</v>
+        <v>-1.5193514223633309</v>
       </c>
       <c r="C16">
         <f>PARS!C16</f>
@@ -2440,7 +2443,7 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28582755023896023</v>
+        <v>0.40958688415259581</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -2508,7 +2511,7 @@
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28368100268246477</v>
+        <v>0.20030830742192129</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
@@ -2576,7 +2579,7 @@
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68984766010374721</v>
+        <v>0.84919556119962092</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -2644,7 +2647,7 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37373926759033771</v>
+        <v>0.18141211343408459</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
@@ -2712,7 +2715,7 @@
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3186562531838972E-2</v>
+        <v>0.7942221978866808</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
@@ -2780,7 +2783,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14688935738363018</v>
+        <v>0.67648502504987107</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
@@ -2848,7 +2851,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85878301224333642</v>
+        <v>0.1080775607866894</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
@@ -2916,7 +2919,7 @@
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76201176155116235</v>
+        <v>0.44542621341633493</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
@@ -2984,7 +2987,7 @@
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26825513250453037</v>
+        <v>0.33913472414011891</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -3052,7 +3055,7 @@
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38480587363308882</v>
+        <v>0.42989262446065457</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
@@ -3120,7 +3123,7 @@
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18284000749409635</v>
+        <v>0.25389323020763832</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
@@ -3188,7 +3191,7 @@
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4387383816964352</v>
+        <v>0.94196230648268053</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
@@ -3256,7 +3259,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35519417116726515</v>
+        <v>6.6400723478801216E-2</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
@@ -3324,7 +3327,7 @@
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78635561472118765</v>
+        <v>0.39934453945251336</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
@@ -3392,7 +3395,7 @@
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29267631128176641</v>
+        <v>0.1562562410609285</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -3460,7 +3463,7 @@
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85686200900946774</v>
+        <v>0.7964362044514729</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
@@ -3528,7 +3531,7 @@
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33450022560761983</v>
+        <v>0.84877094324874414</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -3596,7 +3599,7 @@
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62292382361878118</v>
+        <v>0.3875382149892338</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -3664,7 +3667,7 @@
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61270903421366074</v>
+        <v>0.33187953773689471</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -3732,7 +3735,7 @@
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99905967463407075</v>
+        <v>0.32123172208347728</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -3800,7 +3803,7 @@
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35454688706897064</v>
+        <v>5.0435395157746976E-2</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -3868,7 +3871,7 @@
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94942944593123757</v>
+        <v>0.10622726029118301</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -3936,7 +3939,7 @@
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63415421260614391</v>
+        <v>4.3212527250667487E-2</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -4004,7 +4007,7 @@
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2404053088332132</v>
+        <v>0.74803373996710787</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -4072,7 +4075,7 @@
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92905368632414087</v>
+        <v>0.97685725696322323</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -4140,7 +4143,7 @@
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7535499840838078</v>
+        <v>0.32893482252062234</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4208,7 +4211,7 @@
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="1"/>
-        <v>1.9321608594791706E-2</v>
+        <v>6.7824832909979982E-2</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -4276,7 +4279,7 @@
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95297266936470681</v>
+        <v>0.84774697874550398</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -4344,7 +4347,7 @@
       </c>
       <c r="Q44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26298718699411971</v>
+        <v>6.0969091230077987E-2</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -4412,7 +4415,7 @@
       </c>
       <c r="Q45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17591240891385984</v>
+        <v>0.63764395417513908</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -4480,7 +4483,7 @@
       </c>
       <c r="Q46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10552648025071354</v>
+        <v>0.61401073086943703</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
@@ -4548,7 +4551,7 @@
       </c>
       <c r="Q47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99395002718748005</v>
+        <v>0.48558644933837003</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -4616,7 +4619,7 @@
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97976567085004518</v>
+        <v>0.1806308948144083</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
@@ -4684,7 +4687,7 @@
       </c>
       <c r="Q49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12322479824887711</v>
+        <v>4.8146050290107656E-2</v>
       </c>
     </row>
   </sheetData>
@@ -32953,7 +32956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -33827,7 +33830,7 @@
       </c>
       <c r="B16">
         <f>LN(-E16)</f>
-        <v>-1.4106897062608845</v>
+        <v>-1.4188175528254507</v>
       </c>
       <c r="C16">
         <f>LN(-G16)</f>
@@ -33838,7 +33841,7 @@
         <v>-1.1647520911726548</v>
       </c>
       <c r="E16">
-        <v>-0.24397495405798156</v>
+        <v>-0.24199999999999999</v>
       </c>
       <c r="F16">
         <v>-0.312</v>
@@ -33876,7 +33879,7 @@
       </c>
       <c r="U16">
         <f>-EXP(B16)</f>
-        <v>-0.24397495405798153</v>
+        <v>-0.24199999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
@@ -33905,7 +33908,7 @@
         <v>0.65</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I17">
         <v>4.0999999999999996</v>
@@ -33963,7 +33966,7 @@
         <v>10.4</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I18">
         <v>4.0999999999999996</v>
@@ -34021,7 +34024,7 @@
         <v>1000</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I19">
         <v>4.0999999999999996</v>
@@ -34079,7 +34082,7 @@
         <v>0.7</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I20">
         <v>4.0999999999999996</v>
@@ -34247,7 +34250,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="I23">
         <v>4</v>
@@ -34300,7 +34303,7 @@
         <v>0.05</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="I24">
         <v>4</v>
@@ -34351,7 +34354,7 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="I25">
         <v>4</v>
@@ -34402,7 +34405,7 @@
         <v>3</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="I26">
         <v>4</v>
@@ -34505,7 +34508,7 @@
         <v>0.5</v>
       </c>
       <c r="H28">
-        <v>4</v>
+        <v>4.05</v>
       </c>
       <c r="I28">
         <v>4</v>
@@ -34556,7 +34559,7 @@
         <v>10</v>
       </c>
       <c r="H29">
-        <v>5</v>
+        <v>4.01</v>
       </c>
       <c r="I29">
         <v>5</v>
@@ -34614,7 +34617,7 @@
         <v>4</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>4.01</v>
       </c>
       <c r="I30">
         <v>5</v>
@@ -35655,8 +35658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42A002A-BEAD-45BB-A257-D80A19A6BE2C}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36745,13 +36748,13 @@
         <v>0.15652701064259733</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47">
-        <v>2.5</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="G47">
         <v>91</v>
@@ -36778,6 +36781,9 @@
       </c>
       <c r="G48">
         <v>92</v>
+      </c>
+      <c r="H48" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -48810,8 +48816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50173A7-B186-45C1-8337-B5032812D8C9}">
   <dimension ref="A1:BD56"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="AP35" sqref="AP35"/>
+    <sheetView topLeftCell="AN1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="AW20" sqref="AW20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
help deltaw to be precise
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F22ACED-F263-4EDF-ABEC-CD2E9CF71756}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8738922A-7B69-4E01-BABB-D630936C498E}"/>
   <bookViews>
     <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" firstSheet="1" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="248">
   <si>
     <t>label</t>
   </si>
@@ -892,13 +892,18 @@
   <si>
     <t>showmain</t>
   </si>
+  <si>
+    <t>The outcomes are VERY sensitive to this. This explains why this is also very precisely estimated?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="178" formatCode="0.00000000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -994,7 +999,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1013,6 +1018,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1524,7 +1531,7 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>0.84457210283531869</v>
+        <v>0.89463699069770231</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -1592,7 +1599,7 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q49" ca="1" si="1">RAND()</f>
-        <v>0.43054667908712529</v>
+        <v>0.53089541325096956</v>
       </c>
       <c r="R3" t="s">
         <v>191</v>
@@ -1663,14 +1670,14 @@
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16875262307873462</v>
+        <v>0.70209016988082662</v>
       </c>
       <c r="R4">
         <v>0.6</v>
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>0.79789103075487577</v>
+        <v>0.76395019170000122</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1738,7 +1745,7 @@
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4336819578192883E-2</v>
+        <v>0.54605906639724777</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -1806,7 +1813,7 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62899182298420309</v>
+        <v>0.54487311781668113</v>
       </c>
       <c r="R6" t="s">
         <v>209</v>
@@ -1877,7 +1884,7 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45631854866156796</v>
+        <v>0.89845252579004486</v>
       </c>
       <c r="R7">
         <v>0.5</v>
@@ -1948,7 +1955,7 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16572177089022389</v>
+        <v>0.85073274978654001</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -2016,7 +2023,7 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36382443596468939</v>
+        <v>0.5165618586032531</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -2084,7 +2091,7 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22287174306227731</v>
+        <v>0.79489911435319871</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -2152,7 +2159,7 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85809559138167579</v>
+        <v>0.15694226221072238</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
@@ -2220,7 +2227,7 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78836549629555774</v>
+        <v>0.88967958970466121</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -2288,7 +2295,7 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="1"/>
-        <v>4.7260090469481986E-2</v>
+        <v>0.46283400965467203</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2356,7 +2363,7 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43183295004963962</v>
+        <v>0.38762149025522508</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -2424,7 +2431,7 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93712032964778569</v>
+        <v>0.16675869238302665</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -2492,7 +2499,7 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31167525287323328</v>
+        <v>0.49710939356527684</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -2560,7 +2567,7 @@
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76630222548975424</v>
+        <v>3.2052976644297848E-3</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
@@ -2628,7 +2635,7 @@
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79636301366990103</v>
+        <v>0.44926909139385085</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -2696,7 +2703,7 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80332686628977079</v>
+        <v>0.22588669304658759</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
@@ -2705,7 +2712,7 @@
       </c>
       <c r="B20">
         <f>(D20*$R$4+C20*(1-$R$4))*$R$7 +(1-$R$7)*PARS!B20</f>
-        <v>0.26428970157084952</v>
+        <v>10.354529358116224</v>
       </c>
       <c r="C20">
         <f>PARS!C20</f>
@@ -2717,7 +2724,7 @@
       </c>
       <c r="E20" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <f>PARS!K20</f>
@@ -2764,7 +2771,7 @@
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92308137215062391</v>
+        <v>0.30048732408156165</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
@@ -2832,7 +2839,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77417657748330315</v>
+        <v>0.97051261182327042</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
@@ -2900,7 +2907,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57298090144419589</v>
+        <v>0.79128050192529942</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
@@ -2968,7 +2975,7 @@
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70198227390755163</v>
+        <v>0.65800026835808978</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
@@ -3036,7 +3043,7 @@
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83183663607925307</v>
+        <v>0.78274989372307091</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -3104,7 +3111,7 @@
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37408043729340312</v>
+        <v>0.32996082497130452</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
@@ -3172,7 +3179,7 @@
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76903651166537534</v>
+        <v>0.88964256480076376</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
@@ -3240,7 +3247,7 @@
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44851311943541017</v>
+        <v>0.35167698378298806</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
@@ -3308,7 +3315,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7039404793540553E-2</v>
+        <v>3.6458927708748812E-2</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
@@ -3376,7 +3383,7 @@
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1116875137486826E-3</v>
+        <v>0.21665632849104033</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
@@ -3444,7 +3451,7 @@
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90280217398191653</v>
+        <v>0.45681422509124947</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -3512,7 +3519,7 @@
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2955933007536102E-2</v>
+        <v>0.21321016332716269</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
@@ -3580,7 +3587,7 @@
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59124385193186546</v>
+        <v>3.8341180720692924E-2</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -3648,7 +3655,7 @@
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44838362873642346</v>
+        <v>0.59300860574992609</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -3716,7 +3723,7 @@
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80384464762724606</v>
+        <v>0.11280165123587627</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -3784,7 +3791,7 @@
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20146932329829592</v>
+        <v>0.32149561039209706</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -3852,7 +3859,7 @@
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98468401940999184</v>
+        <v>0.26214014742627767</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -3920,7 +3927,7 @@
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29362312452374262</v>
+        <v>0.95543223604057215</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -3988,7 +3995,7 @@
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9936767371529035</v>
+        <v>0.11278094957975571</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -4056,7 +4063,7 @@
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89191933514325172</v>
+        <v>0.77168083644107532</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -4124,7 +4131,7 @@
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87420449580701953</v>
+        <v>0.55355819137552287</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -4192,7 +4199,7 @@
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21348109984149422</v>
+        <v>0.9982085984187713</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4260,7 +4267,7 @@
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11467032590708592</v>
+        <v>0.24810297198372377</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -4328,7 +4335,7 @@
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92130679248930869</v>
+        <v>0.38675531071768099</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -4396,7 +4403,7 @@
       </c>
       <c r="Q44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29399873023629342</v>
+        <v>0.21684623482213894</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -4464,7 +4471,7 @@
       </c>
       <c r="Q45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56919980668232117</v>
+        <v>0.49985636505138009</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -4532,7 +4539,7 @@
       </c>
       <c r="Q46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86871830136466666</v>
+        <v>0.3949729170060613</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
@@ -4600,7 +4607,7 @@
       </c>
       <c r="Q47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86333826374089728</v>
+        <v>0.1531016970793061</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -4668,7 +4675,7 @@
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44166054939929722</v>
+        <v>0.10921215553040364</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
@@ -4736,7 +4743,7 @@
       </c>
       <c r="Q49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53452877039785562</v>
+        <v>3.332717037729116E-2</v>
       </c>
     </row>
   </sheetData>
@@ -33213,16 +33220,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
-  <dimension ref="A1:V49"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.36328125" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.54296875" customWidth="1"/>
+    <col min="25" max="25" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -33238,7 +33249,7 @@
       <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>192</v>
       </c>
       <c r="F1" t="s">
@@ -33309,7 +33320,7 @@
         <f>G2</f>
         <v>20.430907591983047</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="17">
         <v>20.430907591983047</v>
       </c>
       <c r="F2">
@@ -33366,7 +33377,7 @@
         <f>C3</f>
         <v>1.8814014327029097E-3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="17">
         <v>1.8814014327029097E-3</v>
       </c>
       <c r="F3">
@@ -33421,7 +33432,7 @@
         <f>LN(G4)</f>
         <v>0.18232155679395459</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="17">
         <v>0.8</v>
       </c>
       <c r="F4">
@@ -33483,7 +33494,7 @@
         <f>D4</f>
         <v>0.18232155679395459</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="17">
         <f>E4</f>
         <v>0.8</v>
       </c>
@@ -33539,7 +33550,7 @@
         <f>B6</f>
         <v>0.20836072497837904</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="17">
         <v>1.6156999999999999</v>
       </c>
       <c r="F6">
@@ -33594,7 +33605,7 @@
         <f t="shared" si="3"/>
         <v>-0.69314718055994529</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="17">
         <f>0.19/0.8</f>
         <v>0.23749999999999999</v>
       </c>
@@ -33657,7 +33668,7 @@
         <f t="shared" si="3"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="17">
         <v>1</v>
       </c>
       <c r="F8">
@@ -33719,7 +33730,7 @@
         <f t="shared" si="3"/>
         <v>1.791759469228055</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="17">
         <v>4</v>
       </c>
       <c r="F9">
@@ -33781,7 +33792,7 @@
         <f>D4</f>
         <v>0.18232155679395459</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="17">
         <v>1</v>
       </c>
       <c r="F10">
@@ -33838,7 +33849,7 @@
         <f>LN(G11)</f>
         <v>-1.1771745727096741</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="17">
         <v>0.15407408</v>
       </c>
       <c r="F11">
@@ -33905,7 +33916,7 @@
         <f>-LN(1/G12 -1)</f>
         <v>1.0551933911457412</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="17">
         <v>0.66013195000000002</v>
       </c>
       <c r="F12">
@@ -33970,7 +33981,7 @@
         <f>G13</f>
         <v>1.16649</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="17">
         <v>0.91482224000000001</v>
       </c>
       <c r="F13">
@@ -34031,7 +34042,7 @@
         <f>B14*1.3</f>
         <v>0.33413097860603447</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="17">
         <v>1.29307594</v>
       </c>
       <c r="F14">
@@ -34092,7 +34103,7 @@
         <f>LN(G15)</f>
         <v>-2.5836226227271579</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="17">
         <v>9.4106369999999995E-2</v>
       </c>
       <c r="F15">
@@ -34157,7 +34168,7 @@
         <f>LN(-F16)</f>
         <v>-1.1647520911726548</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="17">
         <v>-0.24199999999999999</v>
       </c>
       <c r="F16">
@@ -34203,7 +34214,7 @@
         <v>-0.24199999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -34219,7 +34230,7 @@
         <f t="shared" si="6"/>
         <v>-0.43078291609245423</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="17">
         <v>0.5</v>
       </c>
       <c r="F17">
@@ -34265,7 +34276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -34281,7 +34292,7 @@
         <f t="shared" si="6"/>
         <v>2.341805806147327</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="17">
         <v>6</v>
       </c>
       <c r="F18">
@@ -34327,7 +34338,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>72</v>
       </c>
@@ -34343,7 +34354,7 @@
         <f>LN(G19/100)</f>
         <v>2.9957322735539909</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="17">
         <v>2000</v>
       </c>
       <c r="F19">
@@ -34388,13 +34399,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>73</v>
       </c>
       <c r="B20">
-        <f>-LN(1/E20 -1)</f>
-        <v>2.0200686909376892E-2</v>
+        <f>-LN(1/E20 -1)*1000</f>
+        <v>20.200680000000126</v>
       </c>
       <c r="C20">
         <f>-LN(1/F20 -1)</f>
@@ -34404,8 +34415,8 @@
         <f>-LN(1/G20 -1)</f>
         <v>0.84729786038720356</v>
       </c>
-      <c r="E20">
-        <v>0.50505</v>
+      <c r="E20" s="17">
+        <v>0.50504999827283203</v>
       </c>
       <c r="F20">
         <v>0.5</v>
@@ -34420,8 +34431,8 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="J20">
-        <f>1/(E20*(1-E20))</f>
-        <v>4.0004080816284064</v>
+        <f>1000/(E20*(1-E20))</f>
+        <v>4000.4080813492396</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -34446,11 +34457,22 @@
         <v>1</v>
       </c>
       <c r="V20">
-        <f>1/(1+EXP(-B20))</f>
-        <v>0.50505</v>
+        <f>1/(1+EXP(-B20/1000))</f>
+        <v>0.50504999827283203</v>
+      </c>
+      <c r="W20" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y20">
+        <f>0.02020068</f>
+        <v>2.0200679999999999E-2</v>
+      </c>
+      <c r="Z20" s="16">
+        <f>1/(1+EXP(-Y20))</f>
+        <v>0.50504999827283203</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -34466,7 +34488,7 @@
         <f>LN(G21/10)</f>
         <v>0.61518563909023349</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="17">
         <v>15.2</v>
       </c>
       <c r="F21">
@@ -34512,7 +34534,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -34528,7 +34550,7 @@
         <f>1-LN(1/(G22-1) -1)</f>
         <v>7.9067547786486871</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="17">
         <v>1.9</v>
       </c>
       <c r="F22">
@@ -34571,7 +34593,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -34584,7 +34606,7 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="17">
         <v>0</v>
       </c>
       <c r="F23">
@@ -34623,7 +34645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>190</v>
       </c>
@@ -34639,7 +34661,7 @@
         <f t="shared" si="7"/>
         <v>0.05</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="17">
         <v>-1.7999999999999999E-2</v>
       </c>
       <c r="F24">
@@ -34679,7 +34701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -34695,7 +34717,7 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="17">
         <v>0.17499999999999999</v>
       </c>
       <c r="F25">
@@ -34734,7 +34756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -34750,7 +34772,7 @@
         <f>LN(G26)</f>
         <v>1.0986122886681098</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="17">
         <v>0.7</v>
       </c>
       <c r="F26">
@@ -34796,7 +34818,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -34809,7 +34831,7 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="17">
         <v>0</v>
       </c>
       <c r="F27">
@@ -34848,7 +34870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -34861,7 +34883,7 @@
       <c r="D28">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="17">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F28">
@@ -34900,7 +34922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -34916,7 +34938,7 @@
         <f t="shared" si="9"/>
         <v>2.3025850929940459</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="17">
         <v>2.5</v>
       </c>
       <c r="F29">
@@ -34962,7 +34984,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -34978,7 +35000,7 @@
         <f t="shared" si="9"/>
         <v>1.3862943611198906</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="17">
         <v>2.5</v>
       </c>
       <c r="F30">
@@ -35027,7 +35049,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -35043,7 +35065,7 @@
         <f t="shared" si="11"/>
         <v>6.9067547786484651</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="17">
         <v>0.3</v>
       </c>
       <c r="F31">
@@ -35086,7 +35108,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -35102,7 +35124,7 @@
         <f>G32</f>
         <v>0.70559799999999995</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="17">
         <v>0.70559799999999995</v>
       </c>
       <c r="F32">
@@ -35169,7 +35191,7 @@
         <f t="shared" si="12"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="17">
         <v>0.73729999999999996</v>
       </c>
       <c r="F33">
@@ -35231,7 +35253,7 @@
         <f t="shared" si="12"/>
         <v>-9.4310679471241415E-2</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="17">
         <v>0.7</v>
       </c>
       <c r="F34">
@@ -35293,7 +35315,7 @@
         <f t="shared" si="12"/>
         <v>2.9957322735539909</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="17">
         <v>10.5</v>
       </c>
       <c r="F35">
@@ -35355,7 +35377,7 @@
         <f t="shared" si="12"/>
         <v>3.1010977891993172</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="17">
         <v>5.5</v>
       </c>
       <c r="F36">
@@ -35418,7 +35440,7 @@
         <f>-LN(1/G37 -1)</f>
         <v>0.84729786038720356</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="17">
         <v>0.53549999999999998</v>
       </c>
       <c r="F37">
@@ -35477,7 +35499,7 @@
       <c r="D38" s="3">
         <v>1</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="17">
         <v>1</v>
       </c>
       <c r="F38">
@@ -35543,7 +35565,7 @@
         <f>C39</f>
         <v>1.9468676899999999</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="17">
         <v>1.9468676899999999</v>
       </c>
       <c r="F39">
@@ -35598,7 +35620,7 @@
         <f>C40</f>
         <v>1.8597309999999999E-2</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="17">
         <v>1.8597309999999999E-2</v>
       </c>
       <c r="F40">
@@ -35652,7 +35674,7 @@
         <f>B41</f>
         <v>0.26712328767123289</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="17">
         <v>0.26712328767123289</v>
       </c>
       <c r="F41">
@@ -35706,7 +35728,7 @@
         <f>C42</f>
         <v>1</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="17">
         <v>1</v>
       </c>
       <c r="F42">
@@ -35764,7 +35786,7 @@
         <f t="shared" si="16"/>
         <v>0.1449</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="17">
         <v>0.1449</v>
       </c>
       <c r="F43">
@@ -35815,7 +35837,7 @@
         <f t="shared" si="16"/>
         <v>0.1449</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="17">
         <v>0.1449</v>
       </c>
       <c r="F44">
@@ -35864,7 +35886,7 @@
         <f>G45</f>
         <v>0</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="17">
         <v>0</v>
       </c>
       <c r="F45">
@@ -35912,7 +35934,7 @@
         <f>B46</f>
         <v>0</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="17">
         <v>0</v>
       </c>
       <c r="F46">
@@ -35961,7 +35983,7 @@
         <f>C47</f>
         <v>1.0547228200000001</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="17">
         <v>1.0547228200000001</v>
       </c>
       <c r="F47">
@@ -36012,7 +36034,7 @@
         <f>C48</f>
         <v>0.99413825</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="17">
         <v>0.99413825</v>
       </c>
       <c r="F48">
@@ -36063,7 +36085,7 @@
         <f>C49</f>
         <v>0.96310580999999995</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="17">
         <v>0.96310580999999995</v>
       </c>
       <c r="F49">

</xml_diff>

<commit_message>
labors small checks and solve solution
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="641" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB703676-555A-4236-8AC8-1365B807F2AA}"/>
+  <xr:revisionPtr revIDLastSave="683" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18DB2268-5E3B-4B53-84D5-AB5CB6231A4C}"/>
   <bookViews>
-    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -33,8 +33,8 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MOMS!$A$1:$J$59</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PARS!$A$1:$V$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PARS4!$A$1:$V$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PARS!$A$1:$V$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PARS4!$A$1:$V$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">W_psid!$A$1:$CT$98</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="253">
   <si>
     <t>label</t>
   </si>
@@ -947,6 +947,9 @@
   <si>
     <t>aaddS</t>
   </si>
+  <si>
+    <t>typeic</t>
+  </si>
 </sst>
 </file>
 
@@ -1461,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1552,7 +1555,7 @@
         <v>21.03734690643789</v>
       </c>
       <c r="E2" t="b">
-        <f t="shared" ref="E2:E49" si="0">AND(D2&gt;=B2,B2&gt;=C2,D2&gt;=C2)</f>
+        <f t="shared" ref="E2:E50" si="0">AND(D2&gt;=B2,B2&gt;=C2,D2&gt;=C2)</f>
         <v>1</v>
       </c>
       <c r="F2">
@@ -1600,7 +1603,7 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>4.16963103111887E-2</v>
+        <v>0.57156645967836395</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -1667,8 +1670,8 @@
         <v>0.64258992231765177</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q49" ca="1" si="1">RAND()</f>
-        <v>0.3024422396214822</v>
+        <f t="shared" ref="Q3:Q50" ca="1" si="1">RAND()</f>
+        <v>0.90612161278018521</v>
       </c>
       <c r="R3" t="s">
         <v>191</v>
@@ -1738,14 +1741,14 @@
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64188785097531753</v>
+        <v>5.458341727377114E-2</v>
       </c>
       <c r="R4">
         <v>0.6</v>
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>0.82321378674783952</v>
+        <v>0.32033659212896748</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1813,7 +1816,7 @@
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97806804023730431</v>
+        <v>0.56045536670221152</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -1881,7 +1884,7 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12621304320051618</v>
+        <v>0.80668367300244792</v>
       </c>
       <c r="R6" t="s">
         <v>209</v>
@@ -1951,7 +1954,7 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74355143158355297</v>
+        <v>9.8709356069474063E-3</v>
       </c>
       <c r="R7">
         <v>0.5</v>
@@ -2021,7 +2024,7 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39724073783709402</v>
+        <v>0.94319158602773689</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -2088,7 +2091,7 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72811320204081287</v>
+        <v>0.8658183792168026</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -2156,7 +2159,7 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49476047408839297</v>
+        <v>0.35281755800331238</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -2224,7 +2227,7 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89378962096080317</v>
+        <v>0.5922939431403752</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
@@ -2292,7 +2295,7 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86453855308475125</v>
+        <v>0.1610029047996413</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -2360,7 +2363,7 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29725457202220074</v>
+        <v>0.28976811482578491</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2428,7 +2431,7 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55125322541293942</v>
+        <v>0.97900694809405575</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -2496,7 +2499,7 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92602092805223923</v>
+        <v>0.65922024274783741</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -2563,7 +2566,7 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87926440115181714</v>
+        <v>0.74356766186580703</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -2630,7 +2633,7 @@
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61716271391235766</v>
+        <v>0.94125455046333251</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
@@ -2697,7 +2700,7 @@
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16674948733827788</v>
+        <v>0.79163155608962887</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -2765,7 +2768,7 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98325076683942059</v>
+        <v>0.95300232027961984</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
@@ -2832,7 +2835,7 @@
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12948690657688822</v>
+        <v>0.2552038869631974</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
@@ -2899,7 +2902,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41865013114617944</v>
+        <v>0.10541207372424044</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
@@ -2966,7 +2969,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37099886413458893</v>
+        <v>5.1063507792289409E-2</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
@@ -3034,7 +3037,7 @@
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2504999670320508</v>
+        <v>0.59501009144677763</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
@@ -3101,7 +3104,7 @@
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9269228527318658E-2</v>
+        <v>0.69935625706837878</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -3168,7 +3171,7 @@
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.3178934408527696E-2</v>
+        <v>0.85705089031488502</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
@@ -3235,7 +3238,7 @@
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67881912705962233</v>
+        <v>0.3862598253194538</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
@@ -3303,7 +3306,7 @@
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93733565317112311</v>
+        <v>0.84392764827064282</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
@@ -3370,7 +3373,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26561794364320124</v>
+        <v>0.45976868392981918</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
@@ -3437,7 +3440,7 @@
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87333071971885123</v>
+        <v>0.95681308117915098</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
@@ -3504,7 +3507,7 @@
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79172633593924524</v>
+        <v>0.69489204487945144</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -3571,7 +3574,7 @@
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48075732692109441</v>
+        <v>0.16918407714962902</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
@@ -3639,7 +3642,7 @@
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14478728669856578</v>
+        <v>4.1428689585160661E-2</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -3706,7 +3709,7 @@
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49579712362805439</v>
+        <v>0.1080865001904644</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -3773,7 +3776,7 @@
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="1"/>
-        <v>9.670339857496224E-2</v>
+        <v>0.45697369080687722</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -3840,7 +3843,7 @@
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7405359127165918</v>
+        <v>0.98817597586019368</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -3907,7 +3910,7 @@
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30859131920183758</v>
+        <v>0.59210672488367777</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -3974,7 +3977,7 @@
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7929762203774734</v>
+        <v>0.46498510095802226</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -4042,7 +4045,7 @@
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6991065232127216</v>
+        <v>0.31059091627165192</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -4110,7 +4113,7 @@
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67220999423687644</v>
+        <v>0.31823908383638444</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -4178,7 +4181,7 @@
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35068871070300667</v>
+        <v>0.75354011002960519</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -4246,7 +4249,7 @@
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93284530844150504</v>
+        <v>0.50958551431911381</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4314,7 +4317,7 @@
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31002171979609072</v>
+        <v>0.40602634743691557</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -4382,7 +4385,7 @@
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98387684048361046</v>
+        <v>0.10580519333948157</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -4450,7 +4453,7 @@
       </c>
       <c r="Q44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10575222892394553</v>
+        <v>5.7652682020384205E-2</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -4518,7 +4521,7 @@
       </c>
       <c r="Q45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23004190606365216</v>
+        <v>0.54526820881746263</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -4586,27 +4589,27 @@
       </c>
       <c r="Q46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22878475066616399</v>
+        <v>0.19190746330208452</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>179</v>
+        <v>252</v>
       </c>
       <c r="B47">
         <f>PARS!B47</f>
-        <v>1.0696163149411613</v>
+        <v>3.5</v>
       </c>
       <c r="C47">
         <f>PARS!C47</f>
-        <v>1.0696163149411613</v>
+        <v>3.5</v>
       </c>
       <c r="D47">
         <f>PARS!D47</f>
-        <v>1.0696163149411613</v>
+        <v>3.5</v>
       </c>
       <c r="E47" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E47" si="2">AND(D47&gt;=B47,B47&gt;=C47,D47&gt;=C47)</f>
         <v>1</v>
       </c>
       <c r="F47">
@@ -4627,11 +4630,11 @@
       </c>
       <c r="J47">
         <f>PARS!O47</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K47">
         <f>PARS!P47</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47">
         <f>PARS!Q47</f>
@@ -4650,28 +4653,28 @@
         <v>0</v>
       </c>
       <c r="P47">
-        <v>0.80782005028098203</v>
+        <v>1.7297503412316</v>
       </c>
       <c r="Q47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30424062893179071</v>
+        <v>0.65888597512593172</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48">
         <f>PARS!B48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="C48">
         <f>PARS!C48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="D48">
         <f>PARS!D48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="E48" t="b">
         <f t="shared" si="0"/>
@@ -4718,28 +4721,28 @@
         <v>0</v>
       </c>
       <c r="P48">
-        <v>7.2670121740322058E-2</v>
+        <v>0.80782005028098203</v>
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25968288327710798</v>
+        <v>0.86422618995173051</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49">
         <f>PARS!B49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="C49">
         <f>PARS!C49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="D49">
         <f>PARS!D49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="E49" t="b">
         <f t="shared" si="0"/>
@@ -4786,11 +4789,79 @@
         <v>0</v>
       </c>
       <c r="P49">
-        <v>0.14486889267994729</v>
+        <v>7.2670121740322058E-2</v>
       </c>
       <c r="Q49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83941293194279099</v>
+        <v>0.74306755341584407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50">
+        <f>PARS!B50</f>
+        <v>0.9618468890261952</v>
+      </c>
+      <c r="C50">
+        <f>PARS!C50</f>
+        <v>0.9618468890261952</v>
+      </c>
+      <c r="D50">
+        <f>PARS!D50</f>
+        <v>0.9618468890261952</v>
+      </c>
+      <c r="E50" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <f>PARS!K50</f>
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <f>PARS!L50</f>
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <f>PARS!M50</f>
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f>PARS!N50</f>
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <f>PARS!O50</f>
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <f>PARS!P50</f>
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <f>PARS!Q50</f>
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <f>PARS!R50</f>
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <f>PARS!S50</f>
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <f>PARS!T50</f>
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0.14486889267994729</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22509139459115857</v>
       </c>
     </row>
   </sheetData>
@@ -33540,17 +33611,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
-  <dimension ref="A1:Z49"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.36328125" customWidth="1"/>
     <col min="5" max="5" width="25.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.54296875" customWidth="1"/>
     <col min="25" max="25" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.453125" bestFit="1" customWidth="1"/>
@@ -33665,15 +33737,15 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P49" si="0">SUM(L2:O2)</f>
+        <f t="shared" ref="P2:P50" si="0">SUM(L2:O2)</f>
         <v>1</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S49" si="1">L2-Q2</f>
+        <f t="shared" ref="S2:S50" si="1">L2-Q2</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T49" si="2">S2+N2+Q2+M2</f>
+        <f t="shared" ref="T2:T50" si="2">S2+N2+Q2+M2</f>
         <v>1</v>
       </c>
       <c r="U2">
@@ -36087,7 +36159,7 @@
         <v>0</v>
       </c>
       <c r="U42">
-        <f t="shared" ref="U42:U49" si="16">T42</f>
+        <f t="shared" ref="U42:U50" si="16">T42</f>
         <v>0</v>
       </c>
       <c r="V42"/>
@@ -36291,83 +36363,59 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47">
+        <v>252</v>
+      </c>
+      <c r="B47" s="17">
         <f>E47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="C47">
+        <v>3.5</v>
+      </c>
+      <c r="C47" s="17">
         <f>B47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="D47">
-        <f>C47</f>
-        <v>1.0696163149411613</v>
+        <v>3.5</v>
+      </c>
+      <c r="D47" s="17">
+        <f>B47</f>
+        <v>3.5</v>
       </c>
       <c r="E47" s="17">
-        <f>EXP(0.0673)</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="F47">
+        <v>3.5</v>
+      </c>
+      <c r="F47" s="17">
         <f>E47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="G47">
+        <v>3.5</v>
+      </c>
+      <c r="G47" s="17">
         <f>E47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="J47">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="O47">
-        <v>1</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="S47">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T47">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="U47">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48">
         <f>E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="C48">
         <f>B48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="D48">
         <f>C48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="E48" s="17">
-        <f>EXP(-0.0062)</f>
-        <v>0.99381918034015848</v>
+        <f>EXP(0.0673)</f>
+        <v>1.0696163149411613</v>
       </c>
       <c r="F48">
         <f>E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="G48">
         <f>E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="J48">
         <f>1</f>
@@ -36395,60 +36443,112 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49">
         <f>E49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="C49">
         <f>B49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="D49">
         <f>C49</f>
+        <v>0.99381918034015848</v>
+      </c>
+      <c r="E49" s="17">
+        <f>EXP(-0.0062)</f>
+        <v>0.99381918034015848</v>
+      </c>
+      <c r="F49">
+        <f>E49</f>
+        <v>0.99381918034015848</v>
+      </c>
+      <c r="G49">
+        <f>E49</f>
+        <v>0.99381918034015848</v>
+      </c>
+      <c r="J49">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50">
+        <f>E50</f>
         <v>0.9618468890261952</v>
       </c>
-      <c r="E49" s="17">
+      <c r="C50">
+        <f>B50</f>
+        <v>0.9618468890261952</v>
+      </c>
+      <c r="D50">
+        <f>C50</f>
+        <v>0.9618468890261952</v>
+      </c>
+      <c r="E50" s="17">
         <f>EXP(-0.0389)</f>
         <v>0.9618468890261952</v>
       </c>
-      <c r="F49">
-        <f>E49</f>
+      <c r="F50">
+        <f>E50</f>
         <v>0.9618468890261952</v>
       </c>
-      <c r="G49">
-        <f>E49</f>
+      <c r="G50">
+        <f>E50</f>
         <v>0.9618468890261952</v>
       </c>
-      <c r="J49">
+      <c r="J50">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="O49">
-        <v>1</v>
-      </c>
-      <c r="P49">
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="S49">
+      <c r="S50">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T49">
+      <c r="T50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U49">
+      <c r="U50">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V49" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V49">
-      <sortCondition ref="I1:I49"/>
+  <autoFilter ref="A1:V50" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V50">
+      <sortCondition ref="I1:I50"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36459,10 +36559,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AAA591-394B-45A3-997C-6B60BB5B6F0D}">
-  <dimension ref="A1:Z52"/>
+  <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A16" zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="G47" sqref="B47:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -36470,6 +36570,7 @@
     <col min="2" max="2" width="8.90625" customWidth="1"/>
     <col min="3" max="4" width="6.36328125" customWidth="1"/>
     <col min="5" max="5" width="25.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
     <col min="22" max="22" width="19.54296875" customWidth="1"/>
     <col min="25" max="25" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="18.453125" bestFit="1" customWidth="1"/>
@@ -36585,15 +36686,15 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P49" si="0">SUM(L2:O2)</f>
+        <f t="shared" ref="P2:P50" si="0">SUM(L2:O2)</f>
         <v>1</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:S49" si="1">L2-Q2</f>
+        <f t="shared" ref="S2:S50" si="1">L2-Q2</f>
         <v>0</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T49" si="2">S2+N2+Q2+M2</f>
+        <f t="shared" ref="T2:T50" si="2">S2+N2+Q2+M2</f>
         <v>1</v>
       </c>
       <c r="U2">
@@ -39043,7 +39144,7 @@
         <v>0</v>
       </c>
       <c r="U42">
-        <f t="shared" ref="U42:U49" si="15">T42</f>
+        <f t="shared" ref="U42:U50" si="15">T42</f>
         <v>0</v>
       </c>
       <c r="V42"/>
@@ -39251,34 +39352,33 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47">
+        <v>252</v>
+      </c>
+      <c r="B47" s="11">
         <f>E47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="C47">
+        <v>3.5</v>
+      </c>
+      <c r="C47" s="11">
         <f>B47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="D47">
-        <f>C47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="E47" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="D47" s="11">
+        <f>B47</f>
+        <v>3.5</v>
+      </c>
+      <c r="E47" s="11">
         <f>PARS!E47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="F47">
-        <f>E47</f>
-        <v>1.0696163149411613</v>
-      </c>
-      <c r="G47">
-        <f>E47</f>
-        <v>1.0696163149411613</v>
+        <v>3.5</v>
+      </c>
+      <c r="F47" s="11">
+        <f>PARS!F47</f>
+        <v>3.5</v>
+      </c>
+      <c r="G47" s="11">
+        <f>PARS!G47</f>
+        <v>3.5</v>
       </c>
       <c r="J47">
-        <f>1</f>
         <v>1</v>
       </c>
       <c r="O47">
@@ -39289,45 +39389,45 @@
         <v>1</v>
       </c>
       <c r="S47">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="S47:S48" si="17">L47-Q47</f>
         <v>0</v>
       </c>
       <c r="T47">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T47:T48" si="18">S47+N47+Q47+M47</f>
         <v>0</v>
       </c>
       <c r="U47">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="U47:U48" si="19">T47</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B48">
         <f>E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="C48">
         <f>B48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="D48">
         <f>C48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="E48" s="17">
         <f>PARS!E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="F48">
         <f>E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="G48">
         <f>E48</f>
-        <v>0.99381918034015848</v>
+        <v>1.0696163149411613</v>
       </c>
       <c r="J48">
         <f>1</f>
@@ -39341,45 +39441,45 @@
         <v>1</v>
       </c>
       <c r="S48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="T48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49">
         <f>E49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="C49">
         <f>B49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="D49">
         <f>C49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="E49" s="17">
         <f>PARS!E49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="F49">
         <f>E49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="G49">
         <f>E49</f>
-        <v>0.9618468890261952</v>
+        <v>0.99381918034015848</v>
       </c>
       <c r="J49">
         <f>1</f>
@@ -39407,54 +39507,106 @@
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>249</v>
-      </c>
-      <c r="B50" s="17">
+        <v>181</v>
+      </c>
+      <c r="B50">
         <f>E50</f>
-        <v>1.1000000000000001</v>
+        <v>0.9618468890261952</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <f>B50</f>
+        <v>0.9618468890261952</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <f>C50</f>
+        <v>0.9618468890261952</v>
       </c>
       <c r="E50" s="17">
-        <v>1.1000000000000001</v>
+        <f>PARS!E50</f>
+        <v>0.9618468890261952</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <f>E50</f>
+        <v>0.9618468890261952</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <f>E50</f>
+        <v>0.9618468890261952</v>
+      </c>
+      <c r="J50">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>250</v>
-      </c>
-      <c r="B51" s="11">
-        <v>0.35</v>
+        <v>249</v>
+      </c>
+      <c r="B51" s="17">
+        <f>E51</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
       </c>
       <c r="E51" s="17">
-        <v>0.35</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>250</v>
+      </c>
+      <c r="B52" s="11">
+        <v>0.35</v>
+      </c>
+      <c r="E52" s="17">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>251</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B53" s="11">
         <v>23</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E53" s="17">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V49" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V49">
-      <sortCondition ref="I1:I49"/>
+  <autoFilter ref="A1:V50" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V50">
+      <sortCondition ref="I1:I50"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new checks on proper inputs
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18DB2268-5E3B-4B53-84D5-AB5CB6231A4C}"/>
+  <xr:revisionPtr revIDLastSave="685" documentId="13_ncr:1_{1F6193A1-24F7-47AE-86D6-8C72A9FF5A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0C687B3-269E-4E77-8AB4-FFBF97383813}"/>
   <bookViews>
-    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="350" yWindow="170" windowWidth="18850" windowHeight="10630" activeTab="3" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>0.57156645967836395</v>
+        <v>0.58994597876812738</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q50" ca="1" si="1">RAND()</f>
-        <v>0.90612161278018521</v>
+        <v>0.7940849879876265</v>
       </c>
       <c r="R3" t="s">
         <v>191</v>
@@ -1741,14 +1741,14 @@
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="1"/>
-        <v>5.458341727377114E-2</v>
+        <v>0.14365803542526023</v>
       </c>
       <c r="R4">
         <v>0.6</v>
       </c>
       <c r="S4">
         <f ca="1">RAND()</f>
-        <v>0.32033659212896748</v>
+        <v>0.47388861920661651</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56045536670221152</v>
+        <v>0.95505603842718556</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80668367300244792</v>
+        <v>0.98275646893500501</v>
       </c>
       <c r="R6" t="s">
         <v>209</v>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8709356069474063E-3</v>
+        <v>0.43481116132383013</v>
       </c>
       <c r="R7">
         <v>0.5</v>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94319158602773689</v>
+        <v>0.1299887905410676</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -2091,7 +2091,7 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8658183792168026</v>
+        <v>0.98465524653922598</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35281755800331238</v>
+        <v>0.78087817157180772</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5922939431403752</v>
+        <v>0.38583064384671684</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
@@ -2295,7 +2295,7 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1610029047996413</v>
+        <v>0.81911966748362586</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28976811482578491</v>
+        <v>0.55553839680094219</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97900694809405575</v>
+        <v>0.20762300055702354</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -2499,7 +2499,7 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65922024274783741</v>
+        <v>0.70408177047192066</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74356766186580703</v>
+        <v>0.2014809548003097</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94125455046333251</v>
+        <v>0.94649924656606321</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.35">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79163155608962887</v>
+        <v>0.32509210739867755</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95300232027961984</v>
+        <v>0.61605778583877446</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2552038869631974</v>
+        <v>0.49476076164563199</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10541207372424044</v>
+        <v>0.25081530441014377</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1063507792289409E-2</v>
+        <v>0.80854201055314767</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.35">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59501009144677763</v>
+        <v>0.15384709104100747</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.35">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69935625706837878</v>
+        <v>0.14119590188244557</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
@@ -3171,7 +3171,7 @@
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85705089031488502</v>
+        <v>0.52113719762615807</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.35">
@@ -3238,7 +3238,7 @@
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3862598253194538</v>
+        <v>0.76215149294123508</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.35">
@@ -3306,7 +3306,7 @@
       </c>
       <c r="Q27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84392764827064282</v>
+        <v>0.72381758772976412</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
@@ -3373,7 +3373,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45976868392981918</v>
+        <v>0.45480505457365561</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="Q29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95681308117915098</v>
+        <v>0.57723458964930419</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="Q30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69489204487945144</v>
+        <v>0.43736209392916681</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -3574,7 +3574,7 @@
       </c>
       <c r="Q31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16918407714962902</v>
+        <v>0.50289665987690468</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
@@ -3642,7 +3642,7 @@
       </c>
       <c r="Q32">
         <f t="shared" ca="1" si="1"/>
-        <v>4.1428689585160661E-2</v>
+        <v>0.54903753471562011</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="Q33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1080865001904644</v>
+        <v>0.49773878460640841</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="Q34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45697369080687722</v>
+        <v>0.31296672608259557</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -3843,7 +3843,7 @@
       </c>
       <c r="Q35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98817597586019368</v>
+        <v>0.26398686700868079</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -3910,7 +3910,7 @@
       </c>
       <c r="Q36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59210672488367777</v>
+        <v>0.57693098042797486</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -3977,7 +3977,7 @@
       </c>
       <c r="Q37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46498510095802226</v>
+        <v>0.86701986183717128</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="Q38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31059091627165192</v>
+        <v>0.38260854457419047</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="Q39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31823908383638444</v>
+        <v>0.49853279315829202</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="Q40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75354011002960519</v>
+        <v>0.23578822221740481</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="Q41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50958551431911381</v>
+        <v>0.19291077411522295</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -4317,7 +4317,7 @@
       </c>
       <c r="Q42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40602634743691557</v>
+        <v>1.0408223074551914E-2</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -4385,7 +4385,7 @@
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10580519333948157</v>
+        <v>0.24615240558694573</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -4453,7 +4453,7 @@
       </c>
       <c r="Q44">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7652682020384205E-2</v>
+        <v>0.55361799324505712</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="Q45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54526820881746263</v>
+        <v>0.1850034244025146</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="Q46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19190746330208452</v>
+        <v>0.4341008715885164</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
@@ -4657,7 +4657,7 @@
       </c>
       <c r="Q47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65888597512593172</v>
+        <v>0.37716188410386076</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="Q48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86422618995173051</v>
+        <v>0.32123899226488295</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.35">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="Q49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74306755341584407</v>
+        <v>9.8222381398271774E-2</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.35">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="Q50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22509139459115857</v>
+        <v>0.8601608780790595</v>
       </c>
     </row>
   </sheetData>
@@ -33613,7 +33613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
+    <sheetView zoomScale="57" zoomScaleNormal="43" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
@@ -39620,8 +39620,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
sa new inpiut +solve correction
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{D747905C-8763-4973-AEA7-B75115B0758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29EF8830-21AB-40C5-9E28-E62947720775}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{D747905C-8763-4973-AEA7-B75115B0758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11950ACA-83E2-46EE-8000-D7AF06287D1C}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="170" windowWidth="18840" windowHeight="10630" firstSheet="6" activeTab="11" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="360" yWindow="170" windowWidth="18840" windowHeight="10630" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -1473,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,7 +1516,7 @@
         <v>78</v>
       </c>
       <c r="B2">
-        <f>PARS!B2</f>
+        <f>PARS!B2*I7+G2*(1-I7)*C2+(1-G2)*(1-I7)*D2</f>
         <v>22.35498373964581</v>
       </c>
       <c r="C2">
@@ -1535,11 +1535,11 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.53105654242295719</v>
+        <v>0.70565949244746939</v>
       </c>
       <c r="H2">
         <f ca="1">RAND()</f>
-        <v>0.2369340678095132</v>
+        <v>0.65769196127086904</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1547,7 +1547,7 @@
         <v>111</v>
       </c>
       <c r="B3">
-        <f>PARS!B3</f>
+        <f>PARS!B3*I8+G3*(1-I8)*C3+(1-G3)*(1-I8)*D3</f>
         <v>1.8814014327029097E-3</v>
       </c>
       <c r="C3">
@@ -1566,11 +1566,11 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.49093251050534092</v>
+        <v>0.82960022595885474</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H52" ca="1" si="1">RAND()</f>
-        <v>0.20520434719207903</v>
+        <v>7.849232483356261E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1578,8 +1578,8 @@
         <v>75</v>
       </c>
       <c r="B4">
-        <f>PARS!B4</f>
-        <v>-0.21072103131565253</v>
+        <f>PARS!B4*I9+G4*(1-I9)*C4+(1-G4)*(1-I9)*D4</f>
+        <v>-8.7401763022181195E-2</v>
       </c>
       <c r="C4">
         <f>PARS!C4</f>
@@ -1597,11 +1597,11 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>8.2968856403746627E-2</v>
+        <v>0.38912849591084697</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46862854232923812</v>
+        <v>5.6863140950835223E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1609,8 +1609,8 @@
         <v>76</v>
       </c>
       <c r="B5">
-        <f>PARS!B5</f>
-        <v>-0.21072103131565253</v>
+        <f>PARS!B5*I10+G5*(1-I10)*C5+(1-G5)*(1-I10)*D5</f>
+        <v>-0.48430963502277175</v>
       </c>
       <c r="C5">
         <f>PARS!C5</f>
@@ -1628,11 +1628,11 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0.16382742191683908</v>
+        <v>0.96174551453589041</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73168201944817213</v>
+        <v>0.74153362301212855</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1640,7 +1640,7 @@
         <v>249</v>
       </c>
       <c r="B6">
-        <f>PARS!B6</f>
+        <f>PARS!B6*I11+G6*(1-I11)*C6+(1-G6)*(1-I11)*D6</f>
         <v>0</v>
       </c>
       <c r="C6">
@@ -1659,11 +1659,11 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.89922009441709028</v>
+        <v>9.4270068424736175E-2</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67706551238939783</v>
+        <v>0.72088439617123712</v>
       </c>
       <c r="I6" t="s">
         <v>206</v>
@@ -1674,7 +1674,7 @@
         <v>106</v>
       </c>
       <c r="B7">
-        <f>PARS!B7</f>
+        <f>PARS!B7*I12+G7*(1-I12)*C7+(1-G7)*(1-I12)*D7</f>
         <v>0.20836072497837904</v>
       </c>
       <c r="C7">
@@ -1693,11 +1693,11 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.91932096982163469</v>
+        <v>0.4113217044552836</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43584826062035265</v>
+        <v>0.34118517076156818</v>
       </c>
       <c r="I7">
         <v>0.5</v>
@@ -1708,8 +1708,8 @@
         <v>74</v>
       </c>
       <c r="B8">
-        <f>PARS!B8</f>
-        <v>-1.4064970684374101</v>
+        <f>PARS!B8*I13+G8*(1-I13)*C8+(1-G8)*(1-I13)*D8</f>
+        <v>-1.64714284940866</v>
       </c>
       <c r="C8">
         <f>PARS!C8</f>
@@ -1727,11 +1727,11 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0.87103404008515395</v>
+        <v>0.52719836279511412</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25913839288354901</v>
+        <v>0.55729883043625617</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1739,8 +1739,8 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <f>PARS!B9</f>
-        <v>-1.0050335853501451E-2</v>
+        <f>PARS!B9*I14+G9*(1-I14)*C9+(1-G9)*(1-I14)*D9</f>
+        <v>8.8440844998536133E-2</v>
       </c>
       <c r="C9">
         <f>PARS!C9</f>
@@ -1758,11 +1758,11 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0.39312911499027259</v>
+        <v>0.70670829246774514</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1207267389165344</v>
+        <v>0.99024436557385676</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1770,8 +1770,8 @@
         <v>93</v>
       </c>
       <c r="B10">
-        <f>PARS!B10</f>
-        <v>1.3837912309017721</v>
+        <f>PARS!B10*I15+G10*(1-I15)*C10+(1-G10)*(1-I15)*D10</f>
+        <v>1.6152003232964534</v>
       </c>
       <c r="C10">
         <f>PARS!C10</f>
@@ -1789,11 +1789,11 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0.37807164831515072</v>
+        <v>0.16071106044667616</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25072836704816082</v>
+        <v>0.47655620488680939</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1801,8 +1801,8 @@
         <v>98</v>
       </c>
       <c r="B11">
-        <f>PARS!B11</f>
-        <v>-1.0050335853501451E-2</v>
+        <f>PARS!B11*I16+G11*(1-I16)*C11+(1-G11)*(1-I16)*D11</f>
+        <v>1.2953205991163744E-2</v>
       </c>
       <c r="C11">
         <f>PARS!C11</f>
@@ -1820,11 +1820,11 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>4.563226419872779E-2</v>
+        <v>0.24434687978672864</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92063822318779487</v>
+        <v>0.74591850432854645</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1832,8 +1832,8 @@
         <v>95</v>
       </c>
       <c r="B12">
-        <f>PARS!B12</f>
-        <v>-1.8703217532696195</v>
+        <f>PARS!B12*I17+G12*(1-I17)*C12+(1-G12)*(1-I17)*D12</f>
+        <v>-1.4633181688701251</v>
       </c>
       <c r="C12">
         <f>PARS!C12</f>
@@ -1851,11 +1851,11 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.67349394205356494</v>
+        <v>0.31228472165726406</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95984424344867092</v>
+        <v>0.86468638637519846</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1863,8 +1863,8 @@
         <v>94</v>
       </c>
       <c r="B13">
-        <f>PARS!B13</f>
-        <v>0.66388228523152282</v>
+        <f>PARS!B13*I18+G13*(1-I18)*C13+(1-G13)*(1-I18)*D13</f>
+        <v>0.11422542005384539</v>
       </c>
       <c r="C13">
         <f>PARS!C13</f>
@@ -1882,11 +1882,11 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0.20805081519983726</v>
+        <v>0.64313475873133097</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30436490415107431</v>
+        <v>3.4183403856123729E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1894,8 +1894,8 @@
         <v>97</v>
       </c>
       <c r="B14">
-        <f>PARS!B14</f>
-        <v>-8.9025505804146685E-2</v>
+        <f>PARS!B14*I19+G14*(1-I19)*C14+(1-G14)*(1-I19)*D14</f>
+        <v>0.93721483979018483</v>
       </c>
       <c r="C14">
         <f>PARS!C14</f>
@@ -1907,17 +1907,17 @@
       </c>
       <c r="E14" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>8.7793255145312332E-2</v>
+        <v>0.42586121365915364</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79898946280639638</v>
+        <v>0.48020001730382811</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1925,8 +1925,8 @@
         <v>99</v>
       </c>
       <c r="B15">
-        <f>PARS!B15</f>
-        <v>0.25702382969694959</v>
+        <f>PARS!B15*I20+G15*(1-I20)*C15+(1-G15)*(1-I20)*D15</f>
+        <v>0.33401065681115644</v>
       </c>
       <c r="C15">
         <f>PARS!C15</f>
@@ -1944,11 +1944,11 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0.60409353771514374</v>
+        <v>7.8022463922200469E-4</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47151743474927721</v>
+        <v>0.62249345155605096</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1956,8 +1956,8 @@
         <v>70</v>
       </c>
       <c r="B16">
-        <f>PARS!B16</f>
-        <v>-2.3633295407393207</v>
+        <f>PARS!B16*I21+G16*(1-I21)*C16+(1-G16)*(1-I21)*D16</f>
+        <v>-2.5836226227271579</v>
       </c>
       <c r="C16">
         <f>PARS!C16</f>
@@ -1969,17 +1969,17 @@
       </c>
       <c r="E16" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>0.14159005981771311</v>
+        <v>0.51736468802637281</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89146959112813073</v>
+        <v>0.95804142526012015</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1987,8 +1987,8 @@
         <v>77</v>
       </c>
       <c r="B17">
-        <f>PARS!B17</f>
-        <v>-1.4146938356415886</v>
+        <f>PARS!B17*I22+G17*(1-I22)*C17+(1-G17)*(1-I22)*D17</f>
+        <v>-1.5264206258049868</v>
       </c>
       <c r="C17">
         <f>PARS!C17</f>
@@ -2006,11 +2006,11 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0.552769905166271</v>
+        <v>0.31785730775376519</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93899008433620257</v>
+        <v>2.8389119349351732E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2018,8 +2018,8 @@
         <v>96</v>
       </c>
       <c r="B18">
-        <f>PARS!B18</f>
-        <v>-0.41551544396166579</v>
+        <f>PARS!B18*I23+G18*(1-I23)*C18+(1-G18)*(1-I23)*D18</f>
+        <v>-0.96267416692065189</v>
       </c>
       <c r="C18">
         <f>PARS!C18</f>
@@ -2037,11 +2037,11 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0.69621332925647528</v>
+        <v>0.7995813223203333</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66099174516013837</v>
+        <v>0.14528750511859556</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2049,8 +2049,8 @@
         <v>71</v>
       </c>
       <c r="B19">
-        <f>PARS!B19</f>
-        <v>1.9878743481543455</v>
+        <f>PARS!B19*I24+G19*(1-I24)*C19+(1-G19)*(1-I24)*D19</f>
+        <v>2.2545082746416285</v>
       </c>
       <c r="C19">
         <f>PARS!C19</f>
@@ -2068,11 +2068,11 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>0.79118853390002408</v>
+        <v>0.11919901494191087</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32638349323062521</v>
+        <v>0.61013533842258982</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -2080,7 +2080,7 @@
         <v>72</v>
       </c>
       <c r="B20">
-        <f>PARS!B20</f>
+        <f>PARS!B20*I25+G20*(1-I25)*C20+(1-G20)*(1-I25)*D20</f>
         <v>2000</v>
       </c>
       <c r="C20">
@@ -2099,11 +2099,11 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0.88325503098242519</v>
+        <v>0.2975561090325638</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61361196136036755</v>
+        <v>0.75382606377527794</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2111,8 +2111,8 @@
         <v>73</v>
       </c>
       <c r="B21">
-        <f>PARS!B21</f>
-        <v>24.401210673453068</v>
+        <f>PARS!B21*I26+G21*(1-I26)*C21+(1-G21)*(1-I26)*D21</f>
+        <v>393.21755459057232</v>
       </c>
       <c r="C21">
         <f>PARS!C21</f>
@@ -2130,11 +2130,11 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>3.8661446103829711E-2</v>
+        <v>3.0206183646077633E-2</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6703521123083993E-2</v>
+        <v>9.8714494250589535E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2142,8 +2142,8 @@
         <v>68</v>
       </c>
       <c r="B22">
-        <f>PARS!B22</f>
-        <v>0.42526773540434409</v>
+        <f>PARS!B22*I27+G22*(1-I27)*C22+(1-G22)*(1-I27)*D22</f>
+        <v>0.58798288520497644</v>
       </c>
       <c r="C22">
         <f>PARS!C22</f>
@@ -2161,11 +2161,11 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0.86502061339991732</v>
+        <v>0.11165963934177736</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12555378973699882</v>
+        <v>4.2207943698611583E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2173,8 +2173,8 @@
         <v>79</v>
       </c>
       <c r="B23">
-        <f>PARS!B23</f>
-        <v>3.1972245773362191</v>
+        <f>PARS!B23*I28+G23*(1-I28)*C23+(1-G23)*(1-I28)*D23</f>
+        <v>4.3004317430634984</v>
       </c>
       <c r="C23">
         <f>PARS!C23</f>
@@ -2192,11 +2192,11 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0.90552454422183626</v>
+        <v>0.52214435739540899</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10093889694236802</v>
+        <v>0.76973651381473984</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2204,7 +2204,7 @@
         <v>80</v>
       </c>
       <c r="B24">
-        <f>PARS!B24</f>
+        <f>PARS!B24*I29+G24*(1-I29)*C24+(1-G24)*(1-I29)*D24</f>
         <v>0</v>
       </c>
       <c r="C24">
@@ -2223,11 +2223,11 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>3.0826840635846953E-3</v>
+        <v>0.81454013501391653</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43427745229095172</v>
+        <v>0.52961167452589664</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2235,8 +2235,8 @@
         <v>190</v>
       </c>
       <c r="B25">
-        <f>PARS!B25</f>
-        <v>-1.6E-2</v>
+        <f>PARS!B25*I30+G25*(1-I30)*C25+(1-G25)*(1-I30)*D25</f>
+        <v>-0.13314866218669968</v>
       </c>
       <c r="C25">
         <f>PARS!C25</f>
@@ -2254,11 +2254,11 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>0.5335079973158724</v>
+        <v>0.91574331093349837</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53650146197884985</v>
+        <v>0.30116553485453745</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2266,8 +2266,8 @@
         <v>81</v>
       </c>
       <c r="B26">
-        <f>PARS!B26</f>
-        <v>0.17499999999999999</v>
+        <f>PARS!B26*I31+G26*(1-I31)*C26+(1-G26)*(1-I31)*D26</f>
+        <v>0.496646342796629</v>
       </c>
       <c r="C26">
         <f>PARS!C26</f>
@@ -2285,11 +2285,11 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <v>0.1379461107019333</v>
+        <v>6.7073144067419932E-3</v>
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41818168574768511</v>
+        <v>0.86321180601678171</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2297,8 +2297,8 @@
         <v>82</v>
       </c>
       <c r="B27">
-        <f>PARS!B27</f>
-        <v>-0.51082562376599072</v>
+        <f>PARS!B27*I32+G27*(1-I32)*C27+(1-G27)*(1-I32)*D27</f>
+        <v>-0.55276232175545625</v>
       </c>
       <c r="C27">
         <f>PARS!C27</f>
@@ -2316,11 +2316,11 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>0.15594482562436407</v>
+        <v>0.65673732407091134</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4922319789623758</v>
+        <v>0.54050678088491444</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2328,7 +2328,7 @@
         <v>100</v>
       </c>
       <c r="B28">
-        <f>PARS!B28</f>
+        <f>PARS!B28*I33+G28*(1-I33)*C28+(1-G28)*(1-I33)*D28</f>
         <v>0</v>
       </c>
       <c r="C28">
@@ -2347,11 +2347,11 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0.36385250657588908</v>
+        <v>0.5764051124739652</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58644776461973447</v>
+        <v>0.81397996868248546</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2359,7 +2359,7 @@
         <v>103</v>
       </c>
       <c r="B29">
-        <f>PARS!B29</f>
+        <f>PARS!B29*I34+G29*(1-I34)*C29+(1-G29)*(1-I34)*D29</f>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C29">
@@ -2378,11 +2378,11 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <v>0.98514857668021316</v>
+        <v>9.142069164412836E-2</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94375708438887573</v>
+        <v>0.1349550851561282</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2390,8 +2390,8 @@
         <v>86</v>
       </c>
       <c r="B30">
-        <f>PARS!B30</f>
-        <v>0.87546873735389985</v>
+        <f>PARS!B30*I35+G30*(1-I35)*C30+(1-G30)*(1-I35)*D30</f>
+        <v>0.83713894111049081</v>
       </c>
       <c r="C30">
         <f>PARS!C30</f>
@@ -2409,11 +2409,11 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <v>0.8781065389559034</v>
+        <v>0.63643517728938259</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>9.398118407004008E-2</v>
+        <v>0.38865015400801828</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2421,8 +2421,8 @@
         <v>83</v>
       </c>
       <c r="B31">
-        <f>PARS!B31</f>
-        <v>0.91629073187415511</v>
+        <f>PARS!B31*I36+G31*(1-I36)*C31+(1-G31)*(1-I36)*D31</f>
+        <v>1.277862732282995</v>
       </c>
       <c r="C31">
         <f>PARS!C31</f>
@@ -2440,11 +2440,11 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <v>0.12871016653382228</v>
+        <v>0.13579284125938318</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61642871575729552</v>
+        <v>0.22584334838783615</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2452,8 +2452,8 @@
         <v>84</v>
       </c>
       <c r="B32">
-        <f>PARS!B32</f>
-        <v>-0.99462257514406194</v>
+        <f>PARS!B32*I37+G32*(1-I37)*C32+(1-G32)*(1-I37)*D32</f>
+        <v>0.94471181985817099</v>
       </c>
       <c r="C32">
         <f>PARS!C32</f>
@@ -2471,11 +2471,11 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <v>0.5450423747539993</v>
+        <v>0.65488318082257346</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24943967840141712</v>
+        <v>0.67100174498123444</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -2483,7 +2483,7 @@
         <v>85</v>
       </c>
       <c r="B33">
-        <f>PARS!B33</f>
+        <f>PARS!B33*I38+G33*(1-I38)*C33+(1-G33)*(1-I38)*D33</f>
         <v>0.70559799999999995</v>
       </c>
       <c r="C33">
@@ -2502,11 +2502,11 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>0.55215907036823553</v>
+        <v>0.21918108700723871</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52997840231627458</v>
+        <v>0.65313692939244294</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2514,8 +2514,8 @@
         <v>87</v>
       </c>
       <c r="B34">
-        <f>PARS!B34</f>
-        <v>-0.3285040669720361</v>
+        <f>PARS!B34*I39+G34*(1-I39)*C34+(1-G34)*(1-I39)*D34</f>
+        <v>-1.5345348954935678</v>
       </c>
       <c r="C34">
         <f>PARS!C34</f>
@@ -2533,11 +2533,11 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <v>0.36597743517783687</v>
+        <v>0.74361854552866957</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81053904671251731</v>
+        <v>0.13956371097270459</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2545,8 +2545,8 @@
         <v>88</v>
       </c>
       <c r="B35">
-        <f>PARS!B35</f>
-        <v>-0.2744368457017603</v>
+        <f>PARS!B35*I40+G35*(1-I40)*C35+(1-G35)*(1-I40)*D35</f>
+        <v>-0.50568533719337683</v>
       </c>
       <c r="C35">
         <f>PARS!C35</f>
@@ -2564,11 +2564,11 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <v>6.9601791823036607E-2</v>
+        <v>0.66453732192708659</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.240987630420193</v>
+        <v>0.21584463695098244</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2576,8 +2576,8 @@
         <v>89</v>
       </c>
       <c r="B36">
-        <f>PARS!B36</f>
-        <v>2.5297206655777931</v>
+        <f>PARS!B36*I41+G36*(1-I41)*C36+(1-G36)*(1-I41)*D36</f>
+        <v>-6.8447657882925643</v>
       </c>
       <c r="C36">
         <f>PARS!C36</f>
@@ -2595,11 +2595,11 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <v>0.77405733771362362</v>
+        <v>0.99363966578890262</v>
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9011513519142591</v>
+        <v>0.23730175329141101</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2607,8 +2607,8 @@
         <v>102</v>
       </c>
       <c r="B37">
-        <f>PARS!B37</f>
-        <v>1.2527629684953681</v>
+        <f>PARS!B37*I42+G37*(1-I42)*C37+(1-G37)*(1-I42)*D37</f>
+        <v>-2.9040792258598831</v>
       </c>
       <c r="C37">
         <f>PARS!C37</f>
@@ -2626,11 +2626,11 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <v>0.87369915063133508</v>
+        <v>0.59998652934069929</v>
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.838891501726994</v>
+        <v>0.37579925928981306</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2638,8 +2638,8 @@
         <v>69</v>
       </c>
       <c r="B38">
-        <f>PARS!B38</f>
-        <v>0.14304340786103839</v>
+        <f>PARS!B38*I43+G38*(1-I43)*C38+(1-G38)*(1-I43)*D38</f>
+        <v>0.76367961433668796</v>
       </c>
       <c r="C38">
         <f>PARS!C38</f>
@@ -2657,11 +2657,11 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <v>0.98561471154886982</v>
+        <v>9.423863964609136E-2</v>
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57681653397881405</v>
+        <v>0.76437868040332513</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2669,7 +2669,7 @@
         <v>107</v>
       </c>
       <c r="B39">
-        <f>PARS!B39</f>
+        <f>PARS!B39*I44+G39*(1-I44)*C39+(1-G39)*(1-I44)*D39</f>
         <v>1</v>
       </c>
       <c r="C39">
@@ -2688,11 +2688,11 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>0.15407604627335114</v>
+        <v>0.69388431646844406</v>
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26535887622413257</v>
+        <v>1.1912546135353308E-2</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2700,8 +2700,8 @@
         <v>108</v>
       </c>
       <c r="B40">
-        <f>PARS!B40</f>
-        <v>1.8427</v>
+        <f>PARS!B40*I45+G40*(1-I45)*C40+(1-G40)*(1-I45)*D40</f>
+        <v>1.8426999999999998</v>
       </c>
       <c r="C40">
         <f>PARS!C40</f>
@@ -2719,11 +2719,11 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>4.4062957175660222E-2</v>
+        <v>0.92087990789729779</v>
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46666659594498661</v>
+        <v>0.14733529846745719</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2731,7 +2731,7 @@
         <v>109</v>
       </c>
       <c r="B41">
-        <f>PARS!B41</f>
+        <f>PARS!B41*I46+G41*(1-I46)*C41+(1-G41)*(1-I46)*D41</f>
         <v>9.7252000000000005E-2</v>
       </c>
       <c r="C41">
@@ -2750,11 +2750,11 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0.40461846550790204</v>
+        <v>0.53038216876950151</v>
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70568223307609879</v>
+        <v>0.91991056429005635</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2762,7 +2762,7 @@
         <v>105</v>
       </c>
       <c r="B42">
-        <f>PARS!B42</f>
+        <f>PARS!B42*I47+G42*(1-I47)*C42+(1-G42)*(1-I47)*D42</f>
         <v>0.26712328767123289</v>
       </c>
       <c r="C42">
@@ -2781,11 +2781,11 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>0.10301469808812802</v>
+        <v>0.8674399980394436</v>
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13952744770783054</v>
+        <v>0.97147493793039075</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2793,7 +2793,7 @@
         <v>110</v>
       </c>
       <c r="B43">
-        <f>PARS!B43</f>
+        <f>PARS!B43*I48+G43*(1-I48)*C43+(1-G43)*(1-I48)*D43</f>
         <v>1</v>
       </c>
       <c r="C43">
@@ -2812,11 +2812,11 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0.75477678349395205</v>
+        <v>0.37699529950601773</v>
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60497053073490892</v>
+        <v>0.80147262074933501</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -2824,7 +2824,7 @@
         <v>90</v>
       </c>
       <c r="B44">
-        <f>PARS!B44</f>
+        <f>PARS!B44*I49+G44*(1-I49)*C44+(1-G44)*(1-I49)*D44</f>
         <v>0.1449</v>
       </c>
       <c r="C44">
@@ -2843,11 +2843,11 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>0.57929408336024069</v>
+        <v>0.61091316560209341</v>
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67185211824554525</v>
+        <v>0.2570437406393018</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2855,7 +2855,7 @@
         <v>91</v>
       </c>
       <c r="B45">
-        <f>PARS!B45</f>
+        <f>PARS!B45*I50+G45*(1-I50)*C45+(1-G45)*(1-I50)*D45</f>
         <v>0.1449</v>
       </c>
       <c r="C45">
@@ -2874,11 +2874,11 @@
         <v>0</v>
       </c>
       <c r="G45">
-        <v>0.33746607981681664</v>
+        <v>0.84998186215767646</v>
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17060767295411627</v>
+        <v>1.2039774797237168E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2886,7 +2886,7 @@
         <v>101</v>
       </c>
       <c r="B46">
-        <f>PARS!B46</f>
+        <f>PARS!B46*I51+G46*(1-I51)*C46+(1-G46)*(1-I51)*D46</f>
         <v>0</v>
       </c>
       <c r="C46">
@@ -2905,11 +2905,11 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0.87650119447756558</v>
+        <v>0.42422420400635719</v>
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28201062209178351</v>
+        <v>0.54840561586591285</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2917,7 +2917,7 @@
         <v>104</v>
       </c>
       <c r="B47">
-        <f>PARS!B47</f>
+        <f>PARS!B47*I52+G47*(1-I52)*C47+(1-G47)*(1-I52)*D47</f>
         <v>0</v>
       </c>
       <c r="C47">
@@ -2936,11 +2936,11 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>0.69279532686013079</v>
+        <v>0.94681852179508197</v>
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75767706396670953</v>
+        <v>0.9297811356742498</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -2948,7 +2948,7 @@
         <v>248</v>
       </c>
       <c r="B48">
-        <f>PARS!B48</f>
+        <f>PARS!B48*I53+G48*(1-I53)*C48+(1-G48)*(1-I53)*D48</f>
         <v>3.7</v>
       </c>
       <c r="C48">
@@ -2964,11 +2964,11 @@
         <v>1</v>
       </c>
       <c r="G48">
-        <v>0.23069947484160258</v>
+        <v>0.82466078800789866</v>
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90849038363052559</v>
+        <v>0.56304067754668652</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2976,8 +2976,8 @@
         <v>250</v>
       </c>
       <c r="B49">
-        <f>PARS!B49</f>
-        <v>0</v>
+        <f>PARS!B49*I54+G49*(1-I54)*C49+(1-G49)*(1-I54)*D49</f>
+        <v>1</v>
       </c>
       <c r="C49">
         <f>PARS!C49</f>
@@ -2989,17 +2989,17 @@
       </c>
       <c r="E49" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
-        <v>0.17321706713356355</v>
+        <v>0.80163096341272844</v>
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18176718335776854</v>
+        <v>0.86950778421927988</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3007,7 +3007,7 @@
         <v>179</v>
       </c>
       <c r="B50">
-        <f>PARS!B50</f>
+        <f>PARS!B50*I55+G50*(1-I55)*C50+(1-G50)*(1-I55)*D50</f>
         <v>1.0696163149411613</v>
       </c>
       <c r="C50">
@@ -3026,11 +3026,11 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>0.63005364527001628</v>
+        <v>0.44932021180770876</v>
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41096975970795058</v>
+        <v>0.84103517626254098</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -3038,8 +3038,8 @@
         <v>180</v>
       </c>
       <c r="B51">
-        <f>PARS!B51</f>
-        <v>0.99381918034015848</v>
+        <f>PARS!B51*I56+G51*(1-I56)*C51+(1-G51)*(1-I56)*D51</f>
+        <v>0.99381918034015859</v>
       </c>
       <c r="C51">
         <f>PARS!C51</f>
@@ -3051,17 +3051,17 @@
       </c>
       <c r="E51" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
-        <v>1.9939515190257939E-2</v>
+        <v>0.52304265856788512</v>
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62984887099733655</v>
+        <v>0.5764932732366026</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -3069,7 +3069,7 @@
         <v>181</v>
       </c>
       <c r="B52">
-        <f>PARS!B52</f>
+        <f>PARS!B52*I57+G52*(1-I57)*C52+(1-G52)*(1-I57)*D52</f>
         <v>0.9618468890261952</v>
       </c>
       <c r="C52">
@@ -3088,11 +3088,11 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>0.60847962300181635</v>
+        <v>0.85636524482008336</v>
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1022556845341378</v>
+        <v>0.82916213180918619</v>
       </c>
     </row>
   </sheetData>
@@ -31328,7 +31328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641FA06B-861E-4739-90D9-A8300FC4235B}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New ganoL with corrected weighted matrix
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{8E1D693F-55B9-4CDA-964D-425A41E85608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09473A77-1C8E-455A-B089-8E50DD2904FB}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4511CC9E-EE0F-4A90-A3F0-8CE8B279B3BD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="360" yWindow="170" windowWidth="18840" windowHeight="10630" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MOMS!$A$1:$J$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PARS!$A$1:$W$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PARS!$A$1:$X$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">PARS4!$A$1:$V$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">W_psid!$A$1:$CT$98</definedName>
   </definedNames>
@@ -74,7 +74,7 @@
     made it so it would take singles into account</t>
       </text>
     </comment>
-    <comment ref="U39" authorId="1" shapeId="0" xr:uid="{3A5A5ACA-AB2A-48F2-965E-C0F7F32044A5}">
+    <comment ref="V39" authorId="1" shapeId="0" xr:uid="{3A5A5ACA-AB2A-48F2-965E-C0F7F32044A5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -82,7 +82,7 @@
     add later - and get rid of THETA?</t>
       </text>
     </comment>
-    <comment ref="U41" authorId="2" shapeId="0" xr:uid="{B0A55D4B-53D8-43EF-BA32-9BB09124DD6C}">
+    <comment ref="V41" authorId="2" shapeId="0" xr:uid="{B0A55D4B-53D8-43EF-BA32-9BB09124DD6C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="261">
   <si>
     <t>label</t>
   </si>
@@ -991,6 +991,9 @@
   <si>
     <t>not lm! (to make this low)</t>
   </si>
+  <si>
+    <t>toestimate_f0</t>
+  </si>
 </sst>
 </file>
 
@@ -1482,10 +1485,10 @@
   <threadedComment ref="E2" dT="2022-07-12T00:27:50.56" personId="{8C1B3605-3BBC-4A56-9DEA-CD9622C706EB}" id="{9781E3DA-46F9-48AE-84BE-37948A9B465D}" parentId="{767204F0-6A68-45A9-81A4-37CA98FC0DF2}">
     <text>made it so it would take singles into account</text>
   </threadedComment>
-  <threadedComment ref="U39" dT="2022-07-11T22:02:30.08" personId="{8C1B3605-3BBC-4A56-9DEA-CD9622C706EB}" id="{3A5A5ACA-AB2A-48F2-965E-C0F7F32044A5}">
+  <threadedComment ref="V39" dT="2022-07-11T22:02:30.08" personId="{8C1B3605-3BBC-4A56-9DEA-CD9622C706EB}" id="{3A5A5ACA-AB2A-48F2-965E-C0F7F32044A5}">
     <text>add later - and get rid of THETA?</text>
   </threadedComment>
-  <threadedComment ref="U41" dT="2022-07-11T19:37:37.39" personId="{8C1B3605-3BBC-4A56-9DEA-CD9622C706EB}" id="{B0A55D4B-53D8-43EF-BA32-9BB09124DD6C}">
+  <threadedComment ref="V41" dT="2022-07-11T19:37:37.39" personId="{8C1B3605-3BBC-4A56-9DEA-CD9622C706EB}" id="{B0A55D4B-53D8-43EF-BA32-9BB09124DD6C}">
     <text>cannot do comparative statics both for THETAHW and for LAMBDA</text>
   </threadedComment>
 </ThreadedComments>
@@ -1533,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1592,7 +1595,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <f>VLOOKUP(A2,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A2,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G2">
@@ -1600,7 +1603,7 @@
       </c>
       <c r="H2">
         <f ca="1">RAND()</f>
-        <v>0.77823757152642858</v>
+        <v>0.55583892110935273</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1624,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <f>VLOOKUP(A3,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A3,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G3">
@@ -1632,7 +1635,7 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H52" ca="1" si="1">RAND()</f>
-        <v>0.89255924756335547</v>
+        <v>0.613721504526624</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1656,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <f>VLOOKUP(A4,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A4,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G4">
@@ -1664,7 +1667,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32640614922115596</v>
+        <v>0.97003780190230682</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1688,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f>VLOOKUP(A5,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A5,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G5">
@@ -1696,7 +1699,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90569437178323986</v>
+        <v>0.40826131370580154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1720,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <f>VLOOKUP(A6,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A6,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G6">
@@ -1728,7 +1731,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66443398394971209</v>
+        <v>0.55181999678455629</v>
       </c>
       <c r="I6" t="s">
         <v>251</v>
@@ -1755,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <f>VLOOKUP(A7,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A7,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G7">
@@ -1763,7 +1766,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12564830123582438</v>
+        <v>0.60020283720784662</v>
       </c>
       <c r="I7">
         <v>0.8</v>
@@ -1775,7 +1778,7 @@
       </c>
       <c r="B8">
         <f>PARS!B8*$I$7+G8*(1-$I$7)*C8+(1-G8)*(1-$I$7)*D8</f>
-        <v>-1.401190425660328</v>
+        <v>-1.4948005192997922</v>
       </c>
       <c r="C8">
         <f>PARS!C8</f>
@@ -1790,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <f>VLOOKUP(A8,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A8,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G8">
@@ -1798,7 +1801,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31333191371261326</v>
+        <v>2.0106585163421786E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1807,7 +1810,7 @@
       </c>
       <c r="B9">
         <f>PARS!B9*$I$7+G9*(1-$I$7)*C9+(1-G9)*(1-$I$7)*D9</f>
-        <v>6.6382134221918507E-2</v>
+        <v>0.1212158258075465</v>
       </c>
       <c r="C9">
         <f>PARS!C9</f>
@@ -1822,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <f>VLOOKUP(A9,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A9,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G9">
@@ -1830,7 +1833,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0219009598231983E-2</v>
+        <v>0.42090064538781624</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1839,7 +1842,7 @@
       </c>
       <c r="B10">
         <f>PARS!B10*$I$7+G10*(1-$I$7)*C10+(1-G10)*(1-$I$7)*D10</f>
-        <v>1.6386021329014464</v>
+        <v>1.7102214511459264</v>
       </c>
       <c r="C10">
         <f>PARS!C10</f>
@@ -1854,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f>VLOOKUP(A10,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A10,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G10">
@@ -1862,7 +1865,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20578567848864404</v>
+        <v>0.49819393450569605</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1886,7 +1889,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <f>VLOOKUP(A11,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A11,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G11">
@@ -1894,7 +1897,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58344595487903261</v>
+        <v>0.66162876020424544</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1918,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <f>VLOOKUP(A12,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A12,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G12">
@@ -1926,7 +1929,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26460192904776847</v>
+        <v>0.33517648795428445</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1950,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <f>VLOOKUP(A13,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A13,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G13">
@@ -1958,7 +1961,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3087814571983656E-2</v>
+        <v>0.5607246590582412</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1982,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <f>VLOOKUP(A14,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A14,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G14">
@@ -1990,7 +1993,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51423567856763674</v>
+        <v>0.60830915114567319</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2014,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f>VLOOKUP(A15,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A15,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G15">
@@ -2022,7 +2025,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.975229589659795</v>
+        <v>0.71750793736182328</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -2046,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <f>VLOOKUP(A16,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A16,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G16">
@@ -2054,7 +2057,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9691248170395339</v>
+        <v>0.20413490902279596</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -2063,7 +2066,7 @@
       </c>
       <c r="B17">
         <f>PARS!B17*$I$7+G17*(1-$I$7)*C17+(1-G17)*(1-$I$7)*D17</f>
-        <v>-1.4561618939362773</v>
+        <v>-1.4282114229925733</v>
       </c>
       <c r="C17">
         <f>PARS!C17</f>
@@ -2078,7 +2081,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <f>VLOOKUP(A17,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A17,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G17">
@@ -2086,7 +2089,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0249469061353533E-2</v>
+        <v>0.86220846249904581</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2095,7 +2098,7 @@
       </c>
       <c r="B18">
         <f>PARS!B18*$I$7+G18*(1-$I$7)*C18+(1-G18)*(1-$I$7)*D18</f>
-        <v>-0.67451752364064388</v>
+        <v>-0.5945175236406437</v>
       </c>
       <c r="C18">
         <f>PARS!C18</f>
@@ -2110,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <f>VLOOKUP(A18,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A18,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G18">
@@ -2118,7 +2121,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18029385246769802</v>
+        <v>0.54078392900953498</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2127,11 +2130,10 @@
       </c>
       <c r="B19">
         <f>PARS!B19*$I$7+G19*(1-$I$7)*C19+(1-G19)*(1-$I$7)*D19</f>
-        <v>1.1736377928400263</v>
+        <v>0.7226831257694355</v>
       </c>
       <c r="C19">
-        <f>PARS!C19</f>
-        <v>1.6094379124341003</v>
+        <v>0.5</v>
       </c>
       <c r="D19">
         <f>PARS!D19</f>
@@ -2139,10 +2141,10 @@
       </c>
       <c r="E19" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <f>VLOOKUP(A19,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A19,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G19">
@@ -2150,7 +2152,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92296727438006732</v>
+        <v>0.35582526975645279</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -2174,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f>VLOOKUP(A20,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A20,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G20">
@@ -2182,7 +2184,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68143096357106681</v>
+        <v>0.33687571353373091</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2206,7 +2208,7 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <f>VLOOKUP(A21,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A21,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G21">
@@ -2214,7 +2216,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0998004386387916E-2</v>
+        <v>0.25887364928219825</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2223,7 +2225,7 @@
       </c>
       <c r="B22">
         <f>PARS!B22*$I$7+G22*(1-$I$7)*C22+(1-G22)*(1-$I$7)*D22</f>
-        <v>0.86938991810770416</v>
+        <v>0.8797865166500809</v>
       </c>
       <c r="C22">
         <f>PARS!C22</f>
@@ -2238,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <f>VLOOKUP(A22,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A22,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G22">
@@ -2246,7 +2248,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93524208229850492</v>
+        <v>0.25925728396013525</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2255,7 +2257,7 @@
       </c>
       <c r="B23">
         <f>PARS!B23*$I$7+G23*(1-$I$7)*C23+(1-G23)*(1-$I$7)*D23</f>
-        <v>3.6579863873705185</v>
+        <v>3.8005269731811664</v>
       </c>
       <c r="C23">
         <f>PARS!C23</f>
@@ -2270,7 +2272,7 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <f>VLOOKUP(A23,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A23,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G23">
@@ -2278,7 +2280,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7640808458894901</v>
+        <v>0.74325930424435227</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2302,7 +2304,7 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <f>VLOOKUP(A24,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A24,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G24">
@@ -2310,7 +2312,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.381765510623857</v>
+        <v>0.54938230394392329</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2319,7 +2321,7 @@
       </c>
       <c r="B25">
         <f>PARS!B25*$I$7+G25*(1-$I$7)*C25+(1-G25)*(1-$I$7)*D25</f>
-        <v>-0.15931202969077907</v>
+        <v>-0.17675574497763347</v>
       </c>
       <c r="C25">
         <f>PARS!C25</f>
@@ -2334,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <f>VLOOKUP(A25,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A25,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G25">
@@ -2342,7 +2344,7 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7078049601407167</v>
+        <v>0.54682715673600113</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2351,7 +2353,7 @@
       </c>
       <c r="B26">
         <f>PARS!B26*$I$7+G26*(1-$I$7)*C26+(1-G26)*(1-$I$7)*D26</f>
-        <v>0.21896831729867083</v>
+        <v>0.20015397174377164</v>
       </c>
       <c r="C26">
         <f>PARS!C26</f>
@@ -2366,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <f>VLOOKUP(A26,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A26,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G26">
@@ -2374,7 +2376,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5375451831628143</v>
+        <v>0.97294313605527405</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2383,7 +2385,7 @@
       </c>
       <c r="B27">
         <f>PARS!B27*$I$7+G27*(1-$I$7)*C27+(1-G27)*(1-$I$7)*D27</f>
-        <v>-0.55559558737545989</v>
+        <v>-0.59609014802157589</v>
       </c>
       <c r="C27">
         <f>PARS!C27</f>
@@ -2398,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <f>VLOOKUP(A27,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A27,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G27">
@@ -2406,7 +2408,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82842094984287395</v>
+        <v>0.6382407231668501</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2430,7 +2432,7 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <f>VLOOKUP(A28,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A28,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G28">
@@ -2438,7 +2440,7 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>7.468454749154807E-2</v>
+        <v>0.21290805096384124</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2447,7 +2449,7 @@
       </c>
       <c r="B29">
         <f>PARS!B29*$I$7+G29*(1-$I$7)*C29+(1-G29)*(1-$I$7)*D29</f>
-        <v>5.556483654368484E-2</v>
+        <v>5.5334121914402443E-2</v>
       </c>
       <c r="C29">
         <f>PARS!C29</f>
@@ -2462,15 +2464,15 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <f>VLOOKUP(A29,PARS!A:V,19,0)</f>
-        <v>1</v>
+        <f>VLOOKUP(A29,PARS!A:W,19,0)</f>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>7.7764634759959095E-2</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60366554880974854</v>
+        <v>0.88011528482836943</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2479,7 +2481,7 @@
       </c>
       <c r="B30">
         <f>PARS!B30*$I$7+G30*(1-$I$7)*C30+(1-G30)*(1-$I$7)*D30</f>
-        <v>1.1837772984036552</v>
+        <v>1.0413385269725801</v>
       </c>
       <c r="C30">
         <f>PARS!C30</f>
@@ -2494,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <f>VLOOKUP(A30,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A30,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G30">
@@ -2502,7 +2504,7 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18184163677824328</v>
+        <v>0.76941134176680781</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2511,7 +2513,7 @@
       </c>
       <c r="B31">
         <f>PARS!B31*$I$7+G31*(1-$I$7)*C31+(1-G31)*(1-$I$7)*D31</f>
-        <v>1.6122398839666197</v>
+        <v>1.7053177908908357</v>
       </c>
       <c r="C31">
         <f>PARS!C31</f>
@@ -2526,7 +2528,7 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <f>VLOOKUP(A31,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A31,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G31">
@@ -2534,7 +2536,7 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47398407691226385</v>
+        <v>0.58126139007785482</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2543,7 +2545,7 @@
       </c>
       <c r="B32">
         <f>PARS!B32*$I$7+G32*(1-$I$7)*C32+(1-G32)*(1-$I$7)*D32</f>
-        <v>1.7887482642195227</v>
+        <v>1.7553061879773808</v>
       </c>
       <c r="C32">
         <f>PARS!C32</f>
@@ -2558,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <f>VLOOKUP(A32,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A32,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G32">
@@ -2566,7 +2568,7 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81742669051888162</v>
+        <v>0.21284615189456757</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -2590,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <f>VLOOKUP(A33,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A33,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G33">
@@ -2598,7 +2600,7 @@
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9824374076152611</v>
+        <v>0.64302820329507226</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2607,7 +2609,7 @@
       </c>
       <c r="B34">
         <f>PARS!B34*$I$7+G34*(1-$I$7)*C34+(1-G34)*(1-$I$7)*D34</f>
-        <v>0.54571694859998998</v>
+        <v>0.24554618404635642</v>
       </c>
       <c r="C34">
         <f>PARS!C34</f>
@@ -2622,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <f>VLOOKUP(A34,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A34,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G34">
@@ -2630,7 +2632,7 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.15819508935976156</v>
+        <v>0.68008447701062069</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2639,7 +2641,7 @@
       </c>
       <c r="B35">
         <f>PARS!B35*$I$7+G35*(1-$I$7)*C35+(1-G35)*(1-$I$7)*D35</f>
-        <v>-0.21978943997261768</v>
+        <v>-0.29490912779217848</v>
       </c>
       <c r="C35">
         <f>PARS!C35</f>
@@ -2654,7 +2656,7 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <f>VLOOKUP(A35,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A35,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G35">
@@ -2662,7 +2664,7 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4961820480345156E-2</v>
+        <v>7.1576207725898344E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2671,7 +2673,7 @@
       </c>
       <c r="B36">
         <f>PARS!B36*$I$7+G36*(1-$I$7)*C36+(1-G36)*(1-$I$7)*D36</f>
-        <v>2.4335414193138298</v>
+        <v>2.6098798760009898</v>
       </c>
       <c r="C36">
         <f>PARS!C36</f>
@@ -2686,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <f>VLOOKUP(A36,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A36,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G36">
@@ -2694,7 +2696,7 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>3.658440476055147E-2</v>
+        <v>0.23276028416288019</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2718,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <f>VLOOKUP(A37,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A37,PARS!A:W,19,0)</f>
         <v>1</v>
       </c>
       <c r="G37">
@@ -2726,7 +2728,7 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88145618897918676</v>
+        <v>4.1810603541957869E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2750,7 +2752,7 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <f>VLOOKUP(A38,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A38,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G38">
@@ -2758,7 +2760,7 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62953968600213739</v>
+        <v>0.76510836974831808</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2767,22 +2769,22 @@
       </c>
       <c r="B39">
         <f>PARS!B39*$I$7+G39*(1-$I$7)*C39+(1-G39)*(1-$I$7)*D39</f>
-        <v>1</v>
+        <v>0.81406601627977282</v>
       </c>
       <c r="C39">
         <f>PARS!C39</f>
-        <v>1</v>
+        <v>0.81406601627977282</v>
       </c>
       <c r="D39">
         <f>PARS!D39</f>
-        <v>1</v>
+        <v>0.81406601627977282</v>
       </c>
       <c r="E39" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F39">
-        <f>VLOOKUP(A39,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A39,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G39">
@@ -2790,7 +2792,7 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39090344333252858</v>
+        <v>0.89652139977119438</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2814,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <f>VLOOKUP(A40,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A40,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G40">
@@ -2822,7 +2824,7 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63170855211959798</v>
+        <v>0.28282931700497393</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2846,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <f>VLOOKUP(A41,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A41,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G41">
@@ -2854,7 +2856,7 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>5.6685729641565819E-2</v>
+        <v>1.6745390078401368E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -2878,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <f>VLOOKUP(A42,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A42,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G42">
@@ -2886,7 +2888,7 @@
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87873272952011583</v>
+        <v>0.48706200299391922</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2910,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <f>VLOOKUP(A43,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A43,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G43">
@@ -2918,7 +2920,7 @@
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3689956610004117</v>
+        <v>0.95708236695961202</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -2942,7 +2944,7 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <f>VLOOKUP(A44,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A44,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G44">
@@ -2950,7 +2952,7 @@
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59909638600060489</v>
+        <v>0.72081605566067242</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2974,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <f>VLOOKUP(A45,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A45,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G45">
@@ -2982,7 +2984,7 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27065778273768482</v>
+        <v>3.0610049063742095E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -3006,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <f>VLOOKUP(A46,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A46,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G46">
@@ -3014,7 +3016,7 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="1"/>
-        <v>3.039882752133849E-4</v>
+        <v>0.9721336094441031</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -3038,7 +3040,7 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <f>VLOOKUP(A47,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A47,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G47">
@@ -3046,7 +3048,7 @@
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3041320089324614</v>
+        <v>0.61301727078443213</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -3070,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <f>VLOOKUP(A48,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A48,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G48">
@@ -3078,7 +3080,7 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45306592192085282</v>
+        <v>0.52037175187136664</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -3102,7 +3104,7 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <f>VLOOKUP(A49,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A49,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G49">
@@ -3110,7 +3112,7 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51270566691111985</v>
+        <v>8.7309692326145827E-2</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3134,7 +3136,7 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <f>VLOOKUP(A50,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A50,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G50">
@@ -3142,7 +3144,7 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39115572012685296</v>
+        <v>0.52116232170684884</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -3166,7 +3168,7 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <f>VLOOKUP(A51,PARS!A:V,19,0)</f>
+        <f>VLOOKUP(A51,PARS!A:W,19,0)</f>
         <v>0</v>
       </c>
       <c r="G51">
@@ -3174,7 +3176,7 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55604886878839088</v>
+        <v>0.27578624635234195</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -3205,7 +3207,7 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85371180129035329</v>
+        <v>0.26442581424135247</v>
       </c>
     </row>
   </sheetData>
@@ -33323,10 +33325,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Z55"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33334,12 +33339,12 @@
     <col min="2" max="4" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.453125" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.54296875" customWidth="1"/>
-    <col min="25" max="25" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.54296875" customWidth="1"/>
+    <col min="26" max="26" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>62</v>
       </c>
@@ -33398,19 +33403,22 @@
         <v>176</v>
       </c>
       <c r="T1" t="s">
+        <v>260</v>
+      </c>
+      <c r="U1" t="s">
         <v>188</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>211</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>191</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -33459,15 +33467,18 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T52" si="2">S2+N2+Q2+M2</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ref="U2:U52" si="2">S2+N2+Q2+M2</f>
         <v>1</v>
       </c>
-      <c r="U2">
-        <f>T2-N2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+      <c r="V2">
+        <f>U2-N2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -33513,15 +33524,18 @@
         <v>0</v>
       </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U3">
-        <f>T3-N3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+      <c r="V3">
+        <f>U3-N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -33537,7 +33551,7 @@
         <v>0.18232155679395459</v>
       </c>
       <c r="E4" s="16">
-        <f>V4</f>
+        <f>W4</f>
         <v>0.70468808971871344</v>
       </c>
       <c r="F4">
@@ -33571,19 +33585,22 @@
         <v>0</v>
       </c>
       <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U4">
-        <f>T4-N4</f>
+      <c r="V4">
+        <f>U4-N4</f>
         <v>1</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <f>EXP(B4)</f>
         <v>0.70468808971871344</v>
       </c>
     </row>
-    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -33630,15 +33647,18 @@
         <v>0</v>
       </c>
       <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U5">
-        <f>T5-N5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+      <c r="V5">
+        <f>U5-N5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -33684,15 +33704,18 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6" si="5">S6+N6+Q6+M6</f>
         <v>0</v>
       </c>
       <c r="U6">
-        <f>T6-N6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+        <f t="shared" ref="U6" si="5">S6+N6+Q6+M6</f>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f>U6-N6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -33739,19 +33762,22 @@
         <v>0</v>
       </c>
       <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U7" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>73</v>
       </c>
       <c r="B8">
-        <v>-1.48055622303644</v>
+        <v>-1.5975688400857699</v>
       </c>
       <c r="C8">
         <f t="shared" ref="C8:D10" si="6">LN(F8)</f>
@@ -33762,8 +33788,8 @@
         <v>-1.0498221244986778</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" ref="E8:E10" si="7">V8</f>
-        <v>0.22751110626478058</v>
+        <f t="shared" ref="E8:E10" si="7">W8</f>
+        <v>0.20238795785841901</v>
       </c>
       <c r="F8">
         <v>0.2</v>
@@ -33779,7 +33805,7 @@
       </c>
       <c r="J8">
         <f>1/E8</f>
-        <v>4.3953898181840234</v>
+        <v>4.9410054362006681</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -33796,24 +33822,27 @@
         <v>1</v>
       </c>
       <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U8">
-        <f t="shared" ref="U8:U40" si="8">T8-N8</f>
+      <c r="V8">
+        <f t="shared" ref="V8:V40" si="8">U8-N8</f>
         <v>1</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <f>EXP(B8)</f>
-        <v>0.22751110626478058</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+        <v>0.20238795785841901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>91</v>
       </c>
       <c r="B9">
-        <v>0.100986933924772</v>
+        <v>0.16952904840680699</v>
       </c>
       <c r="C9">
         <f t="shared" si="6"/>
@@ -33825,7 +33854,7 @@
       </c>
       <c r="E9" s="16">
         <f t="shared" si="7"/>
-        <v>1.1062621871640319</v>
+        <v>1.1847467615391678</v>
       </c>
       <c r="F9">
         <v>0.85</v>
@@ -33841,7 +33870,7 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9:J22" si="9">1/E9</f>
-        <v>0.90394484382003393</v>
+        <v>0.84406223546105885</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -33858,24 +33887,27 @@
         <v>1</v>
       </c>
       <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <f>EXP(B9)</f>
-        <v>1.1062621871640319</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+        <v>1.1847467615391678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>92</v>
       </c>
       <c r="B10">
-        <v>1.55520658335772</v>
+        <v>1.6447307311633199</v>
       </c>
       <c r="C10">
         <f t="shared" si="6"/>
@@ -33887,7 +33919,7 @@
       </c>
       <c r="E10" s="16">
         <f t="shared" si="7"/>
-        <v>4.7360648162787387</v>
+        <v>5.1796150102475682</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -33903,7 +33935,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="9"/>
-        <v>0.21114575893531132</v>
+        <v>0.19306454205989401</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -33920,19 +33952,22 @@
         <v>1</v>
       </c>
       <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <f>EXP(B10)</f>
-        <v>4.7360648162787387</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+        <v>5.1796150102475682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -33949,7 +33984,7 @@
       </c>
       <c r="E11" s="16">
         <f>E9</f>
-        <v>1.1062621871640319</v>
+        <v>1.1847467615391678</v>
       </c>
       <c r="F11">
         <f>F4</f>
@@ -33967,7 +34002,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="9"/>
-        <v>0.90394484382003393</v>
+        <v>0.84406223546105885</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -33981,15 +34016,18 @@
         <v>0</v>
       </c>
       <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -34043,19 +34081,22 @@
         <v>0</v>
       </c>
       <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <f>EXP(B12)</f>
         <v>0.15407408</v>
       </c>
     </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -34107,19 +34148,22 @@
         <v>0</v>
       </c>
       <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <f>1/(1+EXP(-B13))</f>
         <v>0.66013195000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -34171,15 +34215,18 @@
         <v>0</v>
       </c>
       <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -34231,15 +34278,18 @@
         <v>0</v>
       </c>
       <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -34291,24 +34341,27 @@
         <v>0</v>
       </c>
       <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <f>EXP(B16)</f>
         <v>9.4106369999999981E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>76</v>
       </c>
       <c r="B17">
-        <v>-1.44797876639686</v>
+        <v>-1.41304067771723</v>
       </c>
       <c r="C17">
         <f>LN(-G17)</f>
@@ -34319,8 +34372,8 @@
         <v>-1.3093333199837622</v>
       </c>
       <c r="E17" s="16">
-        <f t="shared" ref="E17:E19" si="10">V17</f>
-        <v>-0.23504488892038319</v>
+        <f t="shared" ref="E17:E19" si="10">W17</f>
+        <v>-0.24340204960980388</v>
       </c>
       <c r="F17">
         <v>-0.27</v>
@@ -34336,7 +34389,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="9"/>
-        <v>-4.2545064672252044</v>
+        <v>-4.1084288386358825</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -34353,24 +34406,27 @@
         <v>1</v>
       </c>
       <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <f>-EXP(B17)</f>
-        <v>-0.23504488892038319</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+        <v>-0.24340204960980388</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>95</v>
       </c>
       <c r="B18">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="C18">
         <f t="shared" ref="C18:D19" si="11">LN(F18)</f>
@@ -34382,7 +34438,7 @@
       </c>
       <c r="E18" s="16">
         <f t="shared" si="10"/>
-        <v>0.44932896411722156</v>
+        <v>0.49658530379140953</v>
       </c>
       <c r="F18">
         <v>0.3</v>
@@ -34398,7 +34454,7 @@
       </c>
       <c r="J18">
         <f t="shared" si="9"/>
-        <v>2.2255409284924679</v>
+        <v>2.0137527074704766</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -34415,24 +34471,27 @@
         <v>1</v>
       </c>
       <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <f>EXP(B18)</f>
-        <v>0.44932896411722156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+        <v>0.49658530379140953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>70</v>
       </c>
       <c r="B19">
-        <v>1.0216023722149501</v>
+        <v>0.67</v>
       </c>
       <c r="C19">
         <f t="shared" si="11"/>
@@ -34444,7 +34503,7 @@
       </c>
       <c r="E19" s="16">
         <f t="shared" si="10"/>
-        <v>2.7776420163259656</v>
+        <v>1.9542373206359396</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -34460,7 +34519,7 @@
       </c>
       <c r="J19">
         <f t="shared" si="9"/>
-        <v>0.36001759554412166</v>
+        <v>0.51170857778654244</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -34477,19 +34536,22 @@
         <v>1</v>
       </c>
       <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <f>EXP(B19)</f>
-        <v>2.7776420163259656</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+        <v>1.9542373206359396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>71</v>
       </c>
@@ -34541,15 +34603,18 @@
         <v>0</v>
       </c>
       <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -34565,7 +34630,7 @@
         <v>2.0067069546215124</v>
       </c>
       <c r="E21" s="16">
-        <f>V21</f>
+        <f>W21</f>
         <v>0.50899902812595466</v>
       </c>
       <c r="F21">
@@ -34599,28 +34664,31 @@
         <v>1</v>
       </c>
       <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V21" s="21">
+      <c r="W21" s="21">
         <f>1/(1+EXP(-B21/10))</f>
         <v>0.50899902812595466</v>
       </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
         <v>240</v>
       </c>
-      <c r="Z21" s="15"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA21" s="15"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>67</v>
       </c>
       <c r="B22">
-        <v>0.88400425182202902</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="C22">
         <v>0.7</v>
@@ -34629,8 +34697,8 @@
         <v>1.3</v>
       </c>
       <c r="E22" s="16">
-        <f t="shared" ref="E22:E23" si="12">V22</f>
-        <v>24.205729100058726</v>
+        <f t="shared" ref="E22:E23" si="12">W22</f>
+        <v>24.522353589775612</v>
       </c>
       <c r="F22">
         <v>14.5</v>
@@ -34646,7 +34714,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="9"/>
-        <v>4.1312533733907399E-2</v>
+        <v>4.0779120011422622E-2</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -34663,24 +34731,27 @@
         <v>1</v>
       </c>
       <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <f>EXP(B22)*10</f>
-        <v>24.205729100058726</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+        <v>24.522353589775612</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>78</v>
       </c>
       <c r="B23">
-        <v>3.82182426773669</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <f>1-LN(1/(F23-1) -1)</f>
@@ -34692,7 +34763,7 @@
       </c>
       <c r="E23" s="16">
         <f t="shared" si="12"/>
-        <v>1.9438438357765078</v>
+        <v>1.9525741268224333</v>
       </c>
       <c r="F23">
         <v>1.5</v>
@@ -34708,7 +34779,7 @@
       </c>
       <c r="J23">
         <f>1/((2-E23)*(E23-1))</f>
-        <v>18.866981377444393</v>
+        <v>22.135323991555545</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -34722,19 +34793,22 @@
         <v>1</v>
       </c>
       <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <f>1+1/(1+EXP(-(B23-1)))</f>
-        <v>1.9438438357765078</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+        <v>1.9525741268224333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -34778,20 +34852,23 @@
         <v>0</v>
       </c>
       <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>189</v>
       </c>
       <c r="B25">
-        <v>-0.138195355891432</v>
+        <v>-0.16</v>
       </c>
       <c r="C25">
         <f t="shared" ref="C25:D26" si="13">F25</f>
@@ -34802,8 +34879,8 @@
         <v>0.05</v>
       </c>
       <c r="E25" s="16">
-        <f t="shared" ref="E25:E27" si="14">V25</f>
-        <v>-0.138195355891432</v>
+        <f t="shared" ref="E25:E27" si="14">W25</f>
+        <v>-0.16</v>
       </c>
       <c r="F25">
         <f>-0.35</f>
@@ -34834,24 +34911,27 @@
         <v>1</v>
       </c>
       <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <f>B25</f>
-        <v>-0.138195355891432</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+        <v>-0.16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>80</v>
       </c>
       <c r="B26">
-        <v>0.18027520148399201</v>
+        <v>0.156757269540368</v>
       </c>
       <c r="C26">
         <f t="shared" si="13"/>
@@ -34863,7 +34943,7 @@
       </c>
       <c r="E26" s="16">
         <f t="shared" si="14"/>
-        <v>0.18027520148399201</v>
+        <v>0.156757269540368</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -34893,24 +34973,27 @@
         <v>1</v>
       </c>
       <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <f>B26</f>
-        <v>0.18027520148399201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+        <v>0.156757269540368</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>81</v>
       </c>
       <c r="B27">
-        <v>-0.84824279493960997</v>
+        <v>-0.89886099574725498</v>
       </c>
       <c r="C27">
         <f>LN(F27)</f>
@@ -34922,7 +35005,7 @@
       </c>
       <c r="E27" s="16">
         <f t="shared" si="14"/>
-        <v>0.42816664789613951</v>
+        <v>0.40703300813988641</v>
       </c>
       <c r="F27">
         <v>0.3</v>
@@ -34938,7 +35021,7 @@
       </c>
       <c r="J27">
         <f t="shared" ref="J27" si="15">1/E27</f>
-        <v>2.3355392226686704</v>
+        <v>2.4568032076070021</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -34955,19 +35038,22 @@
         <v>1</v>
       </c>
       <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <f>EXP(B27)</f>
-        <v>0.42816664789613951</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.40703300813988641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -35011,20 +35097,23 @@
         <v>0</v>
       </c>
       <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>102</v>
       </c>
       <c r="B29">
-        <v>2.8839328660299997E-4</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <f>F29</f>
@@ -35035,8 +35124,8 @@
         <v>0.3</v>
       </c>
       <c r="E29" s="16">
-        <f t="shared" ref="E29:E32" si="16">V29</f>
-        <v>2.8839328660299997E-4</v>
+        <f t="shared" ref="E29:E32" si="16">W29</f>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -35055,6 +35144,9 @@
         <v>1</v>
       </c>
       <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="O29">
         <v>1</v>
       </c>
       <c r="P29">
@@ -35063,27 +35155,30 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
         <f>B29</f>
-        <v>2.8839328660299997E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>85</v>
       </c>
       <c r="B30">
-        <v>1.05527981312538</v>
+        <v>0.87723134883653597</v>
       </c>
       <c r="C30">
         <f t="shared" ref="C30:D31" si="17">LN(F30)</f>
@@ -35095,7 +35190,7 @@
       </c>
       <c r="E30" s="16">
         <f t="shared" si="16"/>
-        <v>2.8727788826868608</v>
+        <v>2.4042339979088103</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -35111,7 +35206,7 @@
       </c>
       <c r="J30">
         <f t="shared" ref="J30:J31" si="18">1/E30</f>
-        <v>0.34809501212453814</v>
+        <v>0.41593289208529394</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -35128,24 +35223,27 @@
         <v>1</v>
       </c>
       <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <f>EXP(B30)</f>
-        <v>2.8727788826868608</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+        <v>2.4042339979088103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>82</v>
       </c>
       <c r="B31">
-        <v>1.5136526163447299</v>
+        <v>1.63</v>
       </c>
       <c r="C31">
         <f t="shared" si="17"/>
@@ -35157,7 +35255,7 @@
       </c>
       <c r="E31" s="16">
         <f t="shared" si="16"/>
-        <v>4.5432954389310165</v>
+        <v>5.1038747185367255</v>
       </c>
       <c r="F31">
         <v>1.8</v>
@@ -35173,7 +35271,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="18"/>
-        <v>0.22010455041754629</v>
+        <v>0.19592957412690937</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -35193,24 +35291,27 @@
         <v>1</v>
       </c>
       <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <f>EXP(B31)</f>
-        <v>4.5432954389310165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+        <v>5.1038747185367255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>83</v>
       </c>
       <c r="B32">
-        <v>0.76180259530267702</v>
+        <v>0.72</v>
       </c>
       <c r="C32">
         <f t="shared" ref="C32:D32" si="19">-LN(1/F32 -1)</f>
@@ -35222,7 +35323,7 @@
       </c>
       <c r="E32" s="16">
         <f t="shared" si="16"/>
-        <v>0.68174496873562673</v>
+        <v>0.67260701706776038</v>
       </c>
       <c r="F32">
         <v>0.2</v>
@@ -35238,7 +35339,7 @@
       </c>
       <c r="J32">
         <f>1/(E32*(1-E32))</f>
-        <v>4.6089583163147303</v>
+        <v>4.5411854666038591</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -35252,19 +35353,22 @@
         <v>1</v>
       </c>
       <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V32">
+      <c r="W32">
         <f>1/(1+EXP(-B32))</f>
-        <v>0.68174496873562673</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.67260701706776038</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -35318,24 +35422,27 @@
         <v>0</v>
       </c>
       <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <f>1/(1+EXP(-B33))</f>
         <v>0.66942775013665978</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>86</v>
       </c>
       <c r="B34" s="3">
-        <v>0.55521345569204195</v>
+        <v>0.18</v>
       </c>
       <c r="C34">
         <f>F34</f>
@@ -35347,7 +35454,7 @@
       </c>
       <c r="E34" s="16">
         <f>B34</f>
-        <v>0.55521345569204195</v>
+        <v>0.18</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -35380,24 +35487,27 @@
         <v>1</v>
       </c>
       <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V34">
+      <c r="W34">
         <f>B34</f>
-        <v>0.55521345569204195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>87</v>
       </c>
       <c r="B35">
-        <v>-0.15</v>
+        <v>-0.24389960977445099</v>
       </c>
       <c r="C35">
         <f t="shared" ref="C35:D37" si="20">LN(F35)</f>
@@ -35408,8 +35518,8 @@
         <v>0.40546510810816438</v>
       </c>
       <c r="E35" s="16">
-        <f t="shared" ref="E35:E38" si="21">V35</f>
-        <v>0.86070797642505781</v>
+        <f t="shared" ref="E35:E38" si="21">W35</f>
+        <v>0.78356629271138467</v>
       </c>
       <c r="F35">
         <v>0.1</v>
@@ -35425,7 +35535,7 @@
       </c>
       <c r="J35">
         <f t="shared" ref="J35:J37" si="22">1/E35</f>
-        <v>1.1618342427282831</v>
+        <v>1.2762162044256484</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -35442,24 +35552,27 @@
         <v>1</v>
       </c>
       <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <f>EXP(B35)</f>
-        <v>0.86070797642505781</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+        <v>0.78356629271138467</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>88</v>
       </c>
       <c r="B36">
-        <v>2.4977057011084001</v>
+        <v>2.7181287719673501</v>
       </c>
       <c r="C36">
         <f t="shared" si="20"/>
@@ -35471,7 +35584,7 @@
       </c>
       <c r="E36" s="16">
         <f t="shared" si="21"/>
-        <v>12.154575716956705</v>
+        <v>15.151942960761369</v>
       </c>
       <c r="F36">
         <v>1E-3</v>
@@ -35487,7 +35600,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="22"/>
-        <v>8.2273542350385115E-2</v>
+        <v>6.5998136515539721E-2</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -35504,19 +35617,22 @@
         <v>1</v>
       </c>
       <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V36">
+      <c r="W36">
         <f>EXP(B36)</f>
-        <v>12.154575716956705</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+        <v>15.151942960761369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -35566,19 +35682,22 @@
         <v>1</v>
       </c>
       <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U37">
+      <c r="V37">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <f>EXP(B37)</f>
         <v>4.4816890703380645</v>
       </c>
     </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>68</v>
       </c>
@@ -35631,33 +35750,40 @@
         <v>0</v>
       </c>
       <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U38">
+      <c r="V38">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <f>1/(1+EXP(-B38))</f>
         <v>0.53593792072440882</v>
       </c>
     </row>
-    <row r="39" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B39" s="3">
-        <v>1</v>
+        <f>E39</f>
+        <v>0.81406601627977282</v>
       </c>
       <c r="C39" s="3">
-        <v>1</v>
+        <f>E39</f>
+        <v>0.81406601627977282</v>
       </c>
       <c r="D39" s="3">
-        <v>1</v>
-      </c>
-      <c r="E39" s="16">
-        <v>1</v>
+        <f>E39</f>
+        <v>0.81406601627977282</v>
+      </c>
+      <c r="E39" s="3">
+        <f>E27*2</f>
+        <v>0.81406601627977282</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -35697,16 +35823,19 @@
         <v>0</v>
       </c>
       <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="U39">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U39">
+      <c r="V39">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="V39" s="3"/>
-    </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+      <c r="W39" s="3"/>
+    </row>
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -35752,15 +35881,18 @@
         <v>0</v>
       </c>
       <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -35806,14 +35938,17 @@
         <v>0</v>
       </c>
       <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="U41">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U41" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+      <c r="V41" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -35859,15 +35994,18 @@
         <v>0</v>
       </c>
       <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U42">
-        <f>T42-N42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="V42">
+        <f>U42-N42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -35915,16 +36053,19 @@
         <v>0</v>
       </c>
       <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U43">
-        <f t="shared" ref="U43:U52" si="24">T43</f>
-        <v>0</v>
-      </c>
-      <c r="V43"/>
-    </row>
-    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+      <c r="V43">
+        <f t="shared" ref="V43:V52" si="24">U43</f>
+        <v>0</v>
+      </c>
+      <c r="W43"/>
+    </row>
+    <row r="44" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -35966,15 +36107,18 @@
         <v>0</v>
       </c>
       <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U44">
+      <c r="V44">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -36016,15 +36160,18 @@
         <v>0</v>
       </c>
       <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -36063,15 +36210,18 @@
         <v>0</v>
       </c>
       <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U46">
+      <c r="V46">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -36111,15 +36261,18 @@
         <v>0</v>
       </c>
       <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U47">
+      <c r="V47">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>245</v>
       </c>
@@ -36153,19 +36306,22 @@
         <v>0</v>
       </c>
       <c r="S48">
-        <f t="shared" ref="S48:U48" si="26">SUM(O48:R48)</f>
+        <f t="shared" ref="S48" si="26">SUM(O48:R48)</f>
         <v>0</v>
       </c>
       <c r="T48">
-        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="U48">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
+        <f>SUM(P48:S48)</f>
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <f>SUM(Q48:U48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>247</v>
       </c>
@@ -36204,15 +36360,18 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <f t="shared" ref="T49" si="30">S49+N49+Q49+M49</f>
         <v>0</v>
       </c>
       <c r="U49">
-        <f t="shared" ref="U49" si="31">T49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
+        <f t="shared" ref="U49" si="30">S49+N49+Q49+M49</f>
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <f t="shared" ref="V49" si="31">U49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -36255,15 +36414,18 @@
         <v>0</v>
       </c>
       <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U50">
+      <c r="V50">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -36306,15 +36468,18 @@
         <v>0</v>
       </c>
       <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U51">
+      <c r="V51">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>180</v>
       </c>
@@ -36357,15 +36522,18 @@
         <v>0</v>
       </c>
       <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U52">
+      <c r="V52">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -36377,7 +36545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>256</v>
       </c>
@@ -36389,13 +36557,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W55" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
+  <autoFilter ref="A1:X55" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
     <filterColumn colId="18">
       <filters blank="1">
         <filter val="1"/>
@@ -36846,7 +37014,7 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:D10" si="6">LN(E8)</f>
-        <v>-1.48055622303644</v>
+        <v>-1.5975688400857699</v>
       </c>
       <c r="C8">
         <f t="shared" si="6"/>
@@ -36858,7 +37026,7 @@
       </c>
       <c r="E8" s="16">
         <f>PARS!E8</f>
-        <v>0.22751110626478058</v>
+        <v>0.20238795785841901</v>
       </c>
       <c r="F8">
         <v>0.1</v>
@@ -36874,7 +37042,7 @@
       </c>
       <c r="J8">
         <f>1/E8</f>
-        <v>4.3953898181840234</v>
+        <v>4.9410054362006681</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -36900,7 +37068,7 @@
       </c>
       <c r="V8">
         <f>EXP(B8)</f>
-        <v>0.22751110626478058</v>
+        <v>0.20238795785841901</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -36909,7 +37077,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="6"/>
-        <v>0.100986933924772</v>
+        <v>0.16952904840680705</v>
       </c>
       <c r="C9">
         <f t="shared" si="6"/>
@@ -36921,7 +37089,7 @@
       </c>
       <c r="E9" s="16">
         <f>PARS!E9</f>
-        <v>1.1062621871640319</v>
+        <v>1.1847467615391678</v>
       </c>
       <c r="F9">
         <v>0.85</v>
@@ -36937,7 +37105,7 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9:J22" si="8">1/E9</f>
-        <v>0.90394484382003393</v>
+        <v>0.84406223546105885</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -36963,7 +37131,7 @@
       </c>
       <c r="V9">
         <f>EXP(B9)</f>
-        <v>1.1062621871640319</v>
+        <v>1.1847467615391678</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
@@ -36972,7 +37140,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="6"/>
-        <v>1.55520658335772</v>
+        <v>1.6447307311633199</v>
       </c>
       <c r="C10">
         <f t="shared" si="6"/>
@@ -36984,7 +37152,7 @@
       </c>
       <c r="E10" s="16">
         <f>PARS!E10</f>
-        <v>4.7360648162787387</v>
+        <v>5.1796150102475682</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -37000,7 +37168,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="8"/>
-        <v>0.21114575893531132</v>
+        <v>0.19306454205989401</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -37026,7 +37194,7 @@
       </c>
       <c r="V10">
         <f>EXP(B10)</f>
-        <v>4.7360648162787387</v>
+        <v>5.1796150102475682</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
@@ -37035,7 +37203,7 @@
       </c>
       <c r="B11">
         <f>LN(E11)</f>
-        <v>0.100986933924772</v>
+        <v>0.16952904840680705</v>
       </c>
       <c r="C11">
         <f>C4</f>
@@ -37047,7 +37215,7 @@
       </c>
       <c r="E11" s="16">
         <f>PARS!E11</f>
-        <v>1.1062621871640319</v>
+        <v>1.1847467615391678</v>
       </c>
       <c r="F11">
         <f>F4</f>
@@ -37065,7 +37233,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="8"/>
-        <v>0.90394484382003393</v>
+        <v>0.84406223546105885</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -37417,7 +37585,7 @@
       </c>
       <c r="B17">
         <f>LN(-E17)</f>
-        <v>-1.44797876639686</v>
+        <v>-1.41304067771723</v>
       </c>
       <c r="C17">
         <f>LN(-G17)</f>
@@ -37429,7 +37597,7 @@
       </c>
       <c r="E17" s="16">
         <f>PARS!E17</f>
-        <v>-0.23504488892038319</v>
+        <v>-0.24340204960980388</v>
       </c>
       <c r="F17">
         <v>-0.312</v>
@@ -37445,7 +37613,7 @@
       </c>
       <c r="J17">
         <f t="shared" si="8"/>
-        <v>-4.2545064672252044</v>
+        <v>-4.1084288386358825</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -37471,7 +37639,7 @@
       </c>
       <c r="V17">
         <f>-EXP(B17)</f>
-        <v>-0.23504488892038319</v>
+        <v>-0.24340204960980388</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.35">
@@ -37480,7 +37648,7 @@
       </c>
       <c r="B18">
         <f t="shared" ref="B18:D19" si="9">LN(E18)</f>
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
       <c r="C18">
         <f t="shared" si="9"/>
@@ -37492,7 +37660,7 @@
       </c>
       <c r="E18" s="16">
         <f>PARS!E18</f>
-        <v>0.44932896411722156</v>
+        <v>0.49658530379140953</v>
       </c>
       <c r="F18">
         <v>0.3</v>
@@ -37508,7 +37676,7 @@
       </c>
       <c r="J18">
         <f t="shared" si="8"/>
-        <v>2.2255409284924679</v>
+        <v>2.0137527074704766</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -37534,7 +37702,7 @@
       </c>
       <c r="V18">
         <f>EXP(B18)</f>
-        <v>0.44932896411722156</v>
+        <v>0.49658530379140953</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.35">
@@ -37543,7 +37711,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="9"/>
-        <v>1.0216023722149501</v>
+        <v>0.67</v>
       </c>
       <c r="C19">
         <f t="shared" si="9"/>
@@ -37555,7 +37723,7 @@
       </c>
       <c r="E19" s="16">
         <f>PARS!E19</f>
-        <v>2.7776420163259656</v>
+        <v>1.9542373206359396</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -37571,7 +37739,7 @@
       </c>
       <c r="J19">
         <f t="shared" si="8"/>
-        <v>0.36001759554412166</v>
+        <v>0.51170857778654244</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -37597,7 +37765,7 @@
       </c>
       <c r="V19">
         <f>EXP(B19)</f>
-        <v>2.7776420163259656</v>
+        <v>1.9542373206359396</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.35">
@@ -37742,7 +37910,7 @@
       </c>
       <c r="B22">
         <f>LN(E22/10)</f>
-        <v>0.88400425182202902</v>
+        <v>0.89700000000000013</v>
       </c>
       <c r="C22">
         <f>LN(F22/10)</f>
@@ -37754,7 +37922,7 @@
       </c>
       <c r="E22" s="16">
         <f>PARS!E22</f>
-        <v>24.205729100058726</v>
+        <v>24.522353589775612</v>
       </c>
       <c r="F22">
         <v>14.5</v>
@@ -37770,7 +37938,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="8"/>
-        <v>4.1312533733907399E-2</v>
+        <v>4.0779120011422622E-2</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -37796,7 +37964,7 @@
       </c>
       <c r="V22">
         <f>EXP(B22)*10</f>
-        <v>24.205729100058726</v>
+        <v>24.522353589775612</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.35">
@@ -37805,7 +37973,7 @@
       </c>
       <c r="B23">
         <f>1-LN(1/(E23-1) -1)</f>
-        <v>3.82182426773669</v>
+        <v>4.0000000000000018</v>
       </c>
       <c r="C23">
         <f>1-LN(1/(F23-1) -1)</f>
@@ -37817,7 +37985,7 @@
       </c>
       <c r="E23" s="16">
         <f>PARS!E23</f>
-        <v>1.9438438357765078</v>
+        <v>1.9525741268224333</v>
       </c>
       <c r="F23">
         <v>1.5</v>
@@ -37833,7 +38001,7 @@
       </c>
       <c r="J23">
         <f>1/((2-E23)*(E23-1))</f>
-        <v>18.866981377444393</v>
+        <v>22.135323991555545</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -37856,7 +38024,7 @@
       </c>
       <c r="V23">
         <f>1+1/(1+EXP(-(B23-1)))</f>
-        <v>1.9438438357765078</v>
+        <v>1.9525741268224333</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.35">
@@ -37918,7 +38086,7 @@
       </c>
       <c r="B25">
         <f t="shared" ref="B25:D26" si="10">E25</f>
-        <v>-0.138195355891432</v>
+        <v>-0.16</v>
       </c>
       <c r="C25">
         <f t="shared" si="10"/>
@@ -37930,7 +38098,7 @@
       </c>
       <c r="E25" s="16">
         <f>PARS!E25</f>
-        <v>-0.138195355891432</v>
+        <v>-0.16</v>
       </c>
       <c r="F25">
         <f>-0.15</f>
@@ -37975,7 +38143,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="10"/>
-        <v>0.18027520148399201</v>
+        <v>0.156757269540368</v>
       </c>
       <c r="C26">
         <f t="shared" si="10"/>
@@ -37987,7 +38155,7 @@
       </c>
       <c r="E26" s="16">
         <f>PARS!E26</f>
-        <v>0.18027520148399201</v>
+        <v>0.156757269540368</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -38031,7 +38199,7 @@
       </c>
       <c r="B27">
         <f>LN(E27)</f>
-        <v>-0.84824279493960997</v>
+        <v>-0.89886099574725498</v>
       </c>
       <c r="C27">
         <f>LN(F27)</f>
@@ -38043,7 +38211,7 @@
       </c>
       <c r="E27" s="16">
         <f>PARS!E27</f>
-        <v>0.42816664789613951</v>
+        <v>0.40703300813988641</v>
       </c>
       <c r="F27">
         <v>0.7</v>
@@ -38059,7 +38227,7 @@
       </c>
       <c r="J27">
         <f t="shared" ref="J27" si="11">1/E27</f>
-        <v>2.3355392226686704</v>
+        <v>2.4568032076070021</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -38085,7 +38253,7 @@
       </c>
       <c r="V27">
         <f>EXP(B27)</f>
-        <v>0.42816664789613951</v>
+        <v>0.40703300813988641</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.35">
@@ -38156,7 +38324,7 @@
       </c>
       <c r="E29" s="16">
         <f>PARS!E29</f>
-        <v>2.8839328660299997E-4</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -38200,7 +38368,7 @@
       </c>
       <c r="B30">
         <f t="shared" ref="B30:D31" si="12">LN(E30)</f>
-        <v>1.05527981312538</v>
+        <v>0.87723134883653586</v>
       </c>
       <c r="C30">
         <f t="shared" si="12"/>
@@ -38212,7 +38380,7 @@
       </c>
       <c r="E30" s="16">
         <f>PARS!E30</f>
-        <v>2.8727788826868608</v>
+        <v>2.4042339979088103</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -38228,7 +38396,7 @@
       </c>
       <c r="J30">
         <f t="shared" ref="J30:J31" si="13">1/E30</f>
-        <v>0.34809501212453814</v>
+        <v>0.41593289208529394</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -38254,7 +38422,7 @@
       </c>
       <c r="V30">
         <f>EXP(B30)</f>
-        <v>2.8727788826868608</v>
+        <v>2.4042339979088103</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.35">
@@ -38263,7 +38431,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="12"/>
-        <v>1.5136526163447299</v>
+        <v>1.63</v>
       </c>
       <c r="C31">
         <f t="shared" si="12"/>
@@ -38275,7 +38443,7 @@
       </c>
       <c r="E31" s="16">
         <f>PARS!E31</f>
-        <v>4.5432954389310165</v>
+        <v>5.1038747185367255</v>
       </c>
       <c r="F31">
         <v>1.8</v>
@@ -38291,7 +38459,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="13"/>
-        <v>0.22010455041754629</v>
+        <v>0.19592957412690937</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -38320,7 +38488,7 @@
       </c>
       <c r="V31">
         <f>EXP(B31)</f>
-        <v>4.5432954389310165</v>
+        <v>5.1038747185367255</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.35">
@@ -38329,7 +38497,7 @@
       </c>
       <c r="B32">
         <f t="shared" ref="B32:D32" si="14">-LN(1/E32 -1)</f>
-        <v>0.76180259530267713</v>
+        <v>0.71999999999999986</v>
       </c>
       <c r="C32">
         <f t="shared" si="14"/>
@@ -38341,7 +38509,7 @@
       </c>
       <c r="E32" s="16">
         <f>PARS!E32</f>
-        <v>0.68174496873562673</v>
+        <v>0.67260701706776038</v>
       </c>
       <c r="F32">
         <v>0.1</v>
@@ -38357,7 +38525,7 @@
       </c>
       <c r="J32">
         <f>1/(E32*(1-E32))</f>
-        <v>4.6089583163147303</v>
+        <v>4.5411854666038591</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -38380,7 +38548,7 @@
       </c>
       <c r="V32">
         <f>1/(1+EXP(-B32))</f>
-        <v>0.68174496873562673</v>
+        <v>0.67260701706776038</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.35">
@@ -38457,7 +38625,7 @@
       </c>
       <c r="B34">
         <f t="shared" ref="B34:D37" si="15">LN(E34)</f>
-        <v>-0.58840263432666384</v>
+        <v>-1.7147984280919266</v>
       </c>
       <c r="C34">
         <f t="shared" si="15"/>
@@ -38469,7 +38637,7 @@
       </c>
       <c r="E34" s="16">
         <f>PARS!E34</f>
-        <v>0.55521345569204195</v>
+        <v>0.18</v>
       </c>
       <c r="F34">
         <v>0.1</v>
@@ -38485,7 +38653,7 @@
       </c>
       <c r="J34">
         <f t="shared" ref="J34:J37" si="16">1/E34</f>
-        <v>1.8011090865108033</v>
+        <v>5.5555555555555554</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -38511,7 +38679,7 @@
       </c>
       <c r="V34">
         <f>EXP(B34)</f>
-        <v>0.55521345569204195</v>
+        <v>0.18000000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.35">
@@ -38520,7 +38688,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="15"/>
-        <v>-0.15</v>
+        <v>-0.24389960977445099</v>
       </c>
       <c r="C35">
         <f t="shared" si="15"/>
@@ -38532,7 +38700,7 @@
       </c>
       <c r="E35" s="16">
         <f>PARS!E35</f>
-        <v>0.86070797642505781</v>
+        <v>0.78356629271138467</v>
       </c>
       <c r="F35">
         <v>0.48999999999999994</v>
@@ -38548,7 +38716,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="16"/>
-        <v>1.1618342427282831</v>
+        <v>1.2762162044256484</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -38574,7 +38742,7 @@
       </c>
       <c r="V35">
         <f>EXP(B35)</f>
-        <v>0.86070797642505781</v>
+        <v>0.78356629271138467</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
@@ -38583,7 +38751,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="15"/>
-        <v>2.4977057011084001</v>
+        <v>2.7181287719673501</v>
       </c>
       <c r="C36">
         <f t="shared" si="15"/>
@@ -38595,7 +38763,7 @@
       </c>
       <c r="E36" s="16">
         <f>PARS!E36</f>
-        <v>12.154575716956705</v>
+        <v>15.151942960761369</v>
       </c>
       <c r="F36">
         <v>1E-3</v>
@@ -38611,7 +38779,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="16"/>
-        <v>8.2273542350385115E-2</v>
+        <v>6.5998136515539721E-2</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -38637,7 +38805,7 @@
       </c>
       <c r="V36">
         <f>EXP(B36)</f>
-        <v>12.154575716956705</v>
+        <v>15.151942960761369</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.35">
@@ -38782,7 +38950,7 @@
       </c>
       <c r="E39" s="16">
         <f>PARS!E39</f>
-        <v>1</v>
+        <v>0.81406601627977282</v>
       </c>
       <c r="F39">
         <v>1</v>

</xml_diff>

<commit_message>
sm run in econstat5
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1183" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60CEE8A8-E9D9-4AC0-A6DA-C5A012A4908D}"/>
+  <xr:revisionPtr revIDLastSave="1186" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ECADC25-6939-4DBE-A68D-2F5F5A780C42}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -1683,11 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1724,13 +1723,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>77</v>
       </c>
       <c r="B2">
         <f>PARS!B2*$I$7+G2*(1-$I$7)*C2+(1-G2)*(1-$I$7)*D2</f>
-        <v>24.382751079030985</v>
+        <v>24.382751079030982</v>
       </c>
       <c r="C2">
         <f>PARS!C2</f>
@@ -1753,10 +1752,10 @@
       </c>
       <c r="H2">
         <f ca="1">RAND()</f>
-        <v>0.72340305432067764</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>1.4465584993253455E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -1785,16 +1784,16 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H52" ca="1" si="1">RAND()</f>
-        <v>0.61562076364887031</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.36898924275401113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
       <c r="B4">
         <f>PARS!B4*$I$7+G4*(1-$I$7)*C4+(1-G4)*(1-$I$7)*D4</f>
-        <v>-3.742849730143067E-2</v>
+        <v>-6.2380828835717772E-2</v>
       </c>
       <c r="C4">
         <f>PARS!C4</f>
@@ -1817,16 +1816,16 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10219849890846378</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.40988214125250455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>75</v>
       </c>
       <c r="B5">
         <f>PARS!B5*$I$7+G5*(1-$I$7)*C5+(1-G5)*(1-$I$7)*D5</f>
-        <v>-7.1572501249767939E-2</v>
+        <v>-0.11928750208294654</v>
       </c>
       <c r="C5">
         <f>PARS!C5</f>
@@ -1849,10 +1848,10 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84472865685762921</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.98044926454993997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -1881,13 +1880,13 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18919978313244201</v>
+        <v>0.46985075751505023</v>
       </c>
       <c r="I6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -1916,10 +1915,10 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10067253360837192</v>
+        <v>0.60419085796912209</v>
       </c>
       <c r="I7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1928,7 +1927,7 @@
       </c>
       <c r="B8">
         <f>PARS!B8*$I$7+G8*(1-$I$7)*C8+(1-G8)*(1-$I$7)*D8</f>
-        <v>-1.5969429878018198</v>
+        <v>-1.5767551769130663</v>
       </c>
       <c r="C8">
         <f>PARS!C8</f>
@@ -1951,7 +1950,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.20165412642086E-2</v>
+        <v>0.33841818290499392</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1960,7 +1959,7 @@
       </c>
       <c r="B9">
         <f>PARS!B9*$I$7+G9*(1-$I$7)*C9+(1-G9)*(1-$I$7)*D9</f>
-        <v>0.16076973636148162</v>
+        <v>0.13898722770566341</v>
       </c>
       <c r="C9">
         <f>PARS!C9</f>
@@ -1983,7 +1982,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8103105888539035</v>
+        <v>0.11345277196946313</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1992,7 +1991,7 @@
       </c>
       <c r="B10">
         <f>PARS!B10*$I$7+G10*(1-$I$7)*C10+(1-G10)*(1-$I$7)*D10</f>
-        <v>0.8818743081123106</v>
+        <v>0.98406523919182154</v>
       </c>
       <c r="C10">
         <f>PARS!C10</f>
@@ -2015,16 +2014,16 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16530011166840952</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.18815012423777733</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>97</v>
       </c>
       <c r="B11">
         <f>PARS!B11*$I$7+G11*(1-$I$7)*C11+(1-G11)*(1-$I$7)*D11</f>
-        <v>2.6979474727723926E-2</v>
+        <v>-8.3996541683932724E-2</v>
       </c>
       <c r="C11">
         <f>PARS!C11</f>
@@ -2047,10 +2046,10 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46175832374075754</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>7.185349253231299E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -2079,16 +2078,16 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56135525309054302</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>7.7070510309597662E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>93</v>
       </c>
       <c r="B13">
         <f>PARS!B13*$I$7+G13*(1-$I$7)*C13+(1-G13)*(1-$I$7)*D13</f>
-        <v>-5.4859297264334195E-2</v>
+        <v>-9.1432162107223658E-2</v>
       </c>
       <c r="C13">
         <f>PARS!C13</f>
@@ -2111,10 +2110,10 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52383501972545188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.3104751123102486</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2143,10 +2142,10 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>6.3690445478653768E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.70880692382014276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -2175,10 +2174,10 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21447322352943654</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.28409388072177832</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>69</v>
       </c>
@@ -2207,7 +2206,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42011319085554477</v>
+        <v>0.4782054614917105</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -2216,7 +2215,7 @@
       </c>
       <c r="B17">
         <f>PARS!B17*$I$7+G17*(1-$I$7)*C17+(1-G17)*(1-$I$7)*D17</f>
-        <v>-1.4611938798869857</v>
+        <v>-1.4616472544117625</v>
       </c>
       <c r="C17">
         <f>PARS!C17</f>
@@ -2239,7 +2238,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29273486924413594</v>
+        <v>0.11790472575294608</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2248,7 +2247,7 @@
       </c>
       <c r="B18">
         <f>PARS!B18*$I$7+G18*(1-$I$7)*C18+(1-G18)*(1-$I$7)*D18</f>
-        <v>0.91553117875397017</v>
+        <v>0.92934936033973625</v>
       </c>
       <c r="C18">
         <f>PARS!C18</f>
@@ -2271,7 +2270,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10080549905183089</v>
+        <v>0.86858894091882521</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2280,7 +2279,7 @@
       </c>
       <c r="B19">
         <f>PARS!B19*$I$7+G19*(1-$I$7)*C19+(1-G19)*(1-$I$7)*D19</f>
-        <v>3.5794905892864923</v>
+        <v>3.3068660235007545</v>
       </c>
       <c r="C19">
         <f>PARS!C19</f>
@@ -2303,10 +2302,10 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93984164909325718</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.85194797560476077</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>71</v>
       </c>
@@ -2335,16 +2334,16 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60126540468559808</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.63461157428708792</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>72</v>
       </c>
       <c r="B21">
         <f>PARS!B21*$I$7+G21*(1-$I$7)*C21+(1-G21)*(1-$I$7)*D21</f>
-        <v>-0.12310470047936539</v>
+        <v>-8.4838677726534334E-2</v>
       </c>
       <c r="C21">
         <f>PARS!C21</f>
@@ -2367,7 +2366,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29944886989900599</v>
+        <v>0.41114439478882114</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2376,7 +2375,7 @@
       </c>
       <c r="B22">
         <f>PARS!B22*$I$7+G22*(1-$I$7)*C22+(1-G22)*(1-$I$7)*D22</f>
-        <v>0.10099294951642225</v>
+        <v>9.8550340904683759E-2</v>
       </c>
       <c r="C22">
         <f>PARS!C22</f>
@@ -2399,7 +2398,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95386777917618482</v>
+        <v>0.12891624155294401</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2408,7 +2407,7 @@
       </c>
       <c r="B23">
         <f>PARS!B23*$I$7+G23*(1-$I$7)*C23+(1-G23)*(1-$I$7)*D23</f>
-        <v>-1.2441460351897111</v>
+        <v>-1.3479065844196452</v>
       </c>
       <c r="C23">
         <f>PARS!C23</f>
@@ -2431,10 +2430,10 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91072236283022778</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.59885188186192395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2463,7 +2462,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14744494056398683</v>
+        <v>1.1776090991777011E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2495,7 +2494,7 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66562136683036943</v>
+        <v>0.35221149716064193</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2504,7 +2503,7 @@
       </c>
       <c r="B26">
         <f>PARS!B26*$I$7+G26*(1-$I$7)*C26+(1-G26)*(1-$I$7)*D26</f>
-        <v>-0.87126794567874088</v>
+        <v>-0.78846144493717296</v>
       </c>
       <c r="C26">
         <f>PARS!C26</f>
@@ -2527,7 +2526,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3816557110168879E-2</v>
+        <v>0.64048717780617204</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2536,7 +2535,7 @@
       </c>
       <c r="B27">
         <f>PARS!B27*$I$7+G27*(1-$I$7)*C27+(1-G27)*(1-$I$7)*D27</f>
-        <v>1.3434952269554619</v>
+        <v>1.5740608853093536</v>
       </c>
       <c r="C27">
         <f>PARS!C27</f>
@@ -2559,16 +2558,16 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13797751227757338</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.4378460935717331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>99</v>
       </c>
       <c r="B28">
         <f>PARS!B28*$I$7+G28*(1-$I$7)*C28+(1-G28)*(1-$I$7)*D28</f>
-        <v>2000.0000000000002</v>
+        <v>2000</v>
       </c>
       <c r="C28">
         <f>PARS!C28</f>
@@ -2591,10 +2590,10 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41477678772822801</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.29081544544309101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>102</v>
       </c>
@@ -2623,7 +2622,7 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56233238435390054</v>
+        <v>0.16795616686805315</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2632,7 +2631,7 @@
       </c>
       <c r="B30">
         <f>PARS!B30*$I$7+G30*(1-$I$7)*C30+(1-G30)*(1-$I$7)*D30</f>
-        <v>1.1285517526997335</v>
+        <v>1.2911847489331687</v>
       </c>
       <c r="C30">
         <f>PARS!C30</f>
@@ -2655,7 +2654,7 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83540135634835266</v>
+        <v>0.50894849808537512</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2664,7 +2663,7 @@
       </c>
       <c r="B31">
         <f>PARS!B31*$I$7+G31*(1-$I$7)*C31+(1-G31)*(1-$I$7)*D31</f>
-        <v>1.7167263750615624</v>
+        <v>1.7995442548880241</v>
       </c>
       <c r="C31">
         <f>PARS!C31</f>
@@ -2687,7 +2686,7 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10512574173056843</v>
+        <v>0.62720634379994922</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2696,7 +2695,7 @@
       </c>
       <c r="B32">
         <f>PARS!B32*$I$7+G32*(1-$I$7)*C32+(1-G32)*(1-$I$7)*D32</f>
-        <v>2.1224664621070466</v>
+        <v>3.2007705986155779</v>
       </c>
       <c r="C32">
         <f>PARS!C32</f>
@@ -2719,10 +2718,10 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43437567670250576</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.34008432656872445</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2751,7 +2750,7 @@
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8112887423474201</v>
+        <v>0.6250527313237858</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2760,7 +2759,7 @@
       </c>
       <c r="B34">
         <f>PARS!B34*$I$7+G34*(1-$I$7)*C34+(1-G34)*(1-$I$7)*D34</f>
-        <v>0.32091852249737773</v>
+        <v>0.37429349327863615</v>
       </c>
       <c r="C34">
         <f>PARS!C34</f>
@@ -2783,7 +2782,7 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22887313173731161</v>
+        <v>0.97128200951066246</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2792,7 +2791,7 @@
       </c>
       <c r="B35">
         <f>PARS!B35*$I$7+G35*(1-$I$7)*C35+(1-G35)*(1-$I$7)*D35</f>
-        <v>-0.8474289581502723</v>
+        <v>-0.74786274149679133</v>
       </c>
       <c r="C35">
         <f>PARS!C35</f>
@@ -2815,7 +2814,7 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1378609607658507E-2</v>
+        <v>0.40205250400642933</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2824,7 +2823,7 @@
       </c>
       <c r="B36">
         <f>PARS!B36*$I$7+G36*(1-$I$7)*C36+(1-G36)*(1-$I$7)*D36</f>
-        <v>1.5234904681714236</v>
+        <v>1.3976316737951866</v>
       </c>
       <c r="C36">
         <f>PARS!C36</f>
@@ -2847,7 +2846,7 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5513305710962171E-2</v>
+        <v>0.86343483207896243</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2856,7 +2855,7 @@
       </c>
       <c r="B37">
         <f>PARS!B37*$I$7+G37*(1-$I$7)*C37+(1-G37)*(1-$I$7)*D37</f>
-        <v>1.956114322494845</v>
+        <v>1.9242019886407082</v>
       </c>
       <c r="C37">
         <f>PARS!C37</f>
@@ -2879,7 +2878,7 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69595122067084003</v>
+        <v>0.89869074652314529</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2888,7 +2887,7 @@
       </c>
       <c r="B38">
         <f>PARS!B38*$I$7+G38*(1-$I$7)*C38+(1-G38)*(1-$I$7)*D38</f>
-        <v>0.1933268348314251</v>
+        <v>0.18941121527672114</v>
       </c>
       <c r="C38">
         <f>PARS!C38</f>
@@ -2911,10 +2910,10 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44971685636149439</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.74770124458511111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>106</v>
       </c>
@@ -2943,10 +2942,10 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70682270020208526</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.35061619202706928</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -2975,10 +2974,10 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36049995721543093</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.94271546973104792</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>108</v>
       </c>
@@ -3007,10 +3006,10 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55945876177274856</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.12820390107456248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -3039,10 +3038,10 @@
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83501770733790504</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.54494979351950901</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -3071,16 +3070,16 @@
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41098267025952617</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.30913153992699027</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>89</v>
       </c>
       <c r="B44">
         <f>PARS!B44*$I$7+G44*(1-$I$7)*C44+(1-G44)*(1-$I$7)*D44</f>
-        <v>0.14489999999999997</v>
+        <v>0.1449</v>
       </c>
       <c r="C44">
         <f>PARS!C44</f>
@@ -3103,10 +3102,10 @@
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81353700895499748</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.80631095250434304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3135,10 +3134,10 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44204190807702559</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.77049116712694377</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -3167,10 +3166,10 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13260968569480591</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.70855263238148269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -3199,10 +3198,10 @@
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52635253173136876</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.54026656862745792</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>245</v>
       </c>
@@ -3231,10 +3230,10 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7958491749356873E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.95568492715426523</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>247</v>
       </c>
@@ -3263,10 +3262,10 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2317799705133514E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.84908001543754175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -3295,10 +3294,10 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32857157474698329</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.56879391939588664</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -3327,16 +3326,16 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69322179066861889</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.20081266544736243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>180</v>
       </c>
       <c r="B52">
         <f>PARS!B52*$I$7+G52*(1-$I$7)*C52+(1-G52)*(1-$I$7)*D52</f>
-        <v>0.92210899999999985</v>
+        <v>0.92210900000000007</v>
       </c>
       <c r="C52">
         <f>PARS!C52</f>
@@ -3358,17 +3357,11 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9208774497830103E-2</v>
+        <v>0.12602767509494006</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I52" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I52" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -33490,7 +33483,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AB60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>

</xml_diff>

<commit_message>
clean output + rerun
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1186" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ECADC25-6939-4DBE-A68D-2F5F5A780C42}"/>
+  <xr:revisionPtr revIDLastSave="1198" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CD2627B-672F-46A6-B36B-4DC7C0CED9A7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="4420" yWindow="4420" windowWidth="2370" windowHeight="560" activeTab="1" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -1685,7 +1685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA45EEF9-8519-412C-B944-7FF4BEAF14F3}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="H2">
         <f ca="1">RAND()</f>
-        <v>1.4465584993253455E-2</v>
+        <v>0.24144846719904123</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H52" ca="1" si="1">RAND()</f>
-        <v>0.36898924275401113</v>
+        <v>0.90040258972296161</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40988214125250455</v>
+        <v>0.45556373980542997</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98044926454993997</v>
+        <v>0.42220705651136337</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46985075751505023</v>
+        <v>0.20067557666760105</v>
       </c>
       <c r="I6" t="s">
         <v>251</v>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60419085796912209</v>
+        <v>0.87460472888391094</v>
       </c>
       <c r="I7">
         <v>0.5</v>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33841818290499392</v>
+        <v>0.67849913789991034</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11345277196946313</v>
+        <v>0.92800938151369594</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B10">
         <f>PARS!B10*$I$7+G10*(1-$I$7)*C10+(1-G10)*(1-$I$7)*D10</f>
-        <v>0.98406523919182154</v>
+        <v>0.92728903462514878</v>
       </c>
       <c r="C10">
         <f>PARS!C10</f>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="D10">
         <f>PARS!D10</f>
-        <v>1.3862943611198906</v>
+        <v>1.2527629684953681</v>
       </c>
       <c r="E10" t="b">
         <f t="shared" si="0"/>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18815012423777733</v>
+        <v>0.50665291844795135</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2046,7 +2046,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>7.185349253231299E-2</v>
+        <v>6.3982759850420012E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7070510309597662E-2</v>
+        <v>0.33631095360479568</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2110,7 +2110,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3104751123102486</v>
+        <v>2.5778717242279758E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70880692382014276</v>
+        <v>0.22214856939635319</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28409388072177832</v>
+        <v>0.38446767596619735</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4782054614917105</v>
+        <v>0.2961733691734999</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11790472575294608</v>
+        <v>0.87040464020041985</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2270,7 +2270,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86858894091882521</v>
+        <v>0.67445320888535376</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85194797560476077</v>
+        <v>0.43400604220528927</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -2334,7 +2334,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63461157428708792</v>
+        <v>0.89467831433976652</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41114439478882114</v>
+        <v>0.11277400657570036</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12891624155294401</v>
+        <v>6.321845917356661E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2430,7 +2430,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59885188186192395</v>
+        <v>0.94996735500984997</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1776090991777011E-2</v>
+        <v>9.5509847518945756E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35221149716064193</v>
+        <v>0.91812562054382296</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64048717780617204</v>
+        <v>0.77237777606889801</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4378460935717331</v>
+        <v>0.52831358226228842</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29081544544309101</v>
+        <v>0.39170385949465636</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16795616686805315</v>
+        <v>4.2008772501494929E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50894849808537512</v>
+        <v>0.92047044683431156</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>0.62720634379994922</v>
+        <v>0.98686093361104155</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2695,11 +2695,11 @@
       </c>
       <c r="B32">
         <f>PARS!B32*$I$7+G32*(1-$I$7)*C32+(1-G32)*(1-$I$7)*D32</f>
-        <v>3.2007705986155779</v>
+        <v>3.2605108145752055</v>
       </c>
       <c r="C32">
         <f>PARS!C32</f>
-        <v>-1.3862943611198906</v>
+        <v>-0.40546510810816438</v>
       </c>
       <c r="D32">
         <f>PARS!D32</f>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34008432656872445</v>
+        <v>0.20403907906528662</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6250527313237858</v>
+        <v>0.27533122215839412</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97128200951066246</v>
+        <v>0.13647530059027102</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40205250400642933</v>
+        <v>0.46574865149226929</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86343483207896243</v>
+        <v>0.80480392403779089</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89869074652314529</v>
+        <v>0.42620008420225419</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2887,11 +2887,11 @@
       </c>
       <c r="B38">
         <f>PARS!B38*$I$7+G38*(1-$I$7)*C38+(1-G38)*(1-$I$7)*D38</f>
-        <v>0.18941121527672114</v>
+        <v>0.1937892548070046</v>
       </c>
       <c r="C38">
         <f>PARS!C38</f>
-        <v>-4.0005334613699206E-2</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>PARS!D38</f>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74770124458511111</v>
+        <v>0.95692981709130254</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35061619202706928</v>
+        <v>0.19005118101836249</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94271546973104792</v>
+        <v>0.40281354380382994</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12820390107456248</v>
+        <v>0.20917726085989852</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54494979351950901</v>
+        <v>0.82031951340547826</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -3070,7 +3070,7 @@
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30913153992699027</v>
+        <v>0.59146667079984283</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -3102,7 +3102,7 @@
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80631095250434304</v>
+        <v>0.18222701949247577</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77049116712694377</v>
+        <v>0.27781748822578811</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -3166,7 +3166,7 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70855263238148269</v>
+        <v>0.63645645359945358</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54026656862745792</v>
+        <v>0.56945159950116142</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -3230,7 +3230,7 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="1"/>
-        <v>0.95568492715426523</v>
+        <v>0.13050956905184274</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -3262,7 +3262,7 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84908001543754175</v>
+        <v>0.33442115456985422</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56879391939588664</v>
+        <v>0.91318241689266944</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20081266544736243</v>
+        <v>0.76819863376430619</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12602767509494006</v>
+        <v>0.58498309664133774</v>
       </c>
     </row>
   </sheetData>
@@ -33481,13 +33481,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB60"/>
+  <dimension ref="A1:AB187"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="C161" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomRight" activeCell="F62" sqref="F62:G187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34109,7 +34109,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="6"/>
-        <v>1.3862943611198906</v>
+        <v>1.2527629684953681</v>
       </c>
       <c r="E10" s="15">
         <f>X10</f>
@@ -34119,7 +34119,7 @@
         <v>1.5</v>
       </c>
       <c r="G10" s="10">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="H10">
         <v>5.12</v>
@@ -35588,7 +35588,7 @@
       </c>
       <c r="C32">
         <f>-LN(1/F32 -1)</f>
-        <v>-1.3862943611198906</v>
+        <v>-0.40546510810816438</v>
       </c>
       <c r="D32">
         <f>-LN(1/G32 -1)</f>
@@ -35599,7 +35599,7 @@
         <v>0.62363603584491722</v>
       </c>
       <c r="F32">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G32" s="10">
         <v>0.999</v>
@@ -36002,7 +36002,7 @@
       </c>
       <c r="C38">
         <f>-LN(1/F38 -1)</f>
-        <v>-4.0005334613699206E-2</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <f>-LN(1/G38 -1)</f>
@@ -36013,7 +36013,7 @@
         <v>0.54963604156036339</v>
       </c>
       <c r="F38">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G38" s="10">
         <v>0.56000000000000005</v>
@@ -37188,6 +37188,381 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="G62"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="G63"/>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G67"/>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G68"/>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G69"/>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G70"/>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G71"/>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G74"/>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G75"/>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G76"/>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G78"/>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G79"/>
+    </row>
+    <row r="80" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G80"/>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G81"/>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G93"/>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G94"/>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G95"/>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G96"/>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G97"/>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G99"/>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G100"/>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G101"/>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G102"/>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G105"/>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G106"/>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G107"/>
+    </row>
+    <row r="108" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G108"/>
+    </row>
+    <row r="109" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G109"/>
+    </row>
+    <row r="110" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G110"/>
+    </row>
+    <row r="111" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G111"/>
+    </row>
+    <row r="112" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G112"/>
+    </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G113"/>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G114"/>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G115"/>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G116"/>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G117"/>
+    </row>
+    <row r="118" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G118"/>
+    </row>
+    <row r="119" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G119"/>
+    </row>
+    <row r="120" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G120"/>
+    </row>
+    <row r="121" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G121"/>
+    </row>
+    <row r="122" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G122"/>
+    </row>
+    <row r="123" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G124"/>
+    </row>
+    <row r="125" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G125"/>
+    </row>
+    <row r="126" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G126"/>
+    </row>
+    <row r="127" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G127"/>
+    </row>
+    <row r="128" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G128"/>
+    </row>
+    <row r="129" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G129"/>
+    </row>
+    <row r="130" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G130"/>
+    </row>
+    <row r="131" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G131"/>
+    </row>
+    <row r="132" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G132"/>
+    </row>
+    <row r="133" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G133"/>
+    </row>
+    <row r="134" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G134"/>
+    </row>
+    <row r="135" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G135"/>
+    </row>
+    <row r="136" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G136"/>
+    </row>
+    <row r="137" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G137"/>
+    </row>
+    <row r="138" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G138"/>
+    </row>
+    <row r="139" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G139"/>
+    </row>
+    <row r="140" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G140"/>
+    </row>
+    <row r="141" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G141"/>
+    </row>
+    <row r="142" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G142"/>
+    </row>
+    <row r="143" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G143"/>
+    </row>
+    <row r="144" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G144"/>
+    </row>
+    <row r="145" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G145"/>
+    </row>
+    <row r="146" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G146"/>
+    </row>
+    <row r="147" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G147"/>
+    </row>
+    <row r="148" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G148"/>
+    </row>
+    <row r="149" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G149"/>
+    </row>
+    <row r="150" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G150"/>
+    </row>
+    <row r="151" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G151"/>
+    </row>
+    <row r="152" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G152"/>
+    </row>
+    <row r="153" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G153"/>
+    </row>
+    <row r="154" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G154"/>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G155"/>
+    </row>
+    <row r="156" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G156"/>
+    </row>
+    <row r="157" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G157"/>
+    </row>
+    <row r="158" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G158"/>
+    </row>
+    <row r="159" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G159"/>
+    </row>
+    <row r="160" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G160"/>
+    </row>
+    <row r="161" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G161"/>
+    </row>
+    <row r="162" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G162"/>
+    </row>
+    <row r="163" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G163"/>
+    </row>
+    <row r="164" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G164"/>
+    </row>
+    <row r="165" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G165"/>
+    </row>
+    <row r="166" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G166"/>
+    </row>
+    <row r="167" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G167"/>
+    </row>
+    <row r="168" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G168"/>
+    </row>
+    <row r="169" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G169"/>
+    </row>
+    <row r="170" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G170"/>
+    </row>
+    <row r="171" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G171"/>
+    </row>
+    <row r="172" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G172"/>
+    </row>
+    <row r="173" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G173"/>
+    </row>
+    <row r="174" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G174"/>
+    </row>
+    <row r="175" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G175"/>
+    </row>
+    <row r="176" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G176"/>
+    </row>
+    <row r="177" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G177"/>
+    </row>
+    <row r="178" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G178"/>
+    </row>
+    <row r="179" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G179"/>
+    </row>
+    <row r="180" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G180"/>
+    </row>
+    <row r="181" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G181"/>
+    </row>
+    <row r="182" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G182"/>
+    </row>
+    <row r="183" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G183"/>
+    </row>
+    <row r="184" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G184"/>
+    </row>
+    <row r="185" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G185"/>
+    </row>
+    <row r="186" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G186"/>
+    </row>
+    <row r="187" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G187"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Y60" xr:uid="{D6333A1E-4CCC-47DA-98C3-E7945B8628B8}">

</xml_diff>

<commit_message>
correction in labors errors
</commit_message>
<xml_diff>
--- a/input/PREP.xlsx
+++ b/input/PREP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/tranosov_umich_edu/Documents/Documents/D/Michigan/Res/Female careers in location/Codes/matlab/JMP/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1211" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53BE29E-914C-4D2C-B77F-F0EC3EFD4D02}"/>
+  <xr:revisionPtr revIDLastSave="1259" documentId="8_{1257A13C-7CDD-45B3-91A9-B5EE2763487A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEA54DEF-0992-4615-BD4D-3D63DBD002D2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{3C89D72B-78E5-4CC5-9BC1-023C2A9E36C5}"/>
   </bookViews>
   <sheets>
     <sheet name="PARSTEST" sheetId="11" r:id="rId1"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="283">
   <si>
     <t>label</t>
   </si>
@@ -1073,9 +1073,6 @@
     <t>Commuting</t>
   </si>
   <si>
-    <t>Work</t>
-  </si>
-  <si>
     <t>Home and marriage</t>
   </si>
   <si>
@@ -1086,6 +1083,12 @@
   </si>
   <si>
     <t>Sensitivity to job access</t>
+  </si>
+  <si>
+    <t>NEVER APPEARS! Even with 10% threshold. Baffling. Move to 2</t>
+  </si>
+  <si>
+    <t>Work, Home and Marriage</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1711,7 @@
       </c>
       <c r="H2">
         <f ca="1">RAND()</f>
-        <v>0.64206985265161021</v>
+        <v>0.5834079514890691</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1740,7 +1743,7 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H52" ca="1" si="1">RAND()</f>
-        <v>0.50100231699424858</v>
+        <v>0.15432529907643588</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1772,7 +1775,7 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88931568582175735</v>
+        <v>0.25658000829323435</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1804,7 +1807,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43345480316543816</v>
+        <v>0.83609652207046814</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1836,7 +1839,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43655712566312788</v>
+        <v>0.9774241055755547</v>
       </c>
       <c r="I6" t="s">
         <v>251</v>
@@ -1871,7 +1874,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24940085761962461</v>
+        <v>8.8525151090871335E-3</v>
       </c>
       <c r="I7">
         <v>0.8</v>
@@ -1906,7 +1909,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.79747363694387396</v>
+        <v>0.64652814355908328</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1938,7 +1941,7 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6304388774015024</v>
+        <v>2.5111485110639875E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1970,7 +1973,7 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82152863226681438</v>
+        <v>0.48424962225607937</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2002,7 +2005,7 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54073101494850417</v>
+        <v>0.25640598491356359</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2034,7 +2037,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.4155583560215068E-2</v>
+        <v>0.3310821232789869</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2066,7 +2069,7 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93373328410718159</v>
+        <v>0.90125130304477019</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2098,7 +2101,7 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89837829715539252</v>
+        <v>0.25348863554593004</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -2130,7 +2133,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17637714525681503</v>
+        <v>0.98671858031681703</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -2162,7 +2165,7 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9188569004205781</v>
+        <v>0.87583336218510133</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2194,7 +2197,7 @@
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8605722864909261</v>
+        <v>0.68181287391271628</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2226,7 +2229,7 @@
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14118524550846134</v>
+        <v>1.0774424413778627E-3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2258,7 +2261,7 @@
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80903381107819616</v>
+        <v>0.81567557913241306</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -2290,7 +2293,7 @@
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3873116895248319E-2</v>
+        <v>0.18635538756254033</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -2322,7 +2325,7 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78658777694913007</v>
+        <v>0.9204871439041058</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2354,7 +2357,7 @@
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2624719157237505</v>
+        <v>0.8268386614703962</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2386,7 +2389,7 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68510748506808239</v>
+        <v>0.27750319223286257</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -2418,7 +2421,7 @@
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9808506480180408E-2</v>
+        <v>0.95722443550714453</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2450,7 +2453,7 @@
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35161665455464586</v>
+        <v>0.6067462963914465</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2482,7 +2485,7 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7570724318528993</v>
+        <v>0.76833784423421969</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -2514,7 +2517,7 @@
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91908160603079048</v>
+        <v>0.3726700611925442</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -2546,7 +2549,7 @@
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23540571156462553</v>
+        <v>0.69442626931358098</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2578,7 +2581,7 @@
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78892147480727859</v>
+        <v>0.41398467470825551</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2610,7 +2613,7 @@
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29589096917997959</v>
+        <v>0.54633288062951046</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2642,7 +2645,7 @@
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
-        <v>5.7452256424234571E-2</v>
+        <v>0.48042659572458601</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2674,7 +2677,7 @@
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="1"/>
-        <v>0.29246414162056744</v>
+        <v>0.36378755942353092</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2706,7 +2709,7 @@
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69857579038949547</v>
+        <v>0.67576158321879687</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2738,7 +2741,7 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50507247462889082</v>
+        <v>0.4408926476858811</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -2770,7 +2773,7 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.93652682888134109</v>
+        <v>0.63210409965429937</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2802,7 +2805,7 @@
       </c>
       <c r="H36">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22938555195384303</v>
+        <v>0.45376444653990911</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2834,7 +2837,7 @@
       </c>
       <c r="H37">
         <f t="shared" ca="1" si="1"/>
-        <v>0.51216505782118227</v>
+        <v>0.52041377846869541</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2866,7 +2869,7 @@
       </c>
       <c r="H38">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55448694170793011</v>
+        <v>0.49483109499968148</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2898,7 +2901,7 @@
       </c>
       <c r="H39">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36883291962069442</v>
+        <v>0.32529169551487247</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2930,7 +2933,7 @@
       </c>
       <c r="H40">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61629894579333322</v>
+        <v>0.82106919481797036</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2962,7 +2965,7 @@
       </c>
       <c r="H41">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39629620312344616</v>
+        <v>0.5618468272389544</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2994,7 +2997,7 @@
       </c>
       <c r="H42">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48301936987306704</v>
+        <v>0.19325575926401584</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -3026,7 +3029,7 @@
       </c>
       <c r="H43">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32207704640130985</v>
+        <v>0.60394113393418281</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -3058,7 +3061,7 @@
       </c>
       <c r="H44">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94427385661080521</v>
+        <v>0.69299422418159895</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -3090,7 +3093,7 @@
       </c>
       <c r="H45">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70044535961222076</v>
+        <v>0.28545679243470801</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -3122,7 +3125,7 @@
       </c>
       <c r="H46">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27878930303243732</v>
+        <v>0.40798469831164674</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -3154,7 +3157,7 @@
       </c>
       <c r="H47">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98127175483357354</v>
+        <v>0.47437930965342778</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -3186,7 +3189,7 @@
       </c>
       <c r="H48">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3501770339675661E-3</v>
+        <v>0.10402729611160211</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -3218,7 +3221,7 @@
       </c>
       <c r="H49">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81196645340249407</v>
+        <v>0.40719405975938017</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -3250,7 +3253,7 @@
       </c>
       <c r="H50">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8573698067976</v>
+        <v>0.71641438072973262</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -3282,7 +3285,7 @@
       </c>
       <c r="H51">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74005366518617377</v>
+        <v>0.1550438049692523</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -3313,7 +3316,7 @@
       </c>
       <c r="H52">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46071481717598872</v>
+        <v>0.95996734375533554</v>
       </c>
     </row>
   </sheetData>
@@ -41404,8 +41407,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41713,7 +41716,7 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -41745,7 +41748,7 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -41799,7 +41802,7 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -41831,7 +41834,7 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -41885,7 +41888,7 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -42003,7 +42006,7 @@
         <v>1</v>
       </c>
       <c r="J20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -42035,7 +42038,7 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -42067,7 +42070,7 @@
         <v>1</v>
       </c>
       <c r="J22">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -42120,7 +42123,7 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -42177,7 +42180,7 @@
         <v>1</v>
       </c>
       <c r="J26">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -42208,7 +42211,7 @@
         <v>1</v>
       </c>
       <c r="J27">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -42239,7 +42242,7 @@
         <v>1</v>
       </c>
       <c r="J28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L28" t="s">
         <v>258</v>
@@ -42273,7 +42276,7 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -42353,7 +42356,7 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -42382,7 +42385,7 @@
         <v>1</v>
       </c>
       <c r="J33">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -42411,7 +42414,7 @@
         <v>1</v>
       </c>
       <c r="J34">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -42440,7 +42443,7 @@
         <v>100</v>
       </c>
       <c r="J35">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -42469,7 +42472,7 @@
         <v>1</v>
       </c>
       <c r="J36">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -42498,7 +42501,7 @@
         <v>1</v>
       </c>
       <c r="J37">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -42527,7 +42530,7 @@
         <v>1</v>
       </c>
       <c r="J38">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -42556,7 +42559,7 @@
         <v>1</v>
       </c>
       <c r="J39">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -42585,7 +42588,7 @@
         <v>1</v>
       </c>
       <c r="J40">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -42614,7 +42617,7 @@
         <v>1</v>
       </c>
       <c r="J41">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -42643,7 +42646,7 @@
         <v>1</v>
       </c>
       <c r="J42">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -42672,7 +42675,7 @@
         <v>1</v>
       </c>
       <c r="J43">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -42787,13 +42790,13 @@
         <v>1</v>
       </c>
       <c r="J48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L48" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -42849,6 +42852,9 @@
       <c r="I50">
         <v>1</v>
       </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
       <c r="L50" t="s">
         <v>222</v>
       </c>
@@ -42881,7 +42887,7 @@
         <v>1</v>
       </c>
       <c r="J51">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -42913,7 +42919,7 @@
         <v>1</v>
       </c>
       <c r="J52">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -42942,7 +42948,7 @@
         <v>1</v>
       </c>
       <c r="J53">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -42971,7 +42977,7 @@
         <v>100</v>
       </c>
       <c r="J54">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -43003,7 +43009,7 @@
         <v>1</v>
       </c>
       <c r="J55">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -43032,7 +43038,7 @@
         <v>1</v>
       </c>
       <c r="J56">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -43123,15 +43129,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CADE1A-3CD0-4B5F-AF7C-8162600CAC0D}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -43139,52 +43145,52 @@
         <v>276</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>

</xml_diff>